<commit_message>
add a row for new project in daily-report
</commit_message>
<xml_diff>
--- a/job/templates/DailyReport-v3.xlsx
+++ b/job/templates/DailyReport-v3.xlsx
@@ -128,8 +128,8 @@
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="[$-10409]#,##0;\(#,##0\)"/>
     <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
-    <numFmt numFmtId="167" formatCode="0.0%"/>
-    <numFmt numFmtId="168" formatCode="[$-10409]#,##0.0;\(#,##0.0\)"/>
+    <numFmt numFmtId="166" formatCode="0.0%"/>
+    <numFmt numFmtId="167" formatCode="[$-10409]#,##0.0;\(#,##0.0\)"/>
   </numFmts>
   <fonts count="9">
     <font>
@@ -737,7 +737,7 @@
       <alignment horizontal="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="3" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -749,7 +749,7 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="6" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="4" fillId="6" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -773,7 +773,7 @@
       <alignment horizontal="right" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="168" fontId="4" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="4" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -793,11 +793,11 @@
       <alignment horizontal="right" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="168" fontId="4" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="6" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="4" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="6" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -821,7 +821,7 @@
       <alignment horizontal="right" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="168" fontId="3" fillId="3" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="3" fillId="3" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -829,22 +829,62 @@
       <alignment horizontal="right" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="168" fontId="3" fillId="3" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="168" fontId="3" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="167" fontId="3" fillId="3" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="3" fillId="6" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="3" fillId="6" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="167" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="4" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="3" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="5" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="5" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
       <protection locked="0"/>
@@ -879,46 +919,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="168" fontId="4" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="168" fontId="4" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="168" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="168" fontId="4" fillId="3" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="168" fontId="4" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="168" fontId="4" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="168" fontId="4" fillId="5" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="168" fontId="4" fillId="5" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="168" fontId="4" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="168" fontId="4" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -1226,11 +1226,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S22"/>
+  <dimension ref="A1:S23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="J1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R10" sqref="R10:R14"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.45" customHeight="1"/>
@@ -1247,26 +1247,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="28.5" customHeight="1">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="62"/>
-      <c r="J1" s="62"/>
-      <c r="K1" s="62"/>
-      <c r="L1" s="62"/>
-      <c r="M1" s="62"/>
-      <c r="N1" s="62"/>
-      <c r="O1" s="62"/>
-      <c r="P1" s="62"/>
-      <c r="Q1" s="62"/>
-      <c r="R1" s="62"/>
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="72"/>
+      <c r="G1" s="72"/>
+      <c r="H1" s="72"/>
+      <c r="I1" s="72"/>
+      <c r="J1" s="72"/>
+      <c r="K1" s="72"/>
+      <c r="L1" s="72"/>
+      <c r="M1" s="72"/>
+      <c r="N1" s="72"/>
+      <c r="O1" s="72"/>
+      <c r="P1" s="72"/>
+      <c r="Q1" s="72"/>
+      <c r="R1" s="72"/>
     </row>
     <row r="2" spans="1:19" ht="1.05" customHeight="1"/>
     <row r="3" spans="1:19" ht="15.75" customHeight="1">
@@ -1281,13 +1281,13 @@
       <c r="B4" s="4"/>
     </row>
     <row r="5" spans="1:19" ht="18" customHeight="1">
-      <c r="A5" s="62" t="s">
+      <c r="A5" s="72" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="62"/>
-      <c r="C5" s="62"/>
-      <c r="D5" s="62"/>
-      <c r="E5" s="62"/>
+      <c r="B5" s="72"/>
+      <c r="C5" s="72"/>
+      <c r="D5" s="72"/>
+      <c r="E5" s="72"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
@@ -1301,29 +1301,29 @@
       <c r="C7" s="18"/>
       <c r="D7" s="14"/>
       <c r="E7" s="15"/>
-      <c r="F7" s="63" t="s">
+      <c r="F7" s="73" t="s">
         <v>29</v>
       </c>
-      <c r="G7" s="64"/>
-      <c r="H7" s="63" t="s">
+      <c r="G7" s="74"/>
+      <c r="H7" s="73" t="s">
         <v>4</v>
       </c>
-      <c r="I7" s="64"/>
-      <c r="J7" s="63" t="s">
+      <c r="I7" s="74"/>
+      <c r="J7" s="73" t="s">
         <v>30</v>
       </c>
-      <c r="K7" s="65"/>
-      <c r="L7" s="64"/>
-      <c r="M7" s="66" t="s">
+      <c r="K7" s="75"/>
+      <c r="L7" s="74"/>
+      <c r="M7" s="76" t="s">
         <v>28</v>
       </c>
-      <c r="N7" s="67"/>
-      <c r="O7" s="68"/>
-      <c r="P7" s="66" t="s">
+      <c r="N7" s="77"/>
+      <c r="O7" s="78"/>
+      <c r="P7" s="76" t="s">
         <v>33</v>
       </c>
-      <c r="Q7" s="67"/>
-      <c r="R7" s="67"/>
+      <c r="Q7" s="77"/>
+      <c r="R7" s="77"/>
     </row>
     <row r="8" spans="1:19" s="3" customFormat="1" ht="12.45" customHeight="1">
       <c r="A8" s="11" t="s">
@@ -1335,10 +1335,10 @@
       <c r="C8" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="60" t="s">
+      <c r="D8" s="70" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="61"/>
+      <c r="E8" s="71"/>
       <c r="F8" s="21" t="s">
         <v>9</v>
       </c>
@@ -1431,14 +1431,14 @@
       <c r="A10" s="12"/>
       <c r="B10" s="6"/>
       <c r="C10" s="20"/>
-      <c r="D10" s="69"/>
-      <c r="E10" s="71"/>
-      <c r="F10" s="69"/>
-      <c r="G10" s="71"/>
-      <c r="H10" s="73"/>
-      <c r="I10" s="74"/>
+      <c r="D10" s="60"/>
+      <c r="E10" s="62"/>
+      <c r="F10" s="60"/>
+      <c r="G10" s="62"/>
+      <c r="H10" s="64"/>
+      <c r="I10" s="65"/>
       <c r="J10" s="39" t="e">
-        <f>F10/$B$21</f>
+        <f>F10/$B$22</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K10" s="38" t="e">
@@ -1446,22 +1446,22 @@
         <v>#DIV/0!</v>
       </c>
       <c r="L10" s="39" t="e">
-        <f>G10/$B$21</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M10" s="77"/>
-      <c r="N10" s="69"/>
-      <c r="O10" s="69"/>
+        <f>G10/$B$22</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M10" s="68"/>
+      <c r="N10" s="60"/>
+      <c r="O10" s="60"/>
       <c r="P10" s="30" t="e">
-        <f t="shared" ref="P10:P15" si="0">I10/(J10*$B$22)</f>
+        <f t="shared" ref="P10:P16" si="0">I10/(J10*$B$23)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q10" s="33" t="e">
-        <f>I10/((J10*$B$22)*R10)</f>
+        <f>I10/((J10*$B$23)*R10)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R10" s="33" t="e">
-        <f>H10/(L10*$B$22)</f>
+        <f t="shared" ref="R10:R16" si="1">H10/(L10*$B$23)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1469,14 +1469,14 @@
       <c r="A11" s="12"/>
       <c r="B11" s="6"/>
       <c r="C11" s="20"/>
-      <c r="D11" s="69"/>
-      <c r="E11" s="71"/>
-      <c r="F11" s="69"/>
-      <c r="G11" s="71"/>
-      <c r="H11" s="73"/>
-      <c r="I11" s="74"/>
+      <c r="D11" s="60"/>
+      <c r="E11" s="62"/>
+      <c r="F11" s="60"/>
+      <c r="G11" s="62"/>
+      <c r="H11" s="64"/>
+      <c r="I11" s="65"/>
       <c r="J11" s="39" t="e">
-        <f>F11/$B$21</f>
+        <f>F11/$B$22</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K11" s="38" t="e">
@@ -1484,22 +1484,22 @@
         <v>#DIV/0!</v>
       </c>
       <c r="L11" s="39" t="e">
-        <f>G11/$B$21</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M11" s="77"/>
-      <c r="N11" s="69"/>
-      <c r="O11" s="69"/>
+        <f>G11/$B$22</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M11" s="68"/>
+      <c r="N11" s="60"/>
+      <c r="O11" s="60"/>
       <c r="P11" s="30" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Q11" s="33" t="e">
-        <f>I11/((F11/$B$21*$B$22)*R11)</f>
+        <f>I11/((F11/$B$22*$B$23)*R11)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R11" s="33" t="e">
-        <f t="shared" ref="R11:R15" si="1">H11/(L11*$B$22)</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1507,14 +1507,14 @@
       <c r="A12" s="12"/>
       <c r="B12" s="6"/>
       <c r="C12" s="20"/>
-      <c r="D12" s="69"/>
-      <c r="E12" s="71"/>
-      <c r="F12" s="69"/>
-      <c r="G12" s="71"/>
-      <c r="H12" s="73"/>
-      <c r="I12" s="74"/>
+      <c r="D12" s="60"/>
+      <c r="E12" s="62"/>
+      <c r="F12" s="60"/>
+      <c r="G12" s="62"/>
+      <c r="H12" s="64"/>
+      <c r="I12" s="65"/>
       <c r="J12" s="39" t="e">
-        <f>F12/$B$21</f>
+        <f>F12/$B$22</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K12" s="38" t="e">
@@ -1522,18 +1522,18 @@
         <v>#DIV/0!</v>
       </c>
       <c r="L12" s="39" t="e">
-        <f>G12/$B$21</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M12" s="77"/>
-      <c r="N12" s="69"/>
-      <c r="O12" s="69"/>
+        <f>G12/$B$22</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M12" s="68"/>
+      <c r="N12" s="60"/>
+      <c r="O12" s="60"/>
       <c r="P12" s="30" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Q12" s="33" t="e">
-        <f>I12/((F12/$B$21*$B$22)*R12)</f>
+        <f>I12/((F12/$B$22*$B$23)*R12)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R12" s="33" t="e">
@@ -1545,14 +1545,14 @@
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="20"/>
-      <c r="D13" s="69"/>
-      <c r="E13" s="71"/>
-      <c r="F13" s="69"/>
-      <c r="G13" s="71"/>
-      <c r="H13" s="73"/>
-      <c r="I13" s="74"/>
+      <c r="D13" s="60"/>
+      <c r="E13" s="62"/>
+      <c r="F13" s="60"/>
+      <c r="G13" s="62"/>
+      <c r="H13" s="64"/>
+      <c r="I13" s="65"/>
       <c r="J13" s="39" t="e">
-        <f>F13/$B$21</f>
+        <f>F13/$B$22</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K13" s="38" t="e">
@@ -1560,18 +1560,18 @@
         <v>#DIV/0!</v>
       </c>
       <c r="L13" s="39" t="e">
-        <f>G13/$B$21</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M13" s="77"/>
-      <c r="N13" s="69"/>
-      <c r="O13" s="69"/>
+        <f>G13/$B$22</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M13" s="68"/>
+      <c r="N13" s="60"/>
+      <c r="O13" s="60"/>
       <c r="P13" s="30" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Q13" s="33" t="e">
-        <f>I13/((F13/$B$21*$B$22)*R13)</f>
+        <f>I13/((F13/$B$22*$B$23)*R13)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R13" s="33" t="e">
@@ -1579,18 +1579,18 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="12.45" customHeight="1" thickBot="1">
+    <row r="14" spans="1:19" ht="12.45" customHeight="1">
       <c r="A14" s="40"/>
       <c r="B14" s="41"/>
       <c r="C14" s="42"/>
-      <c r="D14" s="70"/>
-      <c r="E14" s="72"/>
-      <c r="F14" s="70"/>
-      <c r="G14" s="72"/>
-      <c r="H14" s="75"/>
-      <c r="I14" s="76"/>
+      <c r="D14" s="61"/>
+      <c r="E14" s="63"/>
+      <c r="F14" s="61"/>
+      <c r="G14" s="63"/>
+      <c r="H14" s="66"/>
+      <c r="I14" s="67"/>
       <c r="J14" s="44" t="e">
-        <f>F14/$B$21</f>
+        <f>F14/$B$22</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K14" s="43" t="e">
@@ -1598,106 +1598,144 @@
         <v>#DIV/0!</v>
       </c>
       <c r="L14" s="44" t="e">
-        <f>G14/$B$21</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M14" s="78"/>
-      <c r="N14" s="70"/>
-      <c r="O14" s="70"/>
+        <f>G14/$B$22</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M14" s="69"/>
+      <c r="N14" s="61"/>
+      <c r="O14" s="61"/>
       <c r="P14" s="30" t="e">
+        <f t="shared" ref="P14" si="2">I14/(J14*$B$23)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q14" s="45" t="e">
+        <f>I14/((F14/$B$22*$B$23)*R14)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R14" s="45" t="e">
+        <f t="shared" ref="R14" si="3">H14/(L14*$B$23)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" ht="12.45" customHeight="1" thickBot="1">
+      <c r="A15" s="40"/>
+      <c r="B15" s="41"/>
+      <c r="C15" s="42"/>
+      <c r="D15" s="61"/>
+      <c r="E15" s="63"/>
+      <c r="F15" s="61"/>
+      <c r="G15" s="63"/>
+      <c r="H15" s="66"/>
+      <c r="I15" s="67"/>
+      <c r="J15" s="44" t="e">
+        <f>F15/$B$22</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K15" s="43" t="e">
+        <f>J15*(M15/L15)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L15" s="44" t="e">
+        <f>G15/$B$22</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M15" s="69"/>
+      <c r="N15" s="61"/>
+      <c r="O15" s="61"/>
+      <c r="P15" s="30" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="Q14" s="45" t="e">
-        <f>I14/((F14/$B$21*$B$22)*R14)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R14" s="45" t="e">
+      <c r="Q15" s="45" t="e">
+        <f>I15/((F15/$B$22*$B$23)*R15)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R15" s="45" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="13.05" customHeight="1" thickBot="1">
-      <c r="A15" s="46"/>
-      <c r="B15" s="47" t="s">
+    <row r="16" spans="1:19" ht="13.05" customHeight="1" thickBot="1">
+      <c r="A16" s="46"/>
+      <c r="B16" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="48"/>
-      <c r="D15" s="49">
-        <f>SUM(D10:D14)</f>
+      <c r="C16" s="48"/>
+      <c r="D16" s="49">
+        <f t="shared" ref="D16:N16" si="4">SUM(D10:D15)</f>
         <v>0</v>
       </c>
-      <c r="E15" s="49">
-        <f t="shared" ref="E15:H15" si="2">SUM(E10:E14)</f>
+      <c r="E16" s="49">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="F15" s="49">
-        <f t="shared" si="2"/>
+      <c r="F16" s="49">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="G15" s="49">
-        <f t="shared" si="2"/>
+      <c r="G16" s="49">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="H15" s="49">
-        <f t="shared" si="2"/>
+      <c r="H16" s="49">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I15" s="50">
-        <f t="shared" ref="I15:M15" si="3">SUM(I10:I14)</f>
+      <c r="I16" s="50">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="J15" s="51" t="e">
-        <f>SUM(J10:J14)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K15" s="52" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L15" s="52" t="e">
-        <f>SUM(L10:L14)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M15" s="53">
-        <f t="shared" si="3"/>
+      <c r="J16" s="51" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K16" s="52" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L16" s="52" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M16" s="53">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="N15" s="54">
-        <f>SUM(N10:N14)</f>
+      <c r="N16" s="54">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="O15" s="54"/>
-      <c r="P15" s="57" t="e">
+      <c r="O16" s="54"/>
+      <c r="P16" s="57" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="Q15" s="57" t="e">
-        <f>I15/((F15/$B$21*$B$22)*R15)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R15" s="57" t="e">
+      <c r="Q16" s="57" t="e">
+        <f>I16/((F16/$B$22*$B$23)*R16)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R16" s="57" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="S15" s="58"/>
+      <c r="S16" s="58"/>
     </row>
-    <row r="17" spans="1:17" ht="12.45" customHeight="1">
-      <c r="Q17" s="59"/>
-    </row>
-    <row r="21" spans="1:17" ht="12.45" customHeight="1">
-      <c r="A21" s="56" t="s">
-        <v>25</v>
-      </c>
-      <c r="B21" s="56"/>
-      <c r="C21" s="55"/>
+    <row r="18" spans="1:17" ht="12.45" customHeight="1">
+      <c r="Q18" s="59"/>
     </row>
     <row r="22" spans="1:17" ht="12.45" customHeight="1">
       <c r="A22" s="56" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B22" s="56"/>
       <c r="C22" s="55"/>
+    </row>
+    <row r="23" spans="1:17" ht="12.45" customHeight="1">
+      <c r="A23" s="56" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="56"/>
+      <c r="C23" s="55"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
@@ -1718,8 +1756,8 @@
 &amp;I© 2017 SunEdison&amp;I &amp;C&amp;R&amp;"Arial"&amp;8 Page 1 of 2 </oddFooter>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="Q14 D15:H15 J10:L13 Q11:Q13 Q10 P10:P14 R10:R15 P15:Q15 J14:L14 J15:N15" unlockedFormula="1"/>
-    <ignoredError sqref="I15" formula="1" unlockedFormula="1"/>
+    <ignoredError sqref="D16:H16 J10:L13 P10:R13 P16:R16 J16:N16" unlockedFormula="1"/>
+    <ignoredError sqref="I16" formula="1" unlockedFormula="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add a row in daily-report excel template for new site
</commit_message>
<xml_diff>
--- a/job/templates/DailyReport-v3.xlsx
+++ b/job/templates/DailyReport-v3.xlsx
@@ -1226,11 +1226,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S23"/>
+  <dimension ref="A1:S24"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.45" customHeight="1"/>
@@ -1246,7 +1246,7 @@
     <col min="16" max="18" width="19.21875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="28.5" customHeight="1">
+    <row r="1" spans="1:18" ht="28.5" customHeight="1">
       <c r="A1" s="72" t="s">
         <v>0</v>
       </c>
@@ -1268,8 +1268,8 @@
       <c r="Q1" s="72"/>
       <c r="R1" s="72"/>
     </row>
-    <row r="2" spans="1:19" ht="1.05" customHeight="1"/>
-    <row r="3" spans="1:19" ht="15.75" customHeight="1">
+    <row r="2" spans="1:18" ht="1.05" customHeight="1"/>
+    <row r="3" spans="1:18" ht="15.75" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -1277,10 +1277,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="15.75" customHeight="1">
+    <row r="4" spans="1:18" ht="15.75" customHeight="1">
       <c r="B4" s="4"/>
     </row>
-    <row r="5" spans="1:19" ht="18" customHeight="1">
+    <row r="5" spans="1:18" ht="18" customHeight="1">
       <c r="A5" s="72" t="s">
         <v>3</v>
       </c>
@@ -1294,8 +1294,8 @@
       <c r="I5" s="1"/>
       <c r="J5" s="28"/>
     </row>
-    <row r="6" spans="1:19" ht="2.7" customHeight="1" thickBot="1"/>
-    <row r="7" spans="1:19" s="9" customFormat="1" ht="22.5" customHeight="1" thickBot="1">
+    <row r="6" spans="1:18" ht="2.7" customHeight="1" thickBot="1"/>
+    <row r="7" spans="1:18" s="9" customFormat="1" ht="22.5" customHeight="1" thickBot="1">
       <c r="A7" s="10"/>
       <c r="B7" s="13"/>
       <c r="C7" s="18"/>
@@ -1325,7 +1325,7 @@
       <c r="Q7" s="77"/>
       <c r="R7" s="77"/>
     </row>
-    <row r="8" spans="1:19" s="3" customFormat="1" ht="12.45" customHeight="1">
+    <row r="8" spans="1:18" s="3" customFormat="1" ht="12.45" customHeight="1">
       <c r="A8" s="11" t="s">
         <v>5</v>
       </c>
@@ -1379,7 +1379,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:19" s="17" customFormat="1" ht="12.45" customHeight="1">
+    <row r="9" spans="1:18" s="17" customFormat="1" ht="12.45" customHeight="1">
       <c r="A9" s="16"/>
       <c r="B9" s="5"/>
       <c r="C9" s="8"/>
@@ -1427,7 +1427,7 @@
       </c>
       <c r="R9" s="32"/>
     </row>
-    <row r="10" spans="1:19" ht="12.45" customHeight="1">
+    <row r="10" spans="1:18" ht="12.45" customHeight="1">
       <c r="A10" s="12"/>
       <c r="B10" s="6"/>
       <c r="C10" s="20"/>
@@ -1438,34 +1438,34 @@
       <c r="H10" s="64"/>
       <c r="I10" s="65"/>
       <c r="J10" s="39" t="e">
-        <f>F10/$B$22</f>
+        <f t="shared" ref="J10:J16" si="0">F10/$B$23</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K10" s="38" t="e">
-        <f>J10*(M10/L10)</f>
+        <f t="shared" ref="K10:K16" si="1">J10*(M10/L10)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="L10" s="39" t="e">
-        <f>G10/$B$22</f>
+        <f t="shared" ref="L10:L16" si="2">G10/$B$23</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M10" s="68"/>
       <c r="N10" s="60"/>
       <c r="O10" s="60"/>
       <c r="P10" s="30" t="e">
-        <f t="shared" ref="P10:P16" si="0">I10/(J10*$B$23)</f>
+        <f t="shared" ref="P10:P17" si="3">I10/(J10*$B$24)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q10" s="33" t="e">
-        <f>I10/((J10*$B$23)*R10)</f>
+        <f>I10/((J10*$B$24)*R10)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R10" s="33" t="e">
-        <f t="shared" ref="R10:R16" si="1">H10/(L10*$B$23)</f>
+        <f t="shared" ref="R10:R17" si="4">H10/(L10*$B$24)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="12.45" customHeight="1">
+    <row r="11" spans="1:18" ht="12.45" customHeight="1">
       <c r="A11" s="12"/>
       <c r="B11" s="6"/>
       <c r="C11" s="20"/>
@@ -1476,34 +1476,34 @@
       <c r="H11" s="64"/>
       <c r="I11" s="65"/>
       <c r="J11" s="39" t="e">
-        <f>F11/$B$22</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K11" s="38" t="e">
-        <f>J11*(M11/L11)</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L11" s="39" t="e">
-        <f>G11/$B$22</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M11" s="68"/>
       <c r="N11" s="60"/>
       <c r="O11" s="60"/>
       <c r="P11" s="30" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Q11" s="33" t="e">
-        <f>I11/((F11/$B$22*$B$23)*R11)</f>
+        <f t="shared" ref="Q11:Q17" si="5">I11/((F11/$B$23*$B$24)*R11)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R11" s="33" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="12.45" customHeight="1">
+    <row r="12" spans="1:18" ht="12.45" customHeight="1">
       <c r="A12" s="12"/>
       <c r="B12" s="6"/>
       <c r="C12" s="20"/>
@@ -1514,34 +1514,34 @@
       <c r="H12" s="64"/>
       <c r="I12" s="65"/>
       <c r="J12" s="39" t="e">
-        <f>F12/$B$22</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K12" s="38" t="e">
-        <f>J12*(M12/L12)</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L12" s="39" t="e">
-        <f>G12/$B$22</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M12" s="68"/>
       <c r="N12" s="60"/>
       <c r="O12" s="60"/>
       <c r="P12" s="30" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Q12" s="33" t="e">
-        <f>I12/((F12/$B$22*$B$23)*R12)</f>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R12" s="33" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="12.45" customHeight="1">
+    <row r="13" spans="1:18" ht="12.45" customHeight="1">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="20"/>
@@ -1552,34 +1552,34 @@
       <c r="H13" s="64"/>
       <c r="I13" s="65"/>
       <c r="J13" s="39" t="e">
-        <f>F13/$B$22</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K13" s="38" t="e">
-        <f>J13*(M13/L13)</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L13" s="39" t="e">
-        <f>G13/$B$22</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M13" s="68"/>
       <c r="N13" s="60"/>
       <c r="O13" s="60"/>
       <c r="P13" s="30" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Q13" s="33" t="e">
-        <f>I13/((F13/$B$22*$B$23)*R13)</f>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R13" s="33" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="12.45" customHeight="1">
+    <row r="14" spans="1:18" ht="12.45" customHeight="1">
       <c r="A14" s="40"/>
       <c r="B14" s="41"/>
       <c r="C14" s="42"/>
@@ -1590,34 +1590,34 @@
       <c r="H14" s="66"/>
       <c r="I14" s="67"/>
       <c r="J14" s="44" t="e">
-        <f>F14/$B$22</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K14" s="43" t="e">
-        <f>J14*(M14/L14)</f>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L14" s="44" t="e">
-        <f>G14/$B$22</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M14" s="69"/>
       <c r="N14" s="61"/>
       <c r="O14" s="61"/>
       <c r="P14" s="30" t="e">
-        <f t="shared" ref="P14" si="2">I14/(J14*$B$23)</f>
+        <f t="shared" ref="P14" si="6">I14/(J14*$B$24)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q14" s="45" t="e">
-        <f>I14/((F14/$B$22*$B$23)*R14)</f>
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R14" s="45" t="e">
-        <f t="shared" ref="R14" si="3">H14/(L14*$B$23)</f>
+        <f t="shared" ref="R14" si="7">H14/(L14*$B$24)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="12.45" customHeight="1" thickBot="1">
+    <row r="15" spans="1:18" ht="12.45" customHeight="1">
       <c r="A15" s="40"/>
       <c r="B15" s="41"/>
       <c r="C15" s="42"/>
@@ -1627,115 +1627,135 @@
       <c r="G15" s="63"/>
       <c r="H15" s="66"/>
       <c r="I15" s="67"/>
-      <c r="J15" s="44" t="e">
-        <f>F15/$B$22</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K15" s="43" t="e">
-        <f>J15*(M15/L15)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L15" s="44" t="e">
-        <f>G15/$B$22</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="J15" s="44"/>
+      <c r="K15" s="43"/>
+      <c r="L15" s="44"/>
       <c r="M15" s="69"/>
       <c r="N15" s="61"/>
       <c r="O15" s="61"/>
-      <c r="P15" s="30" t="e">
+      <c r="P15" s="30"/>
+      <c r="Q15" s="45"/>
+      <c r="R15" s="45"/>
+    </row>
+    <row r="16" spans="1:18" ht="12.45" customHeight="1" thickBot="1">
+      <c r="A16" s="40"/>
+      <c r="B16" s="41"/>
+      <c r="C16" s="42"/>
+      <c r="D16" s="61"/>
+      <c r="E16" s="63"/>
+      <c r="F16" s="61"/>
+      <c r="G16" s="63"/>
+      <c r="H16" s="66"/>
+      <c r="I16" s="67"/>
+      <c r="J16" s="44" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="Q15" s="45" t="e">
-        <f>I15/((F15/$B$22*$B$23)*R15)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R15" s="45" t="e">
+      <c r="K16" s="43" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
+      <c r="L16" s="44" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M16" s="69"/>
+      <c r="N16" s="61"/>
+      <c r="O16" s="61"/>
+      <c r="P16" s="30" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q16" s="45" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R16" s="45" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
     </row>
-    <row r="16" spans="1:19" ht="13.05" customHeight="1" thickBot="1">
-      <c r="A16" s="46"/>
-      <c r="B16" s="47" t="s">
+    <row r="17" spans="1:19" ht="13.05" customHeight="1" thickBot="1">
+      <c r="A17" s="46"/>
+      <c r="B17" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="48"/>
-      <c r="D16" s="49">
-        <f t="shared" ref="D16:N16" si="4">SUM(D10:D15)</f>
+      <c r="C17" s="48"/>
+      <c r="D17" s="49">
+        <f t="shared" ref="D17:N17" si="8">SUM(D10:D16)</f>
         <v>0</v>
       </c>
-      <c r="E16" s="49">
+      <c r="E17" s="49">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="F17" s="49">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="G17" s="49">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="H17" s="49">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="I17" s="50">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="J17" s="51" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K17" s="52" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L17" s="52" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M17" s="53">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="N17" s="54">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="O17" s="54"/>
+      <c r="P17" s="57" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q17" s="57" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R17" s="57" t="e">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="F16" s="49">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G16" s="49">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="H16" s="49">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="I16" s="50">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="J16" s="51" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K16" s="52" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L16" s="52" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M16" s="53">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="N16" s="54">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="O16" s="54"/>
-      <c r="P16" s="57" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q16" s="57" t="e">
-        <f>I16/((F16/$B$22*$B$23)*R16)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R16" s="57" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S16" s="58"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S17" s="58"/>
     </row>
-    <row r="18" spans="1:17" ht="12.45" customHeight="1">
-      <c r="Q18" s="59"/>
+    <row r="19" spans="1:19" ht="12.45" customHeight="1">
+      <c r="Q19" s="59"/>
     </row>
-    <row r="22" spans="1:17" ht="12.45" customHeight="1">
-      <c r="A22" s="56" t="s">
+    <row r="23" spans="1:19" ht="12.45" customHeight="1">
+      <c r="A23" s="56" t="s">
         <v>25</v>
-      </c>
-      <c r="B22" s="56"/>
-      <c r="C22" s="55"/>
-    </row>
-    <row r="23" spans="1:17" ht="12.45" customHeight="1">
-      <c r="A23" s="56" t="s">
-        <v>26</v>
       </c>
       <c r="B23" s="56"/>
       <c r="C23" s="55"/>
+    </row>
+    <row r="24" spans="1:19" ht="12.45" customHeight="1">
+      <c r="A24" s="56" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" s="56"/>
+      <c r="C24" s="55"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
@@ -1756,8 +1776,8 @@
 &amp;I© 2017 SunEdison&amp;I &amp;C&amp;R&amp;"Arial"&amp;8 Page 1 of 2 </oddFooter>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="D16:H16 J10:L13 P10:R13 P16:R16 J16:N16" unlockedFormula="1"/>
-    <ignoredError sqref="I16" formula="1" unlockedFormula="1"/>
+    <ignoredError sqref="D17:H17 J10:L13 P10:R13 P17:R17 J17:N17" unlockedFormula="1"/>
+    <ignoredError sqref="I17" formula="1" unlockedFormula="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
change daily-report template for new projects
</commit_message>
<xml_diff>
--- a/job/templates/DailyReport-v3.xlsx
+++ b/job/templates/DailyReport-v3.xlsx
@@ -1226,11 +1226,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S24"/>
+  <dimension ref="A1:S28"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.45" customHeight="1"/>
@@ -1438,30 +1438,30 @@
       <c r="H10" s="64"/>
       <c r="I10" s="65"/>
       <c r="J10" s="39" t="e">
-        <f>F10/$B$23</f>
+        <f t="shared" ref="J10:J20" si="0">F10/$B$27</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K10" s="38" t="e">
-        <f t="shared" ref="K10:K16" si="0">J10*(M10/L10)</f>
+        <f t="shared" ref="K10:K20" si="1">J10*(M10/L10)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="L10" s="39" t="e">
-        <f>G10/$B$23</f>
+        <f t="shared" ref="L10:L20" si="2">G10/$B$27</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M10" s="68"/>
       <c r="N10" s="60"/>
       <c r="O10" s="60"/>
       <c r="P10" s="30" t="e">
-        <f>I10/(J10*$B$24)</f>
+        <f>I10/(J10*$B$28)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q10" s="33" t="e">
-        <f>I10/((J10*$B$24)*R10)</f>
+        <f>I10/((J10*$B$28)*R10)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R10" s="33" t="e">
-        <f>H10/(L10*$B$24)</f>
+        <f>H10/(L10*$B$28)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1476,30 +1476,30 @@
       <c r="H11" s="64"/>
       <c r="I11" s="65"/>
       <c r="J11" s="39" t="e">
-        <f>F11/$B$23</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K11" s="38" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L11" s="39" t="e">
-        <f>G11/$B$23</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M11" s="68"/>
       <c r="N11" s="60"/>
       <c r="O11" s="60"/>
       <c r="P11" s="30" t="e">
-        <f>I11/(J11*$B$24)</f>
+        <f>I11/(J11*$B$28)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q11" s="33" t="e">
-        <f>I11/((F11/$B$23*$B$24)*R11)</f>
+        <f t="shared" ref="Q11:Q21" si="3">I11/((F11/$B$27*$B$28)*R11)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R11" s="33" t="e">
-        <f>H11/(L11*$B$24)</f>
+        <f>H11/(L11*$B$28)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1514,30 +1514,30 @@
       <c r="H12" s="64"/>
       <c r="I12" s="65"/>
       <c r="J12" s="39" t="e">
-        <f>F12/$B$23</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K12" s="38" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L12" s="39" t="e">
-        <f>G12/$B$23</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M12" s="68"/>
       <c r="N12" s="60"/>
       <c r="O12" s="60"/>
       <c r="P12" s="30" t="e">
-        <f>I12/(J12*$B$24)</f>
+        <f>I12/(J12*$B$28)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q12" s="33" t="e">
-        <f>I12/((F12/$B$23*$B$24)*R12)</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R12" s="33" t="e">
-        <f>H12/(L12*$B$24)</f>
+        <f>H12/(L12*$B$28)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1552,30 +1552,30 @@
       <c r="H13" s="64"/>
       <c r="I13" s="65"/>
       <c r="J13" s="39" t="e">
-        <f>F13/$B$23</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K13" s="38" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L13" s="39" t="e">
-        <f>G13/$B$23</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M13" s="68"/>
       <c r="N13" s="60"/>
       <c r="O13" s="60"/>
       <c r="P13" s="30" t="e">
-        <f>I13/(J13*$B$24)</f>
+        <f>I13/(J13*$B$28)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q13" s="33" t="e">
-        <f>I13/((F13/$B$23*$B$24)*R13)</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R13" s="33" t="e">
-        <f>H13/(L13*$B$24)</f>
+        <f>H13/(L13*$B$28)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1590,30 +1590,30 @@
       <c r="H14" s="66"/>
       <c r="I14" s="67"/>
       <c r="J14" s="44" t="e">
-        <f>F14/$B$23</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K14" s="43" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L14" s="44" t="e">
-        <f>G14/$B$23</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M14" s="69"/>
       <c r="N14" s="61"/>
       <c r="O14" s="61"/>
       <c r="P14" s="30" t="e">
-        <f t="shared" ref="P14" si="1">I14/(J14*$B$24)</f>
+        <f t="shared" ref="P14" si="4">I14/(J14*$B$28)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q14" s="45" t="e">
-        <f>I14/((F14/$B$23*$B$24)*R14)</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R14" s="45" t="e">
-        <f t="shared" ref="R14" si="2">H14/(L14*$B$24)</f>
+        <f t="shared" ref="R14" si="5">H14/(L14*$B$28)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1628,34 +1628,34 @@
       <c r="H15" s="66"/>
       <c r="I15" s="67"/>
       <c r="J15" s="44" t="e">
-        <f>F15/$B$23</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K15" s="43" t="e">
-        <f t="shared" ref="K15" si="3">J15*(M15/L15)</f>
+        <f t="shared" ref="K15:K16" si="6">J15*(M15/L15)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="L15" s="44" t="e">
-        <f>G15/$B$23</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M15" s="69"/>
       <c r="N15" s="61"/>
       <c r="O15" s="61"/>
       <c r="P15" s="30" t="e">
-        <f>I15/(J15*$B$24)</f>
+        <f>I15/(J15*$B$28)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q15" s="45" t="e">
-        <f>I15/((F15/$B$23*$B$24)*R15)</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R15" s="45" t="e">
-        <f>H15/(L15*$B$24)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" ht="12.45" customHeight="1" thickBot="1">
+        <f>H15/(L15*$B$28)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" ht="12.45" customHeight="1">
       <c r="A16" s="40"/>
       <c r="B16" s="41"/>
       <c r="C16" s="42"/>
@@ -1666,114 +1666,266 @@
       <c r="H16" s="66"/>
       <c r="I16" s="67"/>
       <c r="J16" s="44" t="e">
-        <f>F16/$B$23</f>
+        <f t="shared" ref="J16" si="7">F16/$B$27</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K16" s="43" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L16" s="44" t="e">
-        <f>G16/$B$23</f>
+        <f t="shared" ref="L16" si="8">G16/$B$27</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M16" s="69"/>
       <c r="N16" s="61"/>
       <c r="O16" s="61"/>
       <c r="P16" s="30" t="e">
-        <f>I16/(J16*$B$24)</f>
+        <f>I16/(J16*$B$28)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q16" s="45" t="e">
-        <f>I16/((F16/$B$23*$B$24)*R16)</f>
+        <f t="shared" ref="Q16" si="9">I16/((F16/$B$27*$B$28)*R16)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R16" s="45" t="e">
-        <f>H16/(L16*$B$24)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19" ht="13.05" customHeight="1" thickBot="1">
-      <c r="A17" s="46"/>
-      <c r="B17" s="47" t="s">
+        <f>H16/(L16*$B$28)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" ht="12.45" customHeight="1">
+      <c r="A17" s="40"/>
+      <c r="B17" s="41"/>
+      <c r="C17" s="42"/>
+      <c r="D17" s="61"/>
+      <c r="E17" s="63"/>
+      <c r="F17" s="61"/>
+      <c r="G17" s="63"/>
+      <c r="H17" s="66"/>
+      <c r="I17" s="67"/>
+      <c r="J17" s="44" t="e">
+        <f t="shared" ref="J17" si="10">F17/$B$27</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K17" s="43" t="e">
+        <f t="shared" ref="K17" si="11">J17*(M17/L17)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L17" s="44" t="e">
+        <f t="shared" ref="L17" si="12">G17/$B$27</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M17" s="69"/>
+      <c r="N17" s="61"/>
+      <c r="O17" s="61"/>
+      <c r="P17" s="30" t="e">
+        <f>I17/(J17*$B$28)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q17" s="45" t="e">
+        <f t="shared" ref="Q17" si="13">I17/((F17/$B$27*$B$28)*R17)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R17" s="45" t="e">
+        <f>H17/(L17*$B$28)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" ht="12.45" customHeight="1">
+      <c r="A18" s="40"/>
+      <c r="B18" s="41"/>
+      <c r="C18" s="42"/>
+      <c r="D18" s="61"/>
+      <c r="E18" s="63"/>
+      <c r="F18" s="61"/>
+      <c r="G18" s="63"/>
+      <c r="H18" s="66"/>
+      <c r="I18" s="67"/>
+      <c r="J18" s="44" t="e">
+        <f t="shared" ref="J18" si="14">F18/$B$27</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K18" s="43" t="e">
+        <f t="shared" ref="K18" si="15">J18*(M18/L18)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L18" s="44" t="e">
+        <f t="shared" ref="L18" si="16">G18/$B$27</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M18" s="69"/>
+      <c r="N18" s="61"/>
+      <c r="O18" s="61"/>
+      <c r="P18" s="30" t="e">
+        <f>I18/(J18*$B$28)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q18" s="45" t="e">
+        <f t="shared" ref="Q18" si="17">I18/((F18/$B$27*$B$28)*R18)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R18" s="45" t="e">
+        <f>H18/(L18*$B$28)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" ht="12.45" customHeight="1">
+      <c r="A19" s="40"/>
+      <c r="B19" s="41"/>
+      <c r="C19" s="42"/>
+      <c r="D19" s="61"/>
+      <c r="E19" s="63"/>
+      <c r="F19" s="61"/>
+      <c r="G19" s="63"/>
+      <c r="H19" s="66"/>
+      <c r="I19" s="67"/>
+      <c r="J19" s="44" t="e">
+        <f t="shared" ref="J19" si="18">F19/$B$27</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K19" s="43" t="e">
+        <f t="shared" ref="K19" si="19">J19*(M19/L19)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L19" s="44" t="e">
+        <f t="shared" ref="L19" si="20">G19/$B$27</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M19" s="69"/>
+      <c r="N19" s="61"/>
+      <c r="O19" s="61"/>
+      <c r="P19" s="30" t="e">
+        <f>I19/(J19*$B$28)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q19" s="45" t="e">
+        <f t="shared" ref="Q19" si="21">I19/((F19/$B$27*$B$28)*R19)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R19" s="45" t="e">
+        <f>H19/(L19*$B$28)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" ht="12.45" customHeight="1" thickBot="1">
+      <c r="A20" s="40"/>
+      <c r="B20" s="41"/>
+      <c r="C20" s="42"/>
+      <c r="D20" s="61"/>
+      <c r="E20" s="63"/>
+      <c r="F20" s="61"/>
+      <c r="G20" s="63"/>
+      <c r="H20" s="66"/>
+      <c r="I20" s="67"/>
+      <c r="J20" s="44" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K20" s="43" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L20" s="44" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M20" s="69"/>
+      <c r="N20" s="61"/>
+      <c r="O20" s="61"/>
+      <c r="P20" s="30" t="e">
+        <f>I20/(J20*$B$28)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q20" s="45" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R20" s="45" t="e">
+        <f>H20/(L20*$B$28)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" ht="13.05" customHeight="1" thickBot="1">
+      <c r="A21" s="46"/>
+      <c r="B21" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="C17" s="48"/>
-      <c r="D17" s="49">
-        <f>SUM(D10:D16)</f>
+      <c r="C21" s="48"/>
+      <c r="D21" s="49">
+        <f t="shared" ref="D21:N21" si="22">SUM(D10:D20)</f>
         <v>0</v>
       </c>
-      <c r="E17" s="49">
-        <f>SUM(E10:E16)</f>
+      <c r="E21" s="49">
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
-      <c r="F17" s="49">
-        <f>SUM(F10:F16)</f>
+      <c r="F21" s="49">
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
-      <c r="G17" s="49">
-        <f>SUM(G10:G16)</f>
+      <c r="G21" s="49">
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
-      <c r="H17" s="49">
-        <f>SUM(H10:H16)</f>
+      <c r="H21" s="49">
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
-      <c r="I17" s="50">
-        <f>SUM(I10:I16)</f>
+      <c r="I21" s="50">
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
-      <c r="J17" s="51" t="e">
-        <f>SUM(J10:J16)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K17" s="52" t="e">
-        <f>SUM(K10:K16)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L17" s="52" t="e">
-        <f>SUM(L10:L16)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M17" s="53">
-        <f>SUM(M10:M16)</f>
+      <c r="J21" s="51" t="e">
+        <f t="shared" si="22"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K21" s="52" t="e">
+        <f t="shared" si="22"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L21" s="52" t="e">
+        <f t="shared" si="22"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M21" s="53">
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
-      <c r="N17" s="54">
-        <f>SUM(N10:N16)</f>
+      <c r="N21" s="54">
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
-      <c r="O17" s="54"/>
-      <c r="P17" s="57" t="e">
-        <f>I17/(J17*$B$24)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q17" s="57" t="e">
-        <f>I17/((F17/$B$23*$B$24)*R17)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R17" s="57" t="e">
-        <f>H17/(L17*$B$24)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S17" s="58"/>
-    </row>
-    <row r="19" spans="1:19" ht="12.45" customHeight="1">
-      <c r="Q19" s="59"/>
+      <c r="O21" s="54"/>
+      <c r="P21" s="57" t="e">
+        <f>I21/(J21*$B$28)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q21" s="57" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R21" s="57" t="e">
+        <f>H21/(L21*$B$28)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S21" s="58"/>
     </row>
     <row r="23" spans="1:19" ht="12.45" customHeight="1">
-      <c r="A23" s="56" t="s">
+      <c r="Q23" s="59"/>
+    </row>
+    <row r="27" spans="1:19" ht="12.45" customHeight="1">
+      <c r="A27" s="56" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="56"/>
-      <c r="C23" s="55"/>
-    </row>
-    <row r="24" spans="1:19" ht="12.45" customHeight="1">
-      <c r="A24" s="56" t="s">
+      <c r="B27" s="56"/>
+      <c r="C27" s="55"/>
+    </row>
+    <row r="28" spans="1:19" ht="12.45" customHeight="1">
+      <c r="A28" s="56" t="s">
         <v>26</v>
       </c>
-      <c r="B24" s="56"/>
-      <c r="C24" s="55"/>
+      <c r="B28" s="56"/>
+      <c r="C28" s="55"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
@@ -1794,8 +1946,8 @@
 &amp;I© 2017 SunEdison&amp;I &amp;C&amp;R&amp;"Arial"&amp;8 Page 1 of 2 </oddFooter>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="D17:H17 J10:L13 P10:R13 P17:R17 J17:N17" unlockedFormula="1"/>
-    <ignoredError sqref="I17" formula="1" unlockedFormula="1"/>
+    <ignoredError sqref="D21:H21 J10:L13 P10:R13 P21:R21 J21:N21" unlockedFormula="1"/>
+    <ignoredError sqref="I21" formula="1" unlockedFormula="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update daily/monthly report excel templates
</commit_message>
<xml_diff>
--- a/job/templates/DailyReport-v3.xlsx
+++ b/job/templates/DailyReport-v3.xlsx
@@ -1438,15 +1438,15 @@
       <c r="H10" s="64"/>
       <c r="I10" s="65"/>
       <c r="J10" s="39" t="e">
-        <f t="shared" ref="J10:J20" si="0">F10/$B$27</f>
+        <f t="shared" ref="J10:J21" si="0">F10/$B$27</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K10" s="38" t="e">
-        <f t="shared" ref="K10:K20" si="1">J10*(M10/L10)</f>
+        <f t="shared" ref="K10:K21" si="1">J10*(M10/L10)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="L10" s="39" t="e">
-        <f t="shared" ref="L10:L20" si="2">G10/$B$27</f>
+        <f t="shared" ref="L10:L21" si="2">G10/$B$27</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M10" s="68"/>
@@ -1495,7 +1495,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="Q11" s="33" t="e">
-        <f t="shared" ref="Q11:Q21" si="3">I11/((F11/$B$27*$B$28)*R11)</f>
+        <f t="shared" ref="Q11:Q22" si="3">I11/((F11/$B$27*$B$28)*R11)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R11" s="33" t="e">
@@ -1643,7 +1643,7 @@
       <c r="N15" s="61"/>
       <c r="O15" s="61"/>
       <c r="P15" s="30" t="e">
-        <f>I15/(J15*$B$28)</f>
+        <f t="shared" ref="P15:P22" si="7">I15/(J15*$B$28)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q15" s="45" t="e">
@@ -1651,7 +1651,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="R15" s="45" t="e">
-        <f>H15/(L15*$B$28)</f>
+        <f t="shared" ref="R15:R22" si="8">H15/(L15*$B$28)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1666,7 +1666,7 @@
       <c r="H16" s="66"/>
       <c r="I16" s="67"/>
       <c r="J16" s="44" t="e">
-        <f t="shared" ref="J16" si="7">F16/$B$27</f>
+        <f t="shared" ref="J16" si="9">F16/$B$27</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K16" s="43" t="e">
@@ -1674,22 +1674,22 @@
         <v>#DIV/0!</v>
       </c>
       <c r="L16" s="44" t="e">
-        <f t="shared" ref="L16" si="8">G16/$B$27</f>
+        <f t="shared" ref="L16" si="10">G16/$B$27</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M16" s="69"/>
       <c r="N16" s="61"/>
       <c r="O16" s="61"/>
       <c r="P16" s="30" t="e">
-        <f>I16/(J16*$B$28)</f>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Q16" s="45" t="e">
-        <f t="shared" ref="Q16" si="9">I16/((F16/$B$27*$B$28)*R16)</f>
+        <f t="shared" ref="Q16" si="11">I16/((F16/$B$27*$B$28)*R16)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R16" s="45" t="e">
-        <f>H16/(L16*$B$28)</f>
+        <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1704,30 +1704,30 @@
       <c r="H17" s="66"/>
       <c r="I17" s="67"/>
       <c r="J17" s="44" t="e">
-        <f t="shared" ref="J17" si="10">F17/$B$27</f>
+        <f t="shared" ref="J17" si="12">F17/$B$27</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K17" s="43" t="e">
-        <f t="shared" ref="K17" si="11">J17*(M17/L17)</f>
+        <f t="shared" ref="K17" si="13">J17*(M17/L17)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="L17" s="44" t="e">
-        <f t="shared" ref="L17" si="12">G17/$B$27</f>
+        <f t="shared" ref="L17" si="14">G17/$B$27</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M17" s="69"/>
       <c r="N17" s="61"/>
       <c r="O17" s="61"/>
       <c r="P17" s="30" t="e">
-        <f>I17/(J17*$B$28)</f>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Q17" s="45" t="e">
-        <f t="shared" ref="Q17" si="13">I17/((F17/$B$27*$B$28)*R17)</f>
+        <f t="shared" ref="Q17" si="15">I17/((F17/$B$27*$B$28)*R17)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R17" s="45" t="e">
-        <f>H17/(L17*$B$28)</f>
+        <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1742,30 +1742,30 @@
       <c r="H18" s="66"/>
       <c r="I18" s="67"/>
       <c r="J18" s="44" t="e">
-        <f t="shared" ref="J18" si="14">F18/$B$27</f>
+        <f t="shared" ref="J18" si="16">F18/$B$27</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K18" s="43" t="e">
-        <f t="shared" ref="K18" si="15">J18*(M18/L18)</f>
+        <f t="shared" ref="K18" si="17">J18*(M18/L18)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="L18" s="44" t="e">
-        <f t="shared" ref="L18" si="16">G18/$B$27</f>
+        <f t="shared" ref="L18" si="18">G18/$B$27</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M18" s="69"/>
       <c r="N18" s="61"/>
       <c r="O18" s="61"/>
       <c r="P18" s="30" t="e">
-        <f>I18/(J18*$B$28)</f>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Q18" s="45" t="e">
-        <f t="shared" ref="Q18" si="17">I18/((F18/$B$27*$B$28)*R18)</f>
+        <f t="shared" ref="Q18" si="19">I18/((F18/$B$27*$B$28)*R18)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R18" s="45" t="e">
-        <f>H18/(L18*$B$28)</f>
+        <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1780,34 +1780,34 @@
       <c r="H19" s="66"/>
       <c r="I19" s="67"/>
       <c r="J19" s="44" t="e">
-        <f t="shared" ref="J19" si="18">F19/$B$27</f>
+        <f t="shared" ref="J19:J20" si="20">F19/$B$27</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K19" s="43" t="e">
-        <f t="shared" ref="K19" si="19">J19*(M19/L19)</f>
+        <f t="shared" ref="K19:K20" si="21">J19*(M19/L19)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="L19" s="44" t="e">
-        <f t="shared" ref="L19" si="20">G19/$B$27</f>
+        <f t="shared" ref="L19:L20" si="22">G19/$B$27</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M19" s="69"/>
       <c r="N19" s="61"/>
       <c r="O19" s="61"/>
       <c r="P19" s="30" t="e">
-        <f>I19/(J19*$B$28)</f>
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Q19" s="45" t="e">
-        <f t="shared" ref="Q19" si="21">I19/((F19/$B$27*$B$28)*R19)</f>
+        <f t="shared" ref="Q19:Q20" si="23">I19/((F19/$B$27*$B$28)*R19)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R19" s="45" t="e">
-        <f>H19/(L19*$B$28)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="20" spans="1:19" ht="12.45" customHeight="1" thickBot="1">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" ht="12.45" customHeight="1">
       <c r="A20" s="40"/>
       <c r="B20" s="41"/>
       <c r="C20" s="42"/>
@@ -1818,100 +1818,138 @@
       <c r="H20" s="66"/>
       <c r="I20" s="67"/>
       <c r="J20" s="44" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="20"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K20" s="43" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="21"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L20" s="44" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="22"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M20" s="69"/>
       <c r="N20" s="61"/>
       <c r="O20" s="61"/>
       <c r="P20" s="30" t="e">
-        <f>I20/(J20*$B$28)</f>
+        <f t="shared" ref="P20" si="24">I20/(J20*$B$28)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q20" s="45" t="e">
+        <f t="shared" si="23"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R20" s="45" t="e">
+        <f t="shared" ref="R20" si="25">H20/(L20*$B$28)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" ht="12.45" customHeight="1" thickBot="1">
+      <c r="A21" s="40"/>
+      <c r="B21" s="41"/>
+      <c r="C21" s="42"/>
+      <c r="D21" s="61"/>
+      <c r="E21" s="63"/>
+      <c r="F21" s="61"/>
+      <c r="G21" s="63"/>
+      <c r="H21" s="66"/>
+      <c r="I21" s="67"/>
+      <c r="J21" s="44" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K21" s="43" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L21" s="44" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M21" s="69"/>
+      <c r="N21" s="61"/>
+      <c r="O21" s="61"/>
+      <c r="P21" s="30" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q21" s="45" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="R20" s="45" t="e">
-        <f>H20/(L20*$B$28)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="21" spans="1:19" ht="13.05" customHeight="1" thickBot="1">
-      <c r="A21" s="46"/>
-      <c r="B21" s="47" t="s">
+      <c r="R21" s="45" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" ht="13.05" customHeight="1" thickBot="1">
+      <c r="A22" s="46"/>
+      <c r="B22" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="C21" s="48"/>
-      <c r="D21" s="49">
-        <f t="shared" ref="D21:N21" si="22">SUM(D10:D20)</f>
+      <c r="C22" s="48"/>
+      <c r="D22" s="49">
+        <f t="shared" ref="D22:N22" si="26">SUM(D10:D21)</f>
         <v>0</v>
       </c>
-      <c r="E21" s="49">
-        <f t="shared" si="22"/>
+      <c r="E22" s="49">
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
-      <c r="F21" s="49">
-        <f t="shared" si="22"/>
+      <c r="F22" s="49">
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
-      <c r="G21" s="49">
-        <f t="shared" si="22"/>
+      <c r="G22" s="49">
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
-      <c r="H21" s="49">
-        <f t="shared" si="22"/>
+      <c r="H22" s="49">
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
-      <c r="I21" s="50">
-        <f t="shared" si="22"/>
+      <c r="I22" s="50">
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
-      <c r="J21" s="51" t="e">
-        <f t="shared" si="22"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K21" s="52" t="e">
-        <f t="shared" si="22"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L21" s="52" t="e">
-        <f t="shared" si="22"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M21" s="53">
-        <f t="shared" si="22"/>
+      <c r="J22" s="51" t="e">
+        <f t="shared" si="26"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K22" s="52" t="e">
+        <f t="shared" si="26"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L22" s="52" t="e">
+        <f t="shared" si="26"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M22" s="53">
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
-      <c r="N21" s="54">
-        <f t="shared" si="22"/>
+      <c r="N22" s="54">
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
-      <c r="O21" s="54"/>
-      <c r="P21" s="57" t="e">
-        <f>I21/(J21*$B$28)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q21" s="57" t="e">
+      <c r="O22" s="54"/>
+      <c r="P22" s="57" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q22" s="57" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="R21" s="57" t="e">
-        <f>H21/(L21*$B$28)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S21" s="58"/>
-    </row>
-    <row r="23" spans="1:19" ht="12.45" customHeight="1">
-      <c r="Q23" s="59"/>
+      <c r="R22" s="57" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S22" s="58"/>
+    </row>
+    <row r="24" spans="1:19" ht="12.45" customHeight="1">
+      <c r="Q24" s="59"/>
     </row>
     <row r="27" spans="1:19" ht="12.45" customHeight="1">
       <c r="A27" s="56" t="s">
@@ -1946,8 +1984,8 @@
 &amp;I© 2017 SunEdison&amp;I &amp;C&amp;R&amp;"Arial"&amp;8 Page 1 of 2 </oddFooter>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="D21:H21 J10:L13 P10:R13 P21:R21 J21:N21" unlockedFormula="1"/>
-    <ignoredError sqref="I21" formula="1" unlockedFormula="1"/>
+    <ignoredError sqref="D22:H22 J10:L13 P10:R13 P22:R22 J22:N22" unlockedFormula="1"/>
+    <ignoredError sqref="I22" formula="1" unlockedFormula="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
daily-report execel template update
</commit_message>
<xml_diff>
--- a/job/templates/DailyReport-v3.xlsx
+++ b/job/templates/DailyReport-v3.xlsx
@@ -1226,11 +1226,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S28"/>
+  <dimension ref="A1:S31"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.45" customHeight="1"/>
@@ -1438,30 +1438,30 @@
       <c r="H10" s="64"/>
       <c r="I10" s="65"/>
       <c r="J10" s="39" t="e">
-        <f t="shared" ref="J10:J21" si="0">F10/$B$27</f>
+        <f t="shared" ref="J10:J24" si="0">F10/$B$30</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K10" s="38" t="e">
-        <f t="shared" ref="K10:K21" si="1">J10*(M10/L10)</f>
+        <f t="shared" ref="K10:K24" si="1">J10*(M10/L10)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="L10" s="39" t="e">
-        <f t="shared" ref="L10:L21" si="2">G10/$B$27</f>
+        <f t="shared" ref="L10:L24" si="2">G10/$B$30</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M10" s="68"/>
       <c r="N10" s="60"/>
       <c r="O10" s="60"/>
       <c r="P10" s="30" t="e">
-        <f>I10/(J10*$B$28)</f>
+        <f>I10/(J10*$B$31)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q10" s="33" t="e">
-        <f>I10/((J10*$B$28)*R10)</f>
+        <f>I10/((J10*$B$31)*R10)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R10" s="33" t="e">
-        <f>H10/(L10*$B$28)</f>
+        <f>H10/(L10*$B$31)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1491,15 +1491,15 @@
       <c r="N11" s="60"/>
       <c r="O11" s="60"/>
       <c r="P11" s="30" t="e">
-        <f>I11/(J11*$B$28)</f>
+        <f>I11/(J11*$B$31)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q11" s="33" t="e">
-        <f t="shared" ref="Q11:Q22" si="3">I11/((F11/$B$27*$B$28)*R11)</f>
+        <f t="shared" ref="Q11:Q25" si="3">I11/((F11/$B$30*$B$31)*R11)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R11" s="33" t="e">
-        <f>H11/(L11*$B$28)</f>
+        <f>H11/(L11*$B$31)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1529,7 +1529,7 @@
       <c r="N12" s="60"/>
       <c r="O12" s="60"/>
       <c r="P12" s="30" t="e">
-        <f>I12/(J12*$B$28)</f>
+        <f>I12/(J12*$B$31)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q12" s="33" t="e">
@@ -1537,7 +1537,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="R12" s="33" t="e">
-        <f>H12/(L12*$B$28)</f>
+        <f>H12/(L12*$B$31)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1567,7 +1567,7 @@
       <c r="N13" s="60"/>
       <c r="O13" s="60"/>
       <c r="P13" s="30" t="e">
-        <f>I13/(J13*$B$28)</f>
+        <f>I13/(J13*$B$31)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q13" s="33" t="e">
@@ -1575,7 +1575,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="R13" s="33" t="e">
-        <f>H13/(L13*$B$28)</f>
+        <f>H13/(L13*$B$31)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1605,7 +1605,7 @@
       <c r="N14" s="61"/>
       <c r="O14" s="61"/>
       <c r="P14" s="30" t="e">
-        <f t="shared" ref="P14" si="4">I14/(J14*$B$28)</f>
+        <f t="shared" ref="P14" si="4">I14/(J14*$B$31)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q14" s="45" t="e">
@@ -1613,7 +1613,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="R14" s="45" t="e">
-        <f t="shared" ref="R14" si="5">H14/(L14*$B$28)</f>
+        <f t="shared" ref="R14" si="5">H14/(L14*$B$31)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1643,7 +1643,7 @@
       <c r="N15" s="61"/>
       <c r="O15" s="61"/>
       <c r="P15" s="30" t="e">
-        <f t="shared" ref="P15:P22" si="7">I15/(J15*$B$28)</f>
+        <f t="shared" ref="P15:P25" si="7">I15/(J15*$B$31)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q15" s="45" t="e">
@@ -1651,7 +1651,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="R15" s="45" t="e">
-        <f t="shared" ref="R15:R22" si="8">H15/(L15*$B$28)</f>
+        <f t="shared" ref="R15:R25" si="8">H15/(L15*$B$31)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1666,7 +1666,7 @@
       <c r="H16" s="66"/>
       <c r="I16" s="67"/>
       <c r="J16" s="44" t="e">
-        <f t="shared" ref="J16" si="9">F16/$B$27</f>
+        <f t="shared" ref="J16" si="9">F16/$B$30</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K16" s="43" t="e">
@@ -1674,7 +1674,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="L16" s="44" t="e">
-        <f t="shared" ref="L16" si="10">G16/$B$27</f>
+        <f t="shared" ref="L16" si="10">G16/$B$30</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M16" s="69"/>
@@ -1685,7 +1685,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="Q16" s="45" t="e">
-        <f t="shared" ref="Q16" si="11">I16/((F16/$B$27*$B$28)*R16)</f>
+        <f t="shared" ref="Q16" si="11">I16/((F16/$B$30*$B$31)*R16)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R16" s="45" t="e">
@@ -1704,7 +1704,7 @@
       <c r="H17" s="66"/>
       <c r="I17" s="67"/>
       <c r="J17" s="44" t="e">
-        <f t="shared" ref="J17" si="12">F17/$B$27</f>
+        <f t="shared" ref="J17" si="12">F17/$B$30</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K17" s="43" t="e">
@@ -1712,7 +1712,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="L17" s="44" t="e">
-        <f t="shared" ref="L17" si="14">G17/$B$27</f>
+        <f t="shared" ref="L17" si="14">G17/$B$30</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M17" s="69"/>
@@ -1723,7 +1723,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="Q17" s="45" t="e">
-        <f t="shared" ref="Q17" si="15">I17/((F17/$B$27*$B$28)*R17)</f>
+        <f t="shared" ref="Q17" si="15">I17/((F17/$B$30*$B$31)*R17)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R17" s="45" t="e">
@@ -1742,7 +1742,7 @@
       <c r="H18" s="66"/>
       <c r="I18" s="67"/>
       <c r="J18" s="44" t="e">
-        <f t="shared" ref="J18" si="16">F18/$B$27</f>
+        <f t="shared" ref="J18" si="16">F18/$B$30</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K18" s="43" t="e">
@@ -1750,7 +1750,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="L18" s="44" t="e">
-        <f t="shared" ref="L18" si="18">G18/$B$27</f>
+        <f t="shared" ref="L18" si="18">G18/$B$30</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M18" s="69"/>
@@ -1761,7 +1761,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="Q18" s="45" t="e">
-        <f t="shared" ref="Q18" si="19">I18/((F18/$B$27*$B$28)*R18)</f>
+        <f t="shared" ref="Q18" si="19">I18/((F18/$B$30*$B$31)*R18)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R18" s="45" t="e">
@@ -1780,15 +1780,15 @@
       <c r="H19" s="66"/>
       <c r="I19" s="67"/>
       <c r="J19" s="44" t="e">
-        <f t="shared" ref="J19:J20" si="20">F19/$B$27</f>
+        <f t="shared" ref="J19:J23" si="20">F19/$B$30</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K19" s="43" t="e">
-        <f t="shared" ref="K19:K20" si="21">J19*(M19/L19)</f>
+        <f t="shared" ref="K19:K23" si="21">J19*(M19/L19)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="L19" s="44" t="e">
-        <f t="shared" ref="L19:L20" si="22">G19/$B$27</f>
+        <f t="shared" ref="L19:L23" si="22">G19/$B$30</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M19" s="69"/>
@@ -1799,7 +1799,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="Q19" s="45" t="e">
-        <f t="shared" ref="Q19:Q20" si="23">I19/((F19/$B$27*$B$28)*R19)</f>
+        <f t="shared" ref="Q19:Q23" si="23">I19/((F19/$B$30*$B$31)*R19)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R19" s="45" t="e">
@@ -1818,34 +1818,34 @@
       <c r="H20" s="66"/>
       <c r="I20" s="67"/>
       <c r="J20" s="44" t="e">
-        <f t="shared" si="20"/>
+        <f t="shared" ref="J20" si="24">F20/$B$30</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K20" s="43" t="e">
-        <f t="shared" si="21"/>
+        <f t="shared" ref="K20" si="25">J20*(M20/L20)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="L20" s="44" t="e">
-        <f t="shared" si="22"/>
+        <f t="shared" ref="L20" si="26">G20/$B$30</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M20" s="69"/>
       <c r="N20" s="61"/>
       <c r="O20" s="61"/>
       <c r="P20" s="30" t="e">
-        <f t="shared" ref="P20" si="24">I20/(J20*$B$28)</f>
+        <f t="shared" ref="P20" si="27">I20/(J20*$B$31)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q20" s="45" t="e">
-        <f t="shared" si="23"/>
+        <f t="shared" ref="Q20" si="28">I20/((F20/$B$30*$B$31)*R20)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R20" s="45" t="e">
-        <f t="shared" ref="R20" si="25">H20/(L20*$B$28)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="21" spans="1:19" ht="12.45" customHeight="1" thickBot="1">
+        <f t="shared" ref="R20" si="29">H20/(L20*$B$31)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" ht="12.45" customHeight="1">
       <c r="A21" s="40"/>
       <c r="B21" s="41"/>
       <c r="C21" s="42"/>
@@ -1856,15 +1856,15 @@
       <c r="H21" s="66"/>
       <c r="I21" s="67"/>
       <c r="J21" s="44" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="20"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K21" s="43" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="21"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L21" s="44" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="22"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M21" s="69"/>
@@ -1875,7 +1875,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="Q21" s="45" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="23"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R21" s="45" t="e">
@@ -1883,87 +1883,201 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="22" spans="1:19" ht="13.05" customHeight="1" thickBot="1">
-      <c r="A22" s="46"/>
-      <c r="B22" s="47" t="s">
+    <row r="22" spans="1:19" ht="12.45" customHeight="1">
+      <c r="A22" s="40"/>
+      <c r="B22" s="41"/>
+      <c r="C22" s="42"/>
+      <c r="D22" s="61"/>
+      <c r="E22" s="63"/>
+      <c r="F22" s="61"/>
+      <c r="G22" s="63"/>
+      <c r="H22" s="66"/>
+      <c r="I22" s="67"/>
+      <c r="J22" s="44" t="e">
+        <f t="shared" ref="J22" si="30">F22/$B$30</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K22" s="43" t="e">
+        <f t="shared" ref="K22" si="31">J22*(M22/L22)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L22" s="44" t="e">
+        <f t="shared" ref="L22" si="32">G22/$B$30</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M22" s="69"/>
+      <c r="N22" s="61"/>
+      <c r="O22" s="61"/>
+      <c r="P22" s="30" t="e">
+        <f t="shared" ref="P22" si="33">I22/(J22*$B$31)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q22" s="45" t="e">
+        <f t="shared" ref="Q22" si="34">I22/((F22/$B$30*$B$31)*R22)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R22" s="45" t="e">
+        <f t="shared" ref="R22" si="35">H22/(L22*$B$31)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" ht="12.45" customHeight="1">
+      <c r="A23" s="40"/>
+      <c r="B23" s="41"/>
+      <c r="C23" s="42"/>
+      <c r="D23" s="61"/>
+      <c r="E23" s="63"/>
+      <c r="F23" s="61"/>
+      <c r="G23" s="63"/>
+      <c r="H23" s="66"/>
+      <c r="I23" s="67"/>
+      <c r="J23" s="44" t="e">
+        <f t="shared" si="20"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K23" s="43" t="e">
+        <f t="shared" si="21"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L23" s="44" t="e">
+        <f t="shared" si="22"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M23" s="69"/>
+      <c r="N23" s="61"/>
+      <c r="O23" s="61"/>
+      <c r="P23" s="30" t="e">
+        <f t="shared" ref="P23" si="36">I23/(J23*$B$31)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q23" s="45" t="e">
+        <f t="shared" si="23"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R23" s="45" t="e">
+        <f t="shared" ref="R23" si="37">H23/(L23*$B$31)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" ht="12.45" customHeight="1" thickBot="1">
+      <c r="A24" s="40"/>
+      <c r="B24" s="41"/>
+      <c r="C24" s="42"/>
+      <c r="D24" s="61"/>
+      <c r="E24" s="63"/>
+      <c r="F24" s="61"/>
+      <c r="G24" s="63"/>
+      <c r="H24" s="66"/>
+      <c r="I24" s="67"/>
+      <c r="J24" s="44" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K24" s="43" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L24" s="44" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M24" s="69"/>
+      <c r="N24" s="61"/>
+      <c r="O24" s="61"/>
+      <c r="P24" s="30" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q24" s="45" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R24" s="45" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" ht="13.05" customHeight="1" thickBot="1">
+      <c r="A25" s="46"/>
+      <c r="B25" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="C22" s="48"/>
-      <c r="D22" s="49">
-        <f t="shared" ref="D22:N22" si="26">SUM(D10:D21)</f>
+      <c r="C25" s="48"/>
+      <c r="D25" s="49">
+        <f t="shared" ref="D25:N25" si="38">SUM(D10:D24)</f>
         <v>0</v>
       </c>
-      <c r="E22" s="49">
-        <f t="shared" si="26"/>
+      <c r="E25" s="49">
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
-      <c r="F22" s="49">
-        <f t="shared" si="26"/>
+      <c r="F25" s="49">
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
-      <c r="G22" s="49">
-        <f t="shared" si="26"/>
+      <c r="G25" s="49">
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
-      <c r="H22" s="49">
-        <f t="shared" si="26"/>
+      <c r="H25" s="49">
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
-      <c r="I22" s="50">
-        <f t="shared" si="26"/>
+      <c r="I25" s="50">
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
-      <c r="J22" s="51" t="e">
-        <f t="shared" si="26"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K22" s="52" t="e">
-        <f t="shared" si="26"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L22" s="52" t="e">
-        <f t="shared" si="26"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M22" s="53">
-        <f t="shared" si="26"/>
+      <c r="J25" s="51" t="e">
+        <f t="shared" si="38"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K25" s="52" t="e">
+        <f t="shared" si="38"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L25" s="52" t="e">
+        <f t="shared" si="38"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M25" s="53">
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
-      <c r="N22" s="54">
-        <f t="shared" si="26"/>
+      <c r="N25" s="54">
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
-      <c r="O22" s="54"/>
-      <c r="P22" s="57" t="e">
+      <c r="O25" s="54"/>
+      <c r="P25" s="57" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="Q22" s="57" t="e">
+      <c r="Q25" s="57" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="R22" s="57" t="e">
+      <c r="R25" s="57" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="S22" s="58"/>
-    </row>
-    <row r="24" spans="1:19" ht="12.45" customHeight="1">
-      <c r="Q24" s="59"/>
+      <c r="S25" s="58"/>
     </row>
     <row r="27" spans="1:19" ht="12.45" customHeight="1">
-      <c r="A27" s="56" t="s">
+      <c r="Q27" s="59"/>
+    </row>
+    <row r="30" spans="1:19" ht="12.45" customHeight="1">
+      <c r="A30" s="56" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="56"/>
-      <c r="C27" s="55"/>
-    </row>
-    <row r="28" spans="1:19" ht="12.45" customHeight="1">
-      <c r="A28" s="56" t="s">
+      <c r="B30" s="56"/>
+      <c r="C30" s="55"/>
+    </row>
+    <row r="31" spans="1:19" ht="12.45" customHeight="1">
+      <c r="A31" s="56" t="s">
         <v>26</v>
       </c>
-      <c r="B28" s="56"/>
-      <c r="C28" s="55"/>
+      <c r="B31" s="56"/>
+      <c r="C31" s="55"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
@@ -1984,8 +2098,8 @@
 &amp;I© 2017 SunEdison&amp;I &amp;C&amp;R&amp;"Arial"&amp;8 Page 1 of 2 </oddFooter>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="D22:H22 J10:L13 P10:R13 P22:R22 J22:N22" unlockedFormula="1"/>
-    <ignoredError sqref="I22" formula="1" unlockedFormula="1"/>
+    <ignoredError sqref="D25:H25 J10:L13 P10:R13 P25:R25 J25:N25" unlockedFormula="1"/>
+    <ignoredError sqref="I25" formula="1" unlockedFormula="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add rows in daily/monthly report templates
</commit_message>
<xml_diff>
--- a/job/templates/DailyReport-v3.xlsx
+++ b/job/templates/DailyReport-v3.xlsx
@@ -1226,11 +1226,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S39"/>
+  <dimension ref="A1:S41"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomLeft" activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.45" customHeight="1"/>
@@ -1438,30 +1438,30 @@
       <c r="H10" s="64"/>
       <c r="I10" s="65"/>
       <c r="J10" s="39" t="e">
-        <f t="shared" ref="J10:J32" si="0">F10/$B$38</f>
+        <f t="shared" ref="J10:J34" si="0">F10/$B$40</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K10" s="38" t="e">
-        <f t="shared" ref="K10:K32" si="1">J10*(M10/L10)</f>
+        <f t="shared" ref="K10:K34" si="1">J10*(M10/L10)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="L10" s="39" t="e">
-        <f t="shared" ref="L10:L32" si="2">G10/$B$38</f>
+        <f t="shared" ref="L10:L34" si="2">G10/$B$40</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M10" s="68"/>
       <c r="N10" s="60"/>
       <c r="O10" s="60"/>
       <c r="P10" s="30" t="e">
-        <f>I10/(J10*$B$39)</f>
+        <f>I10/(J10*$B$41)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q10" s="33" t="e">
-        <f>I10/((J10*$B$39)*R10)</f>
+        <f>I10/((J10*$B$41)*R10)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R10" s="33" t="e">
-        <f>H10/(L10*$B$39)</f>
+        <f>H10/(L10*$B$41)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1491,15 +1491,15 @@
       <c r="N11" s="60"/>
       <c r="O11" s="60"/>
       <c r="P11" s="30" t="e">
-        <f>I11/(J11*$B$39)</f>
+        <f>I11/(J11*$B$41)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q11" s="33" t="e">
-        <f t="shared" ref="Q11:Q33" si="3">I11/((F11/$B$38*$B$39)*R11)</f>
+        <f t="shared" ref="Q11:Q35" si="3">I11/((F11/$B$40*$B$41)*R11)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R11" s="33" t="e">
-        <f>H11/(L11*$B$39)</f>
+        <f>H11/(L11*$B$41)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1529,7 +1529,7 @@
       <c r="N12" s="60"/>
       <c r="O12" s="60"/>
       <c r="P12" s="30" t="e">
-        <f>I12/(J12*$B$39)</f>
+        <f>I12/(J12*$B$41)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q12" s="33" t="e">
@@ -1537,7 +1537,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="R12" s="33" t="e">
-        <f>H12/(L12*$B$39)</f>
+        <f>H12/(L12*$B$41)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1567,7 +1567,7 @@
       <c r="N13" s="60"/>
       <c r="O13" s="60"/>
       <c r="P13" s="30" t="e">
-        <f>I13/(J13*$B$39)</f>
+        <f>I13/(J13*$B$41)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q13" s="33" t="e">
@@ -1575,7 +1575,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="R13" s="33" t="e">
-        <f>H13/(L13*$B$39)</f>
+        <f>H13/(L13*$B$41)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1605,7 +1605,7 @@
       <c r="N14" s="61"/>
       <c r="O14" s="61"/>
       <c r="P14" s="30" t="e">
-        <f t="shared" ref="P14" si="4">I14/(J14*$B$39)</f>
+        <f t="shared" ref="P14" si="4">I14/(J14*$B$41)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q14" s="45" t="e">
@@ -1613,7 +1613,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="R14" s="45" t="e">
-        <f t="shared" ref="R14" si="5">H14/(L14*$B$39)</f>
+        <f t="shared" ref="R14" si="5">H14/(L14*$B$41)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1643,7 +1643,7 @@
       <c r="N15" s="61"/>
       <c r="O15" s="61"/>
       <c r="P15" s="30" t="e">
-        <f t="shared" ref="P15:P33" si="7">I15/(J15*$B$39)</f>
+        <f t="shared" ref="P15:P35" si="7">I15/(J15*$B$41)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q15" s="45" t="e">
@@ -1651,7 +1651,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="R15" s="45" t="e">
-        <f t="shared" ref="R15:R33" si="8">H15/(L15*$B$39)</f>
+        <f t="shared" ref="R15:R35" si="8">H15/(L15*$B$41)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1666,7 +1666,7 @@
       <c r="H16" s="66"/>
       <c r="I16" s="67"/>
       <c r="J16" s="44" t="e">
-        <f t="shared" ref="J16" si="9">F16/$B$38</f>
+        <f t="shared" ref="J16" si="9">F16/$B$40</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K16" s="43" t="e">
@@ -1674,7 +1674,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="L16" s="44" t="e">
-        <f t="shared" ref="L16" si="10">G16/$B$38</f>
+        <f t="shared" ref="L16" si="10">G16/$B$40</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M16" s="69"/>
@@ -1685,7 +1685,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="Q16" s="45" t="e">
-        <f t="shared" ref="Q16" si="11">I16/((F16/$B$38*$B$39)*R16)</f>
+        <f t="shared" ref="Q16" si="11">I16/((F16/$B$40*$B$41)*R16)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R16" s="45" t="e">
@@ -1704,7 +1704,7 @@
       <c r="H17" s="66"/>
       <c r="I17" s="67"/>
       <c r="J17" s="44" t="e">
-        <f t="shared" ref="J17" si="12">F17/$B$38</f>
+        <f t="shared" ref="J17" si="12">F17/$B$40</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K17" s="43" t="e">
@@ -1712,7 +1712,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="L17" s="44" t="e">
-        <f t="shared" ref="L17" si="14">G17/$B$38</f>
+        <f t="shared" ref="L17" si="14">G17/$B$40</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M17" s="69"/>
@@ -1723,7 +1723,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="Q17" s="45" t="e">
-        <f t="shared" ref="Q17" si="15">I17/((F17/$B$38*$B$39)*R17)</f>
+        <f t="shared" ref="Q17" si="15">I17/((F17/$B$40*$B$41)*R17)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R17" s="45" t="e">
@@ -1742,7 +1742,7 @@
       <c r="H18" s="66"/>
       <c r="I18" s="67"/>
       <c r="J18" s="44" t="e">
-        <f t="shared" ref="J18" si="16">F18/$B$38</f>
+        <f t="shared" ref="J18" si="16">F18/$B$40</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K18" s="43" t="e">
@@ -1750,7 +1750,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="L18" s="44" t="e">
-        <f t="shared" ref="L18" si="18">G18/$B$38</f>
+        <f t="shared" ref="L18" si="18">G18/$B$40</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M18" s="69"/>
@@ -1761,7 +1761,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="Q18" s="45" t="e">
-        <f t="shared" ref="Q18" si="19">I18/((F18/$B$38*$B$39)*R18)</f>
+        <f t="shared" ref="Q18" si="19">I18/((F18/$B$40*$B$41)*R18)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R18" s="45" t="e">
@@ -1780,7 +1780,7 @@
       <c r="H19" s="66"/>
       <c r="I19" s="67"/>
       <c r="J19" s="44" t="e">
-        <f t="shared" ref="J19:J26" si="20">F19/$B$38</f>
+        <f t="shared" ref="J19:J26" si="20">F19/$B$40</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K19" s="43" t="e">
@@ -1788,7 +1788,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="L19" s="44" t="e">
-        <f t="shared" ref="L19:L26" si="22">G19/$B$38</f>
+        <f t="shared" ref="L19:L26" si="22">G19/$B$40</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M19" s="69"/>
@@ -1799,7 +1799,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="Q19" s="45" t="e">
-        <f t="shared" ref="Q19:Q26" si="23">I19/((F19/$B$38*$B$39)*R19)</f>
+        <f t="shared" ref="Q19:Q26" si="23">I19/((F19/$B$40*$B$41)*R19)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R19" s="45" t="e">
@@ -1818,7 +1818,7 @@
       <c r="H20" s="66"/>
       <c r="I20" s="67"/>
       <c r="J20" s="44" t="e">
-        <f t="shared" ref="J20" si="24">F20/$B$38</f>
+        <f t="shared" ref="J20" si="24">F20/$B$40</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K20" s="43" t="e">
@@ -1826,22 +1826,22 @@
         <v>#DIV/0!</v>
       </c>
       <c r="L20" s="44" t="e">
-        <f t="shared" ref="L20" si="26">G20/$B$38</f>
+        <f t="shared" ref="L20" si="26">G20/$B$40</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M20" s="69"/>
       <c r="N20" s="61"/>
       <c r="O20" s="61"/>
       <c r="P20" s="30" t="e">
-        <f t="shared" ref="P20" si="27">I20/(J20*$B$39)</f>
+        <f t="shared" ref="P20" si="27">I20/(J20*$B$41)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q20" s="45" t="e">
-        <f t="shared" ref="Q20" si="28">I20/((F20/$B$38*$B$39)*R20)</f>
+        <f t="shared" ref="Q20" si="28">I20/((F20/$B$40*$B$41)*R20)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R20" s="45" t="e">
-        <f t="shared" ref="R20" si="29">H20/(L20*$B$39)</f>
+        <f t="shared" ref="R20" si="29">H20/(L20*$B$41)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1894,7 +1894,7 @@
       <c r="H22" s="66"/>
       <c r="I22" s="67"/>
       <c r="J22" s="44" t="e">
-        <f t="shared" ref="J22:J23" si="30">F22/$B$38</f>
+        <f t="shared" ref="J22:J23" si="30">F22/$B$40</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K22" s="43" t="e">
@@ -1902,22 +1902,22 @@
         <v>#DIV/0!</v>
       </c>
       <c r="L22" s="44" t="e">
-        <f t="shared" ref="L22:L23" si="32">G22/$B$38</f>
+        <f t="shared" ref="L22:L23" si="32">G22/$B$40</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M22" s="69"/>
       <c r="N22" s="61"/>
       <c r="O22" s="61"/>
       <c r="P22" s="30" t="e">
-        <f t="shared" ref="P22:P23" si="33">I22/(J22*$B$39)</f>
+        <f t="shared" ref="P22:P23" si="33">I22/(J22*$B$41)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q22" s="45" t="e">
-        <f t="shared" ref="Q22:Q23" si="34">I22/((F22/$B$38*$B$39)*R22)</f>
+        <f t="shared" ref="Q22:Q23" si="34">I22/((F22/$B$40*$B$41)*R22)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R22" s="45" t="e">
-        <f t="shared" ref="R22:R23" si="35">H22/(L22*$B$39)</f>
+        <f t="shared" ref="R22:R23" si="35">H22/(L22*$B$41)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1970,7 +1970,7 @@
       <c r="H24" s="66"/>
       <c r="I24" s="67"/>
       <c r="J24" s="44" t="e">
-        <f t="shared" ref="J24" si="36">F24/$B$38</f>
+        <f t="shared" ref="J24" si="36">F24/$B$40</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K24" s="43" t="e">
@@ -1978,22 +1978,22 @@
         <v>#DIV/0!</v>
       </c>
       <c r="L24" s="44" t="e">
-        <f t="shared" ref="L24" si="38">G24/$B$38</f>
+        <f t="shared" ref="L24" si="38">G24/$B$40</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M24" s="69"/>
       <c r="N24" s="61"/>
       <c r="O24" s="61"/>
       <c r="P24" s="30" t="e">
-        <f t="shared" ref="P24" si="39">I24/(J24*$B$39)</f>
+        <f t="shared" ref="P24" si="39">I24/(J24*$B$41)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q24" s="45" t="e">
-        <f t="shared" ref="Q24" si="40">I24/((F24/$B$38*$B$39)*R24)</f>
+        <f t="shared" ref="Q24" si="40">I24/((F24/$B$40*$B$41)*R24)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R24" s="45" t="e">
-        <f t="shared" ref="R24" si="41">H24/(L24*$B$39)</f>
+        <f t="shared" ref="R24" si="41">H24/(L24*$B$41)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2023,7 +2023,7 @@
       <c r="N25" s="61"/>
       <c r="O25" s="61"/>
       <c r="P25" s="30" t="e">
-        <f t="shared" ref="P25:P26" si="42">I25/(J25*$B$39)</f>
+        <f t="shared" ref="P25:P26" si="42">I25/(J25*$B$41)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q25" s="45" t="e">
@@ -2031,7 +2031,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="R25" s="45" t="e">
-        <f t="shared" ref="R25:R26" si="43">H25/(L25*$B$39)</f>
+        <f t="shared" ref="R25:R26" si="43">H25/(L25*$B$41)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2084,7 +2084,7 @@
       <c r="H27" s="66"/>
       <c r="I27" s="67"/>
       <c r="J27" s="44" t="e">
-        <f t="shared" ref="J27" si="44">F27/$B$38</f>
+        <f t="shared" ref="J27" si="44">F27/$B$40</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K27" s="43" t="e">
@@ -2092,22 +2092,22 @@
         <v>#DIV/0!</v>
       </c>
       <c r="L27" s="44" t="e">
-        <f t="shared" ref="L27" si="46">G27/$B$38</f>
+        <f t="shared" ref="L27" si="46">G27/$B$40</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M27" s="69"/>
       <c r="N27" s="61"/>
       <c r="O27" s="61"/>
       <c r="P27" s="30" t="e">
-        <f t="shared" ref="P27" si="47">I27/(J27*$B$39)</f>
+        <f t="shared" ref="P27" si="47">I27/(J27*$B$41)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q27" s="45" t="e">
-        <f t="shared" ref="Q27" si="48">I27/((F27/$B$38*$B$39)*R27)</f>
+        <f t="shared" ref="Q27" si="48">I27/((F27/$B$40*$B$41)*R27)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R27" s="45" t="e">
-        <f t="shared" ref="R27" si="49">H27/(L27*$B$39)</f>
+        <f t="shared" ref="R27" si="49">H27/(L27*$B$41)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2122,7 +2122,7 @@
       <c r="H28" s="66"/>
       <c r="I28" s="67"/>
       <c r="J28" s="44" t="e">
-        <f t="shared" ref="J28:J29" si="50">F28/$B$38</f>
+        <f t="shared" ref="J28:J29" si="50">F28/$B$40</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K28" s="43" t="e">
@@ -2130,22 +2130,22 @@
         <v>#DIV/0!</v>
       </c>
       <c r="L28" s="44" t="e">
-        <f t="shared" ref="L28:L29" si="52">G28/$B$38</f>
+        <f t="shared" ref="L28:L29" si="52">G28/$B$40</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M28" s="69"/>
       <c r="N28" s="61"/>
       <c r="O28" s="61"/>
       <c r="P28" s="30" t="e">
-        <f t="shared" ref="P28:P29" si="53">I28/(J28*$B$39)</f>
+        <f t="shared" ref="P28:P29" si="53">I28/(J28*$B$41)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q28" s="45" t="e">
-        <f t="shared" ref="Q28:Q29" si="54">I28/((F28/$B$38*$B$39)*R28)</f>
+        <f t="shared" ref="Q28:Q29" si="54">I28/((F28/$B$40*$B$41)*R28)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R28" s="45" t="e">
-        <f t="shared" ref="R28:R29" si="55">H28/(L28*$B$39)</f>
+        <f t="shared" ref="R28:R29" si="55">H28/(L28*$B$41)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2198,7 +2198,7 @@
       <c r="H30" s="66"/>
       <c r="I30" s="67"/>
       <c r="J30" s="44" t="e">
-        <f t="shared" ref="J30" si="56">F30/$B$38</f>
+        <f t="shared" ref="J30" si="56">F30/$B$40</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K30" s="43" t="e">
@@ -2206,22 +2206,22 @@
         <v>#DIV/0!</v>
       </c>
       <c r="L30" s="44" t="e">
-        <f t="shared" ref="L30" si="58">G30/$B$38</f>
+        <f t="shared" ref="L30" si="58">G30/$B$40</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M30" s="69"/>
       <c r="N30" s="61"/>
       <c r="O30" s="61"/>
       <c r="P30" s="30" t="e">
-        <f t="shared" ref="P30" si="59">I30/(J30*$B$39)</f>
+        <f t="shared" ref="P30" si="59">I30/(J30*$B$41)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q30" s="45" t="e">
-        <f t="shared" ref="Q30" si="60">I30/((F30/$B$38*$B$39)*R30)</f>
+        <f t="shared" ref="Q30" si="60">I30/((F30/$B$40*$B$41)*R30)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R30" s="45" t="e">
-        <f t="shared" ref="R30" si="61">H30/(L30*$B$39)</f>
+        <f t="shared" ref="R30" si="61">H30/(L30*$B$41)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2236,7 +2236,7 @@
       <c r="H31" s="66"/>
       <c r="I31" s="67"/>
       <c r="J31" s="44" t="e">
-        <f t="shared" ref="J31" si="62">F31/$B$38</f>
+        <f t="shared" ref="J31" si="62">F31/$B$40</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K31" s="43" t="e">
@@ -2244,26 +2244,26 @@
         <v>#DIV/0!</v>
       </c>
       <c r="L31" s="44" t="e">
-        <f t="shared" ref="L31" si="64">G31/$B$38</f>
+        <f t="shared" ref="L31" si="64">G31/$B$40</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M31" s="69"/>
       <c r="N31" s="61"/>
       <c r="O31" s="61"/>
       <c r="P31" s="30" t="e">
-        <f t="shared" ref="P31" si="65">I31/(J31*$B$39)</f>
+        <f t="shared" ref="P31" si="65">I31/(J31*$B$41)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q31" s="45" t="e">
-        <f t="shared" ref="Q31" si="66">I31/((F31/$B$38*$B$39)*R31)</f>
+        <f t="shared" ref="Q31" si="66">I31/((F31/$B$40*$B$41)*R31)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R31" s="45" t="e">
-        <f t="shared" ref="R31" si="67">H31/(L31*$B$39)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="32" spans="1:18" ht="12.45" customHeight="1" thickBot="1">
+        <f t="shared" ref="R31" si="67">H31/(L31*$B$41)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" ht="12.45" customHeight="1">
       <c r="A32" s="40"/>
       <c r="B32" s="41"/>
       <c r="C32" s="42"/>
@@ -2274,114 +2274,190 @@
       <c r="H32" s="66"/>
       <c r="I32" s="67"/>
       <c r="J32" s="44" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="J32" si="68">F32/$B$40</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K32" s="43" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="K32" si="69">J32*(M32/L32)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="L32" s="44" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="L32" si="70">G32/$B$40</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M32" s="69"/>
       <c r="N32" s="61"/>
       <c r="O32" s="61"/>
       <c r="P32" s="30" t="e">
+        <f t="shared" ref="P32" si="71">I32/(J32*$B$41)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q32" s="45" t="e">
+        <f t="shared" ref="Q32" si="72">I32/((F32/$B$40*$B$41)*R32)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R32" s="45" t="e">
+        <f t="shared" ref="R32" si="73">H32/(L32*$B$41)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" ht="12.45" customHeight="1">
+      <c r="A33" s="40"/>
+      <c r="B33" s="41"/>
+      <c r="C33" s="42"/>
+      <c r="D33" s="61"/>
+      <c r="E33" s="63"/>
+      <c r="F33" s="61"/>
+      <c r="G33" s="63"/>
+      <c r="H33" s="66"/>
+      <c r="I33" s="67"/>
+      <c r="J33" s="44" t="e">
+        <f t="shared" ref="J33" si="74">F33/$B$40</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K33" s="43" t="e">
+        <f t="shared" ref="K33" si="75">J33*(M33/L33)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L33" s="44" t="e">
+        <f t="shared" ref="L33" si="76">G33/$B$40</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M33" s="69"/>
+      <c r="N33" s="61"/>
+      <c r="O33" s="61"/>
+      <c r="P33" s="30" t="e">
+        <f t="shared" ref="P33" si="77">I33/(J33*$B$41)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q33" s="45" t="e">
+        <f t="shared" ref="Q33" si="78">I33/((F33/$B$40*$B$41)*R33)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R33" s="45" t="e">
+        <f t="shared" ref="R33" si="79">H33/(L33*$B$41)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" ht="12.45" customHeight="1" thickBot="1">
+      <c r="A34" s="40"/>
+      <c r="B34" s="41"/>
+      <c r="C34" s="42"/>
+      <c r="D34" s="61"/>
+      <c r="E34" s="63"/>
+      <c r="F34" s="61"/>
+      <c r="G34" s="63"/>
+      <c r="H34" s="66"/>
+      <c r="I34" s="67"/>
+      <c r="J34" s="44" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K34" s="43" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L34" s="44" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M34" s="69"/>
+      <c r="N34" s="61"/>
+      <c r="O34" s="61"/>
+      <c r="P34" s="30" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="Q32" s="45" t="e">
+      <c r="Q34" s="45" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="R32" s="45" t="e">
+      <c r="R34" s="45" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="33" spans="1:19" ht="13.05" customHeight="1" thickBot="1">
-      <c r="A33" s="46"/>
-      <c r="B33" s="47" t="s">
+    <row r="35" spans="1:19" ht="13.05" customHeight="1" thickBot="1">
+      <c r="A35" s="46"/>
+      <c r="B35" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="C33" s="48"/>
-      <c r="D33" s="49">
-        <f t="shared" ref="D33:N33" si="68">SUM(D10:D32)</f>
+      <c r="C35" s="48"/>
+      <c r="D35" s="49">
+        <f t="shared" ref="D35:N35" si="80">SUM(D10:D34)</f>
         <v>0</v>
       </c>
-      <c r="E33" s="49">
-        <f t="shared" si="68"/>
+      <c r="E35" s="49">
+        <f t="shared" si="80"/>
         <v>0</v>
       </c>
-      <c r="F33" s="49">
-        <f t="shared" si="68"/>
+      <c r="F35" s="49">
+        <f t="shared" si="80"/>
         <v>0</v>
       </c>
-      <c r="G33" s="49">
-        <f t="shared" si="68"/>
+      <c r="G35" s="49">
+        <f t="shared" si="80"/>
         <v>0</v>
       </c>
-      <c r="H33" s="49">
-        <f t="shared" si="68"/>
+      <c r="H35" s="49">
+        <f t="shared" si="80"/>
         <v>0</v>
       </c>
-      <c r="I33" s="50">
-        <f t="shared" si="68"/>
+      <c r="I35" s="50">
+        <f t="shared" si="80"/>
         <v>0</v>
       </c>
-      <c r="J33" s="51" t="e">
-        <f t="shared" si="68"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K33" s="52" t="e">
-        <f t="shared" si="68"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L33" s="52" t="e">
-        <f t="shared" si="68"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M33" s="53">
-        <f t="shared" si="68"/>
+      <c r="J35" s="51" t="e">
+        <f t="shared" si="80"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K35" s="52" t="e">
+        <f t="shared" si="80"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L35" s="52" t="e">
+        <f t="shared" si="80"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M35" s="53">
+        <f t="shared" si="80"/>
         <v>0</v>
       </c>
-      <c r="N33" s="54">
-        <f t="shared" si="68"/>
+      <c r="N35" s="54">
+        <f t="shared" si="80"/>
         <v>0</v>
       </c>
-      <c r="O33" s="54"/>
-      <c r="P33" s="57" t="e">
+      <c r="O35" s="54"/>
+      <c r="P35" s="57" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="Q33" s="57" t="e">
+      <c r="Q35" s="57" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="R33" s="57" t="e">
+      <c r="R35" s="57" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="S33" s="58"/>
-    </row>
-    <row r="35" spans="1:19" ht="12.45" customHeight="1">
-      <c r="Q35" s="59"/>
-    </row>
-    <row r="38" spans="1:19" ht="12.45" customHeight="1">
-      <c r="A38" s="56" t="s">
+      <c r="S35" s="58"/>
+    </row>
+    <row r="37" spans="1:19" ht="12.45" customHeight="1">
+      <c r="Q37" s="59"/>
+    </row>
+    <row r="40" spans="1:19" ht="12.45" customHeight="1">
+      <c r="A40" s="56" t="s">
         <v>25</v>
       </c>
-      <c r="B38" s="56"/>
-      <c r="C38" s="55"/>
-    </row>
-    <row r="39" spans="1:19" ht="12.45" customHeight="1">
-      <c r="A39" s="56" t="s">
+      <c r="B40" s="56"/>
+      <c r="C40" s="55"/>
+    </row>
+    <row r="41" spans="1:19" ht="12.45" customHeight="1">
+      <c r="A41" s="56" t="s">
         <v>26</v>
       </c>
-      <c r="B39" s="56"/>
-      <c r="C39" s="55"/>
+      <c r="B41" s="56"/>
+      <c r="C41" s="55"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
@@ -2402,8 +2478,8 @@
 &amp;I© 2017 SunEdison&amp;I &amp;C&amp;R&amp;"Arial"&amp;8 Page 1 of 2 </oddFooter>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="D33:H33 J10:L13 P10:R13 P33:R33 J33:N33" unlockedFormula="1"/>
-    <ignoredError sqref="I33" formula="1" unlockedFormula="1"/>
+    <ignoredError sqref="D35:H35 J10:L13 P10:R13 P35:R35 J35:N35" unlockedFormula="1"/>
+    <ignoredError sqref="I35" formula="1" unlockedFormula="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add rows for excel dailyreport/monthreport
</commit_message>
<xml_diff>
--- a/job/templates/DailyReport-v3.xlsx
+++ b/job/templates/DailyReport-v3.xlsx
@@ -1226,11 +1226,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S41"/>
+  <dimension ref="A1:S44"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A30" sqref="A30"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.45" customHeight="1"/>
@@ -1438,30 +1438,30 @@
       <c r="H10" s="64"/>
       <c r="I10" s="65"/>
       <c r="J10" s="39" t="e">
-        <f t="shared" ref="J10:J34" si="0">F10/$B$40</f>
+        <f t="shared" ref="J10:J37" si="0">F10/$B$43</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K10" s="38" t="e">
-        <f t="shared" ref="K10:K34" si="1">J10*(M10/L10)</f>
+        <f t="shared" ref="K10:K37" si="1">J10*(M10/L10)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="L10" s="39" t="e">
-        <f t="shared" ref="L10:L34" si="2">G10/$B$40</f>
+        <f t="shared" ref="L10:L37" si="2">G10/$B$43</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M10" s="68"/>
       <c r="N10" s="60"/>
       <c r="O10" s="60"/>
       <c r="P10" s="30" t="e">
-        <f>I10/(J10*$B$41)</f>
+        <f>I10/(J10*$B$44)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q10" s="33" t="e">
-        <f>I10/((J10*$B$41)*R10)</f>
+        <f>I10/((J10*$B$44)*R10)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R10" s="33" t="e">
-        <f>H10/(L10*$B$41)</f>
+        <f>H10/(L10*$B$44)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1491,15 +1491,15 @@
       <c r="N11" s="60"/>
       <c r="O11" s="60"/>
       <c r="P11" s="30" t="e">
-        <f>I11/(J11*$B$41)</f>
+        <f>I11/(J11*$B$44)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q11" s="33" t="e">
-        <f t="shared" ref="Q11:Q35" si="3">I11/((F11/$B$40*$B$41)*R11)</f>
+        <f t="shared" ref="Q11:Q38" si="3">I11/((F11/$B$43*$B$44)*R11)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R11" s="33" t="e">
-        <f>H11/(L11*$B$41)</f>
+        <f>H11/(L11*$B$44)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1529,7 +1529,7 @@
       <c r="N12" s="60"/>
       <c r="O12" s="60"/>
       <c r="P12" s="30" t="e">
-        <f>I12/(J12*$B$41)</f>
+        <f>I12/(J12*$B$44)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q12" s="33" t="e">
@@ -1537,7 +1537,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="R12" s="33" t="e">
-        <f>H12/(L12*$B$41)</f>
+        <f>H12/(L12*$B$44)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1567,7 +1567,7 @@
       <c r="N13" s="60"/>
       <c r="O13" s="60"/>
       <c r="P13" s="30" t="e">
-        <f>I13/(J13*$B$41)</f>
+        <f>I13/(J13*$B$44)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q13" s="33" t="e">
@@ -1575,7 +1575,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="R13" s="33" t="e">
-        <f>H13/(L13*$B$41)</f>
+        <f>H13/(L13*$B$44)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1605,7 +1605,7 @@
       <c r="N14" s="61"/>
       <c r="O14" s="61"/>
       <c r="P14" s="30" t="e">
-        <f t="shared" ref="P14" si="4">I14/(J14*$B$41)</f>
+        <f t="shared" ref="P14" si="4">I14/(J14*$B$44)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q14" s="45" t="e">
@@ -1613,7 +1613,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="R14" s="45" t="e">
-        <f t="shared" ref="R14" si="5">H14/(L14*$B$41)</f>
+        <f t="shared" ref="R14" si="5">H14/(L14*$B$44)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1643,7 +1643,7 @@
       <c r="N15" s="61"/>
       <c r="O15" s="61"/>
       <c r="P15" s="30" t="e">
-        <f t="shared" ref="P15:P35" si="7">I15/(J15*$B$41)</f>
+        <f t="shared" ref="P15:P38" si="7">I15/(J15*$B$44)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q15" s="45" t="e">
@@ -1651,7 +1651,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="R15" s="45" t="e">
-        <f t="shared" ref="R15:R35" si="8">H15/(L15*$B$41)</f>
+        <f t="shared" ref="R15:R38" si="8">H15/(L15*$B$44)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1666,7 +1666,7 @@
       <c r="H16" s="66"/>
       <c r="I16" s="67"/>
       <c r="J16" s="44" t="e">
-        <f t="shared" ref="J16" si="9">F16/$B$40</f>
+        <f t="shared" ref="J16" si="9">F16/$B$43</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K16" s="43" t="e">
@@ -1674,7 +1674,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="L16" s="44" t="e">
-        <f t="shared" ref="L16" si="10">G16/$B$40</f>
+        <f t="shared" ref="L16" si="10">G16/$B$43</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M16" s="69"/>
@@ -1685,7 +1685,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="Q16" s="45" t="e">
-        <f t="shared" ref="Q16" si="11">I16/((F16/$B$40*$B$41)*R16)</f>
+        <f t="shared" ref="Q16" si="11">I16/((F16/$B$43*$B$44)*R16)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R16" s="45" t="e">
@@ -1704,7 +1704,7 @@
       <c r="H17" s="66"/>
       <c r="I17" s="67"/>
       <c r="J17" s="44" t="e">
-        <f t="shared" ref="J17" si="12">F17/$B$40</f>
+        <f t="shared" ref="J17" si="12">F17/$B$43</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K17" s="43" t="e">
@@ -1712,7 +1712,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="L17" s="44" t="e">
-        <f t="shared" ref="L17" si="14">G17/$B$40</f>
+        <f t="shared" ref="L17" si="14">G17/$B$43</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M17" s="69"/>
@@ -1723,7 +1723,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="Q17" s="45" t="e">
-        <f t="shared" ref="Q17" si="15">I17/((F17/$B$40*$B$41)*R17)</f>
+        <f t="shared" ref="Q17" si="15">I17/((F17/$B$43*$B$44)*R17)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R17" s="45" t="e">
@@ -1742,7 +1742,7 @@
       <c r="H18" s="66"/>
       <c r="I18" s="67"/>
       <c r="J18" s="44" t="e">
-        <f t="shared" ref="J18" si="16">F18/$B$40</f>
+        <f t="shared" ref="J18" si="16">F18/$B$43</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K18" s="43" t="e">
@@ -1750,7 +1750,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="L18" s="44" t="e">
-        <f t="shared" ref="L18" si="18">G18/$B$40</f>
+        <f t="shared" ref="L18" si="18">G18/$B$43</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M18" s="69"/>
@@ -1761,7 +1761,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="Q18" s="45" t="e">
-        <f t="shared" ref="Q18" si="19">I18/((F18/$B$40*$B$41)*R18)</f>
+        <f t="shared" ref="Q18" si="19">I18/((F18/$B$43*$B$44)*R18)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R18" s="45" t="e">
@@ -1780,7 +1780,7 @@
       <c r="H19" s="66"/>
       <c r="I19" s="67"/>
       <c r="J19" s="44" t="e">
-        <f t="shared" ref="J19:J26" si="20">F19/$B$40</f>
+        <f t="shared" ref="J19:J26" si="20">F19/$B$43</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K19" s="43" t="e">
@@ -1788,7 +1788,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="L19" s="44" t="e">
-        <f t="shared" ref="L19:L26" si="22">G19/$B$40</f>
+        <f t="shared" ref="L19:L26" si="22">G19/$B$43</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M19" s="69"/>
@@ -1799,7 +1799,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="Q19" s="45" t="e">
-        <f t="shared" ref="Q19:Q26" si="23">I19/((F19/$B$40*$B$41)*R19)</f>
+        <f t="shared" ref="Q19:Q26" si="23">I19/((F19/$B$43*$B$44)*R19)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R19" s="45" t="e">
@@ -1818,7 +1818,7 @@
       <c r="H20" s="66"/>
       <c r="I20" s="67"/>
       <c r="J20" s="44" t="e">
-        <f t="shared" ref="J20" si="24">F20/$B$40</f>
+        <f t="shared" ref="J20" si="24">F20/$B$43</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K20" s="43" t="e">
@@ -1826,22 +1826,22 @@
         <v>#DIV/0!</v>
       </c>
       <c r="L20" s="44" t="e">
-        <f t="shared" ref="L20" si="26">G20/$B$40</f>
+        <f t="shared" ref="L20" si="26">G20/$B$43</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M20" s="69"/>
       <c r="N20" s="61"/>
       <c r="O20" s="61"/>
       <c r="P20" s="30" t="e">
-        <f t="shared" ref="P20" si="27">I20/(J20*$B$41)</f>
+        <f t="shared" ref="P20" si="27">I20/(J20*$B$44)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q20" s="45" t="e">
-        <f t="shared" ref="Q20" si="28">I20/((F20/$B$40*$B$41)*R20)</f>
+        <f t="shared" ref="Q20" si="28">I20/((F20/$B$43*$B$44)*R20)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R20" s="45" t="e">
-        <f t="shared" ref="R20" si="29">H20/(L20*$B$41)</f>
+        <f t="shared" ref="R20" si="29">H20/(L20*$B$44)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1894,7 +1894,7 @@
       <c r="H22" s="66"/>
       <c r="I22" s="67"/>
       <c r="J22" s="44" t="e">
-        <f t="shared" ref="J22:J23" si="30">F22/$B$40</f>
+        <f t="shared" ref="J22:J23" si="30">F22/$B$43</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K22" s="43" t="e">
@@ -1902,22 +1902,22 @@
         <v>#DIV/0!</v>
       </c>
       <c r="L22" s="44" t="e">
-        <f t="shared" ref="L22:L23" si="32">G22/$B$40</f>
+        <f t="shared" ref="L22:L23" si="32">G22/$B$43</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M22" s="69"/>
       <c r="N22" s="61"/>
       <c r="O22" s="61"/>
       <c r="P22" s="30" t="e">
-        <f t="shared" ref="P22:P23" si="33">I22/(J22*$B$41)</f>
+        <f t="shared" ref="P22:P23" si="33">I22/(J22*$B$44)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q22" s="45" t="e">
-        <f t="shared" ref="Q22:Q23" si="34">I22/((F22/$B$40*$B$41)*R22)</f>
+        <f t="shared" ref="Q22:Q23" si="34">I22/((F22/$B$43*$B$44)*R22)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R22" s="45" t="e">
-        <f t="shared" ref="R22:R23" si="35">H22/(L22*$B$41)</f>
+        <f t="shared" ref="R22:R23" si="35">H22/(L22*$B$44)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1970,7 +1970,7 @@
       <c r="H24" s="66"/>
       <c r="I24" s="67"/>
       <c r="J24" s="44" t="e">
-        <f t="shared" ref="J24" si="36">F24/$B$40</f>
+        <f t="shared" ref="J24" si="36">F24/$B$43</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K24" s="43" t="e">
@@ -1978,22 +1978,22 @@
         <v>#DIV/0!</v>
       </c>
       <c r="L24" s="44" t="e">
-        <f t="shared" ref="L24" si="38">G24/$B$40</f>
+        <f t="shared" ref="L24" si="38">G24/$B$43</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M24" s="69"/>
       <c r="N24" s="61"/>
       <c r="O24" s="61"/>
       <c r="P24" s="30" t="e">
-        <f t="shared" ref="P24" si="39">I24/(J24*$B$41)</f>
+        <f t="shared" ref="P24" si="39">I24/(J24*$B$44)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q24" s="45" t="e">
-        <f t="shared" ref="Q24" si="40">I24/((F24/$B$40*$B$41)*R24)</f>
+        <f t="shared" ref="Q24" si="40">I24/((F24/$B$43*$B$44)*R24)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R24" s="45" t="e">
-        <f t="shared" ref="R24" si="41">H24/(L24*$B$41)</f>
+        <f t="shared" ref="R24" si="41">H24/(L24*$B$44)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2023,7 +2023,7 @@
       <c r="N25" s="61"/>
       <c r="O25" s="61"/>
       <c r="P25" s="30" t="e">
-        <f t="shared" ref="P25:P26" si="42">I25/(J25*$B$41)</f>
+        <f t="shared" ref="P25:P26" si="42">I25/(J25*$B$44)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q25" s="45" t="e">
@@ -2031,7 +2031,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="R25" s="45" t="e">
-        <f t="shared" ref="R25:R26" si="43">H25/(L25*$B$41)</f>
+        <f t="shared" ref="R25:R26" si="43">H25/(L25*$B$44)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2084,30 +2084,30 @@
       <c r="H27" s="66"/>
       <c r="I27" s="67"/>
       <c r="J27" s="44" t="e">
-        <f t="shared" ref="J27" si="44">F27/$B$40</f>
+        <f t="shared" ref="J27:J29" si="44">F27/$B$43</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K27" s="43" t="e">
-        <f t="shared" ref="K27" si="45">J27*(M27/L27)</f>
+        <f t="shared" ref="K27:K29" si="45">J27*(M27/L27)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="L27" s="44" t="e">
-        <f t="shared" ref="L27" si="46">G27/$B$40</f>
+        <f t="shared" ref="L27:L29" si="46">G27/$B$43</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M27" s="69"/>
       <c r="N27" s="61"/>
       <c r="O27" s="61"/>
       <c r="P27" s="30" t="e">
-        <f t="shared" ref="P27" si="47">I27/(J27*$B$41)</f>
+        <f t="shared" ref="P27:P29" si="47">I27/(J27*$B$44)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q27" s="45" t="e">
-        <f t="shared" ref="Q27" si="48">I27/((F27/$B$40*$B$41)*R27)</f>
+        <f t="shared" ref="Q27:Q29" si="48">I27/((F27/$B$43*$B$44)*R27)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R27" s="45" t="e">
-        <f t="shared" ref="R27" si="49">H27/(L27*$B$41)</f>
+        <f t="shared" ref="R27:R29" si="49">H27/(L27*$B$44)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2122,30 +2122,30 @@
       <c r="H28" s="66"/>
       <c r="I28" s="67"/>
       <c r="J28" s="44" t="e">
-        <f t="shared" ref="J28:J29" si="50">F28/$B$40</f>
+        <f t="shared" si="44"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K28" s="43" t="e">
-        <f t="shared" ref="K28:K29" si="51">J28*(M28/L28)</f>
+        <f t="shared" si="45"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L28" s="44" t="e">
-        <f t="shared" ref="L28:L29" si="52">G28/$B$40</f>
+        <f t="shared" si="46"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M28" s="69"/>
       <c r="N28" s="61"/>
       <c r="O28" s="61"/>
       <c r="P28" s="30" t="e">
-        <f t="shared" ref="P28:P29" si="53">I28/(J28*$B$41)</f>
+        <f t="shared" si="47"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Q28" s="45" t="e">
-        <f t="shared" ref="Q28:Q29" si="54">I28/((F28/$B$40*$B$41)*R28)</f>
+        <f t="shared" si="48"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R28" s="45" t="e">
-        <f t="shared" ref="R28:R29" si="55">H28/(L28*$B$41)</f>
+        <f t="shared" si="49"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2160,30 +2160,30 @@
       <c r="H29" s="66"/>
       <c r="I29" s="67"/>
       <c r="J29" s="44" t="e">
-        <f t="shared" si="50"/>
+        <f t="shared" si="44"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K29" s="43" t="e">
-        <f t="shared" si="51"/>
+        <f t="shared" si="45"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L29" s="44" t="e">
-        <f t="shared" si="52"/>
+        <f t="shared" si="46"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M29" s="69"/>
       <c r="N29" s="61"/>
       <c r="O29" s="61"/>
       <c r="P29" s="30" t="e">
-        <f t="shared" si="53"/>
+        <f t="shared" si="47"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Q29" s="45" t="e">
-        <f t="shared" si="54"/>
+        <f t="shared" si="48"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R29" s="45" t="e">
-        <f t="shared" si="55"/>
+        <f t="shared" si="49"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2198,30 +2198,30 @@
       <c r="H30" s="66"/>
       <c r="I30" s="67"/>
       <c r="J30" s="44" t="e">
-        <f t="shared" ref="J30" si="56">F30/$B$40</f>
+        <f t="shared" ref="J30:J32" si="50">F30/$B$43</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K30" s="43" t="e">
-        <f t="shared" ref="K30" si="57">J30*(M30/L30)</f>
+        <f t="shared" ref="K30:K32" si="51">J30*(M30/L30)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="L30" s="44" t="e">
-        <f t="shared" ref="L30" si="58">G30/$B$40</f>
+        <f t="shared" ref="L30:L32" si="52">G30/$B$43</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M30" s="69"/>
       <c r="N30" s="61"/>
       <c r="O30" s="61"/>
       <c r="P30" s="30" t="e">
-        <f t="shared" ref="P30" si="59">I30/(J30*$B$41)</f>
+        <f t="shared" ref="P30:P32" si="53">I30/(J30*$B$44)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q30" s="45" t="e">
-        <f t="shared" ref="Q30" si="60">I30/((F30/$B$40*$B$41)*R30)</f>
+        <f t="shared" ref="Q30:Q32" si="54">I30/((F30/$B$43*$B$44)*R30)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R30" s="45" t="e">
-        <f t="shared" ref="R30" si="61">H30/(L30*$B$41)</f>
+        <f t="shared" ref="R30:R32" si="55">H30/(L30*$B$44)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2236,30 +2236,30 @@
       <c r="H31" s="66"/>
       <c r="I31" s="67"/>
       <c r="J31" s="44" t="e">
-        <f t="shared" ref="J31" si="62">F31/$B$40</f>
+        <f t="shared" si="50"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K31" s="43" t="e">
-        <f t="shared" ref="K31" si="63">J31*(M31/L31)</f>
+        <f t="shared" si="51"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L31" s="44" t="e">
-        <f t="shared" ref="L31" si="64">G31/$B$40</f>
+        <f t="shared" si="52"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M31" s="69"/>
       <c r="N31" s="61"/>
       <c r="O31" s="61"/>
       <c r="P31" s="30" t="e">
-        <f t="shared" ref="P31" si="65">I31/(J31*$B$41)</f>
+        <f t="shared" si="53"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Q31" s="45" t="e">
-        <f t="shared" ref="Q31" si="66">I31/((F31/$B$40*$B$41)*R31)</f>
+        <f t="shared" si="54"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R31" s="45" t="e">
-        <f t="shared" ref="R31" si="67">H31/(L31*$B$41)</f>
+        <f t="shared" si="55"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2274,30 +2274,30 @@
       <c r="H32" s="66"/>
       <c r="I32" s="67"/>
       <c r="J32" s="44" t="e">
-        <f t="shared" ref="J32" si="68">F32/$B$40</f>
+        <f t="shared" si="50"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K32" s="43" t="e">
-        <f t="shared" ref="K32" si="69">J32*(M32/L32)</f>
+        <f t="shared" si="51"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L32" s="44" t="e">
-        <f t="shared" ref="L32" si="70">G32/$B$40</f>
+        <f t="shared" si="52"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M32" s="69"/>
       <c r="N32" s="61"/>
       <c r="O32" s="61"/>
       <c r="P32" s="30" t="e">
-        <f t="shared" ref="P32" si="71">I32/(J32*$B$41)</f>
+        <f t="shared" si="53"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Q32" s="45" t="e">
-        <f t="shared" ref="Q32" si="72">I32/((F32/$B$40*$B$41)*R32)</f>
+        <f t="shared" si="54"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R32" s="45" t="e">
-        <f t="shared" ref="R32" si="73">H32/(L32*$B$41)</f>
+        <f t="shared" si="55"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2312,34 +2312,34 @@
       <c r="H33" s="66"/>
       <c r="I33" s="67"/>
       <c r="J33" s="44" t="e">
-        <f t="shared" ref="J33" si="74">F33/$B$40</f>
+        <f t="shared" ref="J33" si="56">F33/$B$43</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K33" s="43" t="e">
-        <f t="shared" ref="K33" si="75">J33*(M33/L33)</f>
+        <f t="shared" ref="K33" si="57">J33*(M33/L33)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="L33" s="44" t="e">
-        <f t="shared" ref="L33" si="76">G33/$B$40</f>
+        <f t="shared" ref="L33" si="58">G33/$B$43</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M33" s="69"/>
       <c r="N33" s="61"/>
       <c r="O33" s="61"/>
       <c r="P33" s="30" t="e">
-        <f t="shared" ref="P33" si="77">I33/(J33*$B$41)</f>
+        <f t="shared" ref="P33" si="59">I33/(J33*$B$44)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q33" s="45" t="e">
-        <f t="shared" ref="Q33" si="78">I33/((F33/$B$40*$B$41)*R33)</f>
+        <f t="shared" ref="Q33" si="60">I33/((F33/$B$43*$B$44)*R33)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R33" s="45" t="e">
-        <f t="shared" ref="R33" si="79">H33/(L33*$B$41)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="34" spans="1:19" ht="12.45" customHeight="1" thickBot="1">
+        <f t="shared" ref="R33" si="61">H33/(L33*$B$44)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" ht="12.45" customHeight="1">
       <c r="A34" s="40"/>
       <c r="B34" s="41"/>
       <c r="C34" s="42"/>
@@ -2350,114 +2350,228 @@
       <c r="H34" s="66"/>
       <c r="I34" s="67"/>
       <c r="J34" s="44" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="J34" si="62">F34/$B$43</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K34" s="43" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="K34" si="63">J34*(M34/L34)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="L34" s="44" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="L34" si="64">G34/$B$43</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M34" s="69"/>
       <c r="N34" s="61"/>
       <c r="O34" s="61"/>
       <c r="P34" s="30" t="e">
+        <f t="shared" ref="P34" si="65">I34/(J34*$B$44)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q34" s="45" t="e">
+        <f t="shared" ref="Q34" si="66">I34/((F34/$B$43*$B$44)*R34)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R34" s="45" t="e">
+        <f t="shared" ref="R34" si="67">H34/(L34*$B$44)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" ht="12.45" customHeight="1">
+      <c r="A35" s="40"/>
+      <c r="B35" s="41"/>
+      <c r="C35" s="42"/>
+      <c r="D35" s="61"/>
+      <c r="E35" s="63"/>
+      <c r="F35" s="61"/>
+      <c r="G35" s="63"/>
+      <c r="H35" s="66"/>
+      <c r="I35" s="67"/>
+      <c r="J35" s="44" t="e">
+        <f t="shared" ref="J35" si="68">F35/$B$43</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K35" s="43" t="e">
+        <f t="shared" ref="K35" si="69">J35*(M35/L35)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L35" s="44" t="e">
+        <f t="shared" ref="L35" si="70">G35/$B$43</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M35" s="69"/>
+      <c r="N35" s="61"/>
+      <c r="O35" s="61"/>
+      <c r="P35" s="30" t="e">
+        <f t="shared" ref="P35" si="71">I35/(J35*$B$44)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q35" s="45" t="e">
+        <f t="shared" ref="Q35" si="72">I35/((F35/$B$43*$B$44)*R35)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R35" s="45" t="e">
+        <f t="shared" ref="R35" si="73">H35/(L35*$B$44)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" ht="12.45" customHeight="1">
+      <c r="A36" s="40"/>
+      <c r="B36" s="41"/>
+      <c r="C36" s="42"/>
+      <c r="D36" s="61"/>
+      <c r="E36" s="63"/>
+      <c r="F36" s="61"/>
+      <c r="G36" s="63"/>
+      <c r="H36" s="66"/>
+      <c r="I36" s="67"/>
+      <c r="J36" s="44" t="e">
+        <f t="shared" ref="J36" si="74">F36/$B$43</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K36" s="43" t="e">
+        <f t="shared" ref="K36" si="75">J36*(M36/L36)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L36" s="44" t="e">
+        <f t="shared" ref="L36" si="76">G36/$B$43</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M36" s="69"/>
+      <c r="N36" s="61"/>
+      <c r="O36" s="61"/>
+      <c r="P36" s="30" t="e">
+        <f t="shared" ref="P36" si="77">I36/(J36*$B$44)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q36" s="45" t="e">
+        <f t="shared" ref="Q36" si="78">I36/((F36/$B$43*$B$44)*R36)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R36" s="45" t="e">
+        <f t="shared" ref="R36" si="79">H36/(L36*$B$44)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" ht="12.45" customHeight="1" thickBot="1">
+      <c r="A37" s="40"/>
+      <c r="B37" s="41"/>
+      <c r="C37" s="42"/>
+      <c r="D37" s="61"/>
+      <c r="E37" s="63"/>
+      <c r="F37" s="61"/>
+      <c r="G37" s="63"/>
+      <c r="H37" s="66"/>
+      <c r="I37" s="67"/>
+      <c r="J37" s="44" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K37" s="43" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L37" s="44" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M37" s="69"/>
+      <c r="N37" s="61"/>
+      <c r="O37" s="61"/>
+      <c r="P37" s="30" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="Q34" s="45" t="e">
+      <c r="Q37" s="45" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="R34" s="45" t="e">
+      <c r="R37" s="45" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="35" spans="1:19" ht="13.05" customHeight="1" thickBot="1">
-      <c r="A35" s="46"/>
-      <c r="B35" s="47" t="s">
+    <row r="38" spans="1:19" ht="13.05" customHeight="1" thickBot="1">
+      <c r="A38" s="46"/>
+      <c r="B38" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="C35" s="48"/>
-      <c r="D35" s="49">
-        <f t="shared" ref="D35:N35" si="80">SUM(D10:D34)</f>
+      <c r="C38" s="48"/>
+      <c r="D38" s="49">
+        <f t="shared" ref="D38:N38" si="80">SUM(D10:D37)</f>
         <v>0</v>
       </c>
-      <c r="E35" s="49">
+      <c r="E38" s="49">
         <f t="shared" si="80"/>
         <v>0</v>
       </c>
-      <c r="F35" s="49">
+      <c r="F38" s="49">
         <f t="shared" si="80"/>
         <v>0</v>
       </c>
-      <c r="G35" s="49">
+      <c r="G38" s="49">
         <f t="shared" si="80"/>
         <v>0</v>
       </c>
-      <c r="H35" s="49">
+      <c r="H38" s="49">
         <f t="shared" si="80"/>
         <v>0</v>
       </c>
-      <c r="I35" s="50">
+      <c r="I38" s="50">
         <f t="shared" si="80"/>
         <v>0</v>
       </c>
-      <c r="J35" s="51" t="e">
+      <c r="J38" s="51" t="e">
         <f t="shared" si="80"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K35" s="52" t="e">
+      <c r="K38" s="52" t="e">
         <f t="shared" si="80"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="L35" s="52" t="e">
+      <c r="L38" s="52" t="e">
         <f t="shared" si="80"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="M35" s="53">
+      <c r="M38" s="53">
         <f t="shared" si="80"/>
         <v>0</v>
       </c>
-      <c r="N35" s="54">
+      <c r="N38" s="54">
         <f t="shared" si="80"/>
         <v>0</v>
       </c>
-      <c r="O35" s="54"/>
-      <c r="P35" s="57" t="e">
+      <c r="O38" s="54"/>
+      <c r="P38" s="57" t="e">
         <f t="shared" si="7"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="Q35" s="57" t="e">
+      <c r="Q38" s="57" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="R35" s="57" t="e">
+      <c r="R38" s="57" t="e">
         <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="S35" s="58"/>
-    </row>
-    <row r="37" spans="1:19" ht="12.45" customHeight="1">
-      <c r="Q37" s="59"/>
+      <c r="S38" s="58"/>
     </row>
     <row r="40" spans="1:19" ht="12.45" customHeight="1">
-      <c r="A40" s="56" t="s">
+      <c r="Q40" s="59"/>
+    </row>
+    <row r="43" spans="1:19" ht="12.45" customHeight="1">
+      <c r="A43" s="56" t="s">
         <v>25</v>
       </c>
-      <c r="B40" s="56"/>
-      <c r="C40" s="55"/>
-    </row>
-    <row r="41" spans="1:19" ht="12.45" customHeight="1">
-      <c r="A41" s="56" t="s">
+      <c r="B43" s="56"/>
+      <c r="C43" s="55"/>
+    </row>
+    <row r="44" spans="1:19" ht="12.45" customHeight="1">
+      <c r="A44" s="56" t="s">
         <v>26</v>
       </c>
-      <c r="B41" s="56"/>
-      <c r="C41" s="55"/>
+      <c r="B44" s="56"/>
+      <c r="C44" s="55"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
@@ -2478,8 +2592,8 @@
 &amp;I© 2017 SunEdison&amp;I &amp;C&amp;R&amp;"Arial"&amp;8 Page 1 of 2 </oddFooter>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="D35:H35 J10:L13 P10:R13 P35:R35 J35:N35" unlockedFormula="1"/>
-    <ignoredError sqref="I35" formula="1" unlockedFormula="1"/>
+    <ignoredError sqref="D38:H38 J10:L13 P10:R13 P38:R38 J38:N38" unlockedFormula="1"/>
+    <ignoredError sqref="I38" formula="1" unlockedFormula="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
change xls template for new site
</commit_message>
<xml_diff>
--- a/job/templates/DailyReport-v3.xlsx
+++ b/job/templates/DailyReport-v3.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6945"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6948"/>
   </bookViews>
   <sheets>
     <sheet name="DailyProductionReport" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">DailyProductionReport!$1:$1</definedName>
   </definedNames>
-  <calcPr calcId="144525" concurrentCalc="0"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -124,14 +124,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="[$-10409]#,##0;\(#,##0\)"/>
     <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
     <numFmt numFmtId="166" formatCode="0.0%"/>
     <numFmt numFmtId="167" formatCode="[$-10409]#,##0.0;\(#,##0.0\)"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -625,7 +625,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -844,7 +844,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="167" fontId="4" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
       <protection locked="0"/>
@@ -1014,7 +1013,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1049,7 +1047,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1225,51 +1222,51 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:S51"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.4" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.45" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="17.140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="25.28515625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="21.28515625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="17.109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="25.33203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="21.33203125" style="2" customWidth="1"/>
     <col min="4" max="9" width="13" style="2" customWidth="1"/>
-    <col min="10" max="12" width="12.85546875" style="2" customWidth="1"/>
-    <col min="13" max="13" width="19.28515625" style="2" customWidth="1"/>
-    <col min="14" max="14" width="21.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21.7109375" style="2" customWidth="1"/>
-    <col min="16" max="18" width="19.28515625" style="2" customWidth="1"/>
+    <col min="10" max="12" width="12.88671875" style="2" customWidth="1"/>
+    <col min="13" max="13" width="19.33203125" style="2" customWidth="1"/>
+    <col min="14" max="14" width="21.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.6640625" style="2" customWidth="1"/>
+    <col min="16" max="18" width="19.33203125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="72" t="s">
+    <row r="1" spans="1:18" ht="28.5" customHeight="1">
+      <c r="A1" s="71" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="72"/>
-      <c r="C1" s="72"/>
-      <c r="D1" s="72"/>
-      <c r="E1" s="72"/>
-      <c r="F1" s="72"/>
-      <c r="G1" s="72"/>
-      <c r="H1" s="72"/>
-      <c r="I1" s="72"/>
-      <c r="J1" s="72"/>
-      <c r="K1" s="72"/>
-      <c r="L1" s="72"/>
-      <c r="M1" s="72"/>
-      <c r="N1" s="72"/>
-      <c r="O1" s="72"/>
-      <c r="P1" s="72"/>
-      <c r="Q1" s="72"/>
-      <c r="R1" s="72"/>
-    </row>
-    <row r="2" spans="1:18" ht="1.1499999999999999" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="3" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="71"/>
+      <c r="C1" s="71"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="71"/>
+      <c r="G1" s="71"/>
+      <c r="H1" s="71"/>
+      <c r="I1" s="71"/>
+      <c r="J1" s="71"/>
+      <c r="K1" s="71"/>
+      <c r="L1" s="71"/>
+      <c r="M1" s="71"/>
+      <c r="N1" s="71"/>
+      <c r="O1" s="71"/>
+      <c r="P1" s="71"/>
+      <c r="Q1" s="71"/>
+      <c r="R1" s="71"/>
+    </row>
+    <row r="2" spans="1:18" ht="1.2" customHeight="1"/>
+    <row r="3" spans="1:18" ht="15.75" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -1277,55 +1274,55 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" ht="15.75" customHeight="1">
       <c r="B4" s="4"/>
     </row>
-    <row r="5" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="72" t="s">
+    <row r="5" spans="1:18" ht="18" customHeight="1">
+      <c r="A5" s="71" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="72"/>
-      <c r="C5" s="72"/>
-      <c r="D5" s="72"/>
-      <c r="E5" s="72"/>
+      <c r="B5" s="71"/>
+      <c r="C5" s="71"/>
+      <c r="D5" s="71"/>
+      <c r="E5" s="71"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="28"/>
     </row>
-    <row r="6" spans="1:18" ht="2.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:18" s="9" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" ht="2.7" customHeight="1" thickBot="1"/>
+    <row r="7" spans="1:18" s="9" customFormat="1" ht="22.5" customHeight="1" thickBot="1">
       <c r="A7" s="10"/>
       <c r="B7" s="13"/>
       <c r="C7" s="18"/>
       <c r="D7" s="14"/>
       <c r="E7" s="15"/>
-      <c r="F7" s="73" t="s">
+      <c r="F7" s="72" t="s">
         <v>29</v>
       </c>
-      <c r="G7" s="74"/>
-      <c r="H7" s="73" t="s">
+      <c r="G7" s="73"/>
+      <c r="H7" s="72" t="s">
         <v>4</v>
       </c>
-      <c r="I7" s="74"/>
-      <c r="J7" s="73" t="s">
+      <c r="I7" s="73"/>
+      <c r="J7" s="72" t="s">
         <v>30</v>
       </c>
-      <c r="K7" s="75"/>
-      <c r="L7" s="74"/>
-      <c r="M7" s="76" t="s">
+      <c r="K7" s="74"/>
+      <c r="L7" s="73"/>
+      <c r="M7" s="75" t="s">
         <v>28</v>
       </c>
-      <c r="N7" s="77"/>
-      <c r="O7" s="78"/>
-      <c r="P7" s="76" t="s">
+      <c r="N7" s="76"/>
+      <c r="O7" s="77"/>
+      <c r="P7" s="75" t="s">
         <v>33</v>
       </c>
-      <c r="Q7" s="77"/>
-      <c r="R7" s="77"/>
-    </row>
-    <row r="8" spans="1:18" s="3" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q7" s="76"/>
+      <c r="R7" s="76"/>
+    </row>
+    <row r="8" spans="1:18" s="3" customFormat="1" ht="12.45" customHeight="1">
       <c r="A8" s="11" t="s">
         <v>5</v>
       </c>
@@ -1335,10 +1332,10 @@
       <c r="C8" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="70" t="s">
+      <c r="D8" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="71"/>
+      <c r="E8" s="70"/>
       <c r="F8" s="21" t="s">
         <v>9</v>
       </c>
@@ -1379,7 +1376,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:18" s="17" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" s="17" customFormat="1" ht="12.45" customHeight="1">
       <c r="A9" s="16"/>
       <c r="B9" s="5"/>
       <c r="C9" s="8"/>
@@ -1427,31 +1424,31 @@
       </c>
       <c r="R9" s="32"/>
     </row>
-    <row r="10" spans="1:18" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" ht="12.45" customHeight="1">
       <c r="A10" s="12"/>
       <c r="B10" s="6"/>
       <c r="C10" s="20"/>
-      <c r="D10" s="60"/>
-      <c r="E10" s="62"/>
-      <c r="F10" s="60"/>
-      <c r="G10" s="62"/>
-      <c r="H10" s="64"/>
-      <c r="I10" s="65"/>
+      <c r="D10" s="59"/>
+      <c r="E10" s="61"/>
+      <c r="F10" s="59"/>
+      <c r="G10" s="61"/>
+      <c r="H10" s="63"/>
+      <c r="I10" s="64"/>
       <c r="J10" s="39" t="e">
         <f t="shared" ref="J10:J15" si="0">F10/$B$50</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K10" s="38" t="e">
-        <f t="shared" ref="K10:K44" si="1">J10*(M10/L10)</f>
+        <f t="shared" ref="K10:K46" si="1">J10*(M10/L10)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="L10" s="39" t="e">
         <f t="shared" ref="L10:L15" si="2">G10/$B$50</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M10" s="68"/>
-      <c r="N10" s="60"/>
-      <c r="O10" s="60"/>
+      <c r="M10" s="67"/>
+      <c r="N10" s="59"/>
+      <c r="O10" s="59"/>
       <c r="P10" s="30" t="e">
         <f>I10/(J10*$B$51)</f>
         <v>#DIV/0!</v>
@@ -1465,16 +1462,16 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" ht="12.45" customHeight="1">
       <c r="A11" s="12"/>
       <c r="B11" s="6"/>
       <c r="C11" s="20"/>
-      <c r="D11" s="60"/>
-      <c r="E11" s="62"/>
-      <c r="F11" s="60"/>
-      <c r="G11" s="62"/>
-      <c r="H11" s="64"/>
-      <c r="I11" s="65"/>
+      <c r="D11" s="59"/>
+      <c r="E11" s="61"/>
+      <c r="F11" s="59"/>
+      <c r="G11" s="61"/>
+      <c r="H11" s="63"/>
+      <c r="I11" s="64"/>
       <c r="J11" s="39" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -1487,9 +1484,9 @@
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="M11" s="68"/>
-      <c r="N11" s="60"/>
-      <c r="O11" s="60"/>
+      <c r="M11" s="67"/>
+      <c r="N11" s="59"/>
+      <c r="O11" s="59"/>
       <c r="P11" s="30" t="e">
         <f>I11/(J11*$B$51)</f>
         <v>#DIV/0!</v>
@@ -1503,16 +1500,16 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" ht="12.45" customHeight="1">
       <c r="A12" s="12"/>
       <c r="B12" s="6"/>
       <c r="C12" s="20"/>
-      <c r="D12" s="60"/>
-      <c r="E12" s="62"/>
-      <c r="F12" s="60"/>
-      <c r="G12" s="62"/>
-      <c r="H12" s="64"/>
-      <c r="I12" s="65"/>
+      <c r="D12" s="59"/>
+      <c r="E12" s="61"/>
+      <c r="F12" s="59"/>
+      <c r="G12" s="61"/>
+      <c r="H12" s="63"/>
+      <c r="I12" s="64"/>
       <c r="J12" s="39" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -1525,9 +1522,9 @@
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="M12" s="68"/>
-      <c r="N12" s="60"/>
-      <c r="O12" s="60"/>
+      <c r="M12" s="67"/>
+      <c r="N12" s="59"/>
+      <c r="O12" s="59"/>
       <c r="P12" s="30" t="e">
         <f>I12/(J12*$B$51)</f>
         <v>#DIV/0!</v>
@@ -1541,16 +1538,16 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" ht="12.45" customHeight="1">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="20"/>
-      <c r="D13" s="60"/>
-      <c r="E13" s="62"/>
-      <c r="F13" s="60"/>
-      <c r="G13" s="62"/>
-      <c r="H13" s="64"/>
-      <c r="I13" s="65"/>
+      <c r="D13" s="59"/>
+      <c r="E13" s="61"/>
+      <c r="F13" s="59"/>
+      <c r="G13" s="61"/>
+      <c r="H13" s="63"/>
+      <c r="I13" s="64"/>
       <c r="J13" s="39" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -1563,9 +1560,9 @@
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="M13" s="68"/>
-      <c r="N13" s="60"/>
-      <c r="O13" s="60"/>
+      <c r="M13" s="67"/>
+      <c r="N13" s="59"/>
+      <c r="O13" s="59"/>
       <c r="P13" s="30" t="e">
         <f>I13/(J13*$B$51)</f>
         <v>#DIV/0!</v>
@@ -1579,16 +1576,16 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" ht="12.45" customHeight="1">
       <c r="A14" s="40"/>
       <c r="B14" s="41"/>
       <c r="C14" s="42"/>
-      <c r="D14" s="61"/>
-      <c r="E14" s="63"/>
-      <c r="F14" s="61"/>
-      <c r="G14" s="63"/>
-      <c r="H14" s="66"/>
-      <c r="I14" s="67"/>
+      <c r="D14" s="60"/>
+      <c r="E14" s="62"/>
+      <c r="F14" s="60"/>
+      <c r="G14" s="62"/>
+      <c r="H14" s="65"/>
+      <c r="I14" s="66"/>
       <c r="J14" s="44" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -1601,9 +1598,9 @@
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="M14" s="69"/>
-      <c r="N14" s="61"/>
-      <c r="O14" s="61"/>
+      <c r="M14" s="68"/>
+      <c r="N14" s="60"/>
+      <c r="O14" s="60"/>
       <c r="P14" s="30" t="e">
         <f t="shared" ref="P14" si="3">I14/(J14*$B$51)</f>
         <v>#DIV/0!</v>
@@ -1617,16 +1614,16 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" ht="12.45" customHeight="1">
       <c r="A15" s="40"/>
       <c r="B15" s="41"/>
       <c r="C15" s="42"/>
-      <c r="D15" s="61"/>
-      <c r="E15" s="63"/>
-      <c r="F15" s="61"/>
-      <c r="G15" s="63"/>
-      <c r="H15" s="66"/>
-      <c r="I15" s="67"/>
+      <c r="D15" s="60"/>
+      <c r="E15" s="62"/>
+      <c r="F15" s="60"/>
+      <c r="G15" s="62"/>
+      <c r="H15" s="65"/>
+      <c r="I15" s="66"/>
       <c r="J15" s="44" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -1639,9 +1636,9 @@
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="M15" s="69"/>
-      <c r="N15" s="61"/>
-      <c r="O15" s="61"/>
+      <c r="M15" s="68"/>
+      <c r="N15" s="60"/>
+      <c r="O15" s="60"/>
       <c r="P15" s="30" t="e">
         <f>I15/(J15*$B$51)</f>
         <v>#DIV/0!</v>
@@ -1655,16 +1652,16 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18" ht="12.45" customHeight="1">
       <c r="A16" s="40"/>
       <c r="B16" s="41"/>
       <c r="C16" s="42"/>
-      <c r="D16" s="61"/>
-      <c r="E16" s="63"/>
-      <c r="F16" s="61"/>
-      <c r="G16" s="63"/>
-      <c r="H16" s="66"/>
-      <c r="I16" s="67"/>
+      <c r="D16" s="60"/>
+      <c r="E16" s="62"/>
+      <c r="F16" s="60"/>
+      <c r="G16" s="62"/>
+      <c r="H16" s="65"/>
+      <c r="I16" s="66"/>
       <c r="J16" s="44" t="e">
         <f t="shared" ref="J16" si="6">F16/$B$50</f>
         <v>#DIV/0!</v>
@@ -1677,9 +1674,9 @@
         <f t="shared" ref="L16" si="7">G16/$B$50</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M16" s="69"/>
-      <c r="N16" s="61"/>
-      <c r="O16" s="61"/>
+      <c r="M16" s="68"/>
+      <c r="N16" s="60"/>
+      <c r="O16" s="60"/>
       <c r="P16" s="30" t="e">
         <f>I16/(J16*$B$51)</f>
         <v>#DIV/0!</v>
@@ -1693,16 +1690,16 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="17" spans="1:18" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:18" ht="12.45" customHeight="1">
       <c r="A17" s="40"/>
       <c r="B17" s="41"/>
       <c r="C17" s="42"/>
-      <c r="D17" s="61"/>
-      <c r="E17" s="63"/>
-      <c r="F17" s="61"/>
-      <c r="G17" s="63"/>
-      <c r="H17" s="66"/>
-      <c r="I17" s="67"/>
+      <c r="D17" s="60"/>
+      <c r="E17" s="62"/>
+      <c r="F17" s="60"/>
+      <c r="G17" s="62"/>
+      <c r="H17" s="65"/>
+      <c r="I17" s="66"/>
       <c r="J17" s="44" t="e">
         <f t="shared" ref="J17" si="9">F17/$B$50</f>
         <v>#DIV/0!</v>
@@ -1715,9 +1712,9 @@
         <f t="shared" ref="L17" si="11">G17/$B$50</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M17" s="69"/>
-      <c r="N17" s="61"/>
-      <c r="O17" s="61"/>
+      <c r="M17" s="68"/>
+      <c r="N17" s="60"/>
+      <c r="O17" s="60"/>
       <c r="P17" s="30" t="e">
         <f>I17/(J17*$B$51)</f>
         <v>#DIV/0!</v>
@@ -1731,16 +1728,16 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="18" spans="1:18" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:18" ht="12.45" customHeight="1">
       <c r="A18" s="40"/>
       <c r="B18" s="41"/>
       <c r="C18" s="42"/>
-      <c r="D18" s="61"/>
-      <c r="E18" s="63"/>
-      <c r="F18" s="61"/>
-      <c r="G18" s="63"/>
-      <c r="H18" s="66"/>
-      <c r="I18" s="67"/>
+      <c r="D18" s="60"/>
+      <c r="E18" s="62"/>
+      <c r="F18" s="60"/>
+      <c r="G18" s="62"/>
+      <c r="H18" s="65"/>
+      <c r="I18" s="66"/>
       <c r="J18" s="44" t="e">
         <f t="shared" ref="J18" si="13">F18/$B$50</f>
         <v>#DIV/0!</v>
@@ -1753,9 +1750,9 @@
         <f t="shared" ref="L18" si="15">G18/$B$50</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M18" s="69"/>
-      <c r="N18" s="61"/>
-      <c r="O18" s="61"/>
+      <c r="M18" s="68"/>
+      <c r="N18" s="60"/>
+      <c r="O18" s="60"/>
       <c r="P18" s="30" t="e">
         <f>I18/(J18*$B$51)</f>
         <v>#DIV/0!</v>
@@ -1769,16 +1766,16 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="19" spans="1:18" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:18" ht="12.45" customHeight="1">
       <c r="A19" s="40"/>
       <c r="B19" s="41"/>
       <c r="C19" s="42"/>
-      <c r="D19" s="61"/>
-      <c r="E19" s="63"/>
-      <c r="F19" s="61"/>
-      <c r="G19" s="63"/>
-      <c r="H19" s="66"/>
-      <c r="I19" s="67"/>
+      <c r="D19" s="60"/>
+      <c r="E19" s="62"/>
+      <c r="F19" s="60"/>
+      <c r="G19" s="62"/>
+      <c r="H19" s="65"/>
+      <c r="I19" s="66"/>
       <c r="J19" s="44" t="e">
         <f>F19/$B$50</f>
         <v>#DIV/0!</v>
@@ -1791,9 +1788,9 @@
         <f>G19/$B$50</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M19" s="69"/>
-      <c r="N19" s="61"/>
-      <c r="O19" s="61"/>
+      <c r="M19" s="68"/>
+      <c r="N19" s="60"/>
+      <c r="O19" s="60"/>
       <c r="P19" s="30" t="e">
         <f>I19/(J19*$B$51)</f>
         <v>#DIV/0!</v>
@@ -1807,16 +1804,16 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="20" spans="1:18" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:18" ht="12.45" customHeight="1">
       <c r="A20" s="40"/>
       <c r="B20" s="41"/>
       <c r="C20" s="42"/>
-      <c r="D20" s="61"/>
-      <c r="E20" s="63"/>
-      <c r="F20" s="61"/>
-      <c r="G20" s="63"/>
-      <c r="H20" s="66"/>
-      <c r="I20" s="67"/>
+      <c r="D20" s="60"/>
+      <c r="E20" s="62"/>
+      <c r="F20" s="60"/>
+      <c r="G20" s="62"/>
+      <c r="H20" s="65"/>
+      <c r="I20" s="66"/>
       <c r="J20" s="44" t="e">
         <f t="shared" ref="J20" si="18">F20/$B$50</f>
         <v>#DIV/0!</v>
@@ -1829,9 +1826,9 @@
         <f t="shared" ref="L20" si="20">G20/$B$50</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M20" s="69"/>
-      <c r="N20" s="61"/>
-      <c r="O20" s="61"/>
+      <c r="M20" s="68"/>
+      <c r="N20" s="60"/>
+      <c r="O20" s="60"/>
       <c r="P20" s="30" t="e">
         <f t="shared" ref="P20" si="21">I20/(J20*$B$51)</f>
         <v>#DIV/0!</v>
@@ -1845,16 +1842,16 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="21" spans="1:18" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:18" ht="12.45" customHeight="1">
       <c r="A21" s="40"/>
       <c r="B21" s="41"/>
       <c r="C21" s="42"/>
-      <c r="D21" s="61"/>
-      <c r="E21" s="63"/>
-      <c r="F21" s="61"/>
-      <c r="G21" s="63"/>
-      <c r="H21" s="66"/>
-      <c r="I21" s="67"/>
+      <c r="D21" s="60"/>
+      <c r="E21" s="62"/>
+      <c r="F21" s="60"/>
+      <c r="G21" s="62"/>
+      <c r="H21" s="65"/>
+      <c r="I21" s="66"/>
       <c r="J21" s="44" t="e">
         <f>F21/$B$50</f>
         <v>#DIV/0!</v>
@@ -1867,9 +1864,9 @@
         <f>G21/$B$50</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M21" s="69"/>
-      <c r="N21" s="61"/>
-      <c r="O21" s="61"/>
+      <c r="M21" s="68"/>
+      <c r="N21" s="60"/>
+      <c r="O21" s="60"/>
       <c r="P21" s="30" t="e">
         <f>I21/(J21*$B$51)</f>
         <v>#DIV/0!</v>
@@ -1883,16 +1880,16 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="22" spans="1:18" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:18" ht="12.45" customHeight="1">
       <c r="A22" s="40"/>
       <c r="B22" s="41"/>
       <c r="C22" s="42"/>
-      <c r="D22" s="61"/>
-      <c r="E22" s="63"/>
-      <c r="F22" s="61"/>
-      <c r="G22" s="63"/>
-      <c r="H22" s="66"/>
-      <c r="I22" s="67"/>
+      <c r="D22" s="60"/>
+      <c r="E22" s="62"/>
+      <c r="F22" s="60"/>
+      <c r="G22" s="62"/>
+      <c r="H22" s="65"/>
+      <c r="I22" s="66"/>
       <c r="J22" s="44" t="e">
         <f>F22/$B$50</f>
         <v>#DIV/0!</v>
@@ -1905,9 +1902,9 @@
         <f>G22/$B$50</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M22" s="69"/>
-      <c r="N22" s="61"/>
-      <c r="O22" s="61"/>
+      <c r="M22" s="68"/>
+      <c r="N22" s="60"/>
+      <c r="O22" s="60"/>
       <c r="P22" s="30" t="e">
         <f>I22/(J22*$B$51)</f>
         <v>#DIV/0!</v>
@@ -1921,16 +1918,16 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="23" spans="1:18" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:18" ht="12.45" customHeight="1">
       <c r="A23" s="40"/>
       <c r="B23" s="41"/>
       <c r="C23" s="42"/>
-      <c r="D23" s="61"/>
-      <c r="E23" s="63"/>
-      <c r="F23" s="61"/>
-      <c r="G23" s="63"/>
-      <c r="H23" s="66"/>
-      <c r="I23" s="67"/>
+      <c r="D23" s="60"/>
+      <c r="E23" s="62"/>
+      <c r="F23" s="60"/>
+      <c r="G23" s="62"/>
+      <c r="H23" s="65"/>
+      <c r="I23" s="66"/>
       <c r="J23" s="44" t="e">
         <f>F23/$B$50</f>
         <v>#DIV/0!</v>
@@ -1943,9 +1940,9 @@
         <f>G23/$B$50</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M23" s="69"/>
-      <c r="N23" s="61"/>
-      <c r="O23" s="61"/>
+      <c r="M23" s="68"/>
+      <c r="N23" s="60"/>
+      <c r="O23" s="60"/>
       <c r="P23" s="30" t="e">
         <f>I23/(J23*$B$51)</f>
         <v>#DIV/0!</v>
@@ -1959,16 +1956,16 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="24" spans="1:18" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:18" ht="12.45" customHeight="1">
       <c r="A24" s="40"/>
       <c r="B24" s="41"/>
       <c r="C24" s="42"/>
-      <c r="D24" s="61"/>
-      <c r="E24" s="63"/>
-      <c r="F24" s="61"/>
-      <c r="G24" s="63"/>
-      <c r="H24" s="66"/>
-      <c r="I24" s="67"/>
+      <c r="D24" s="60"/>
+      <c r="E24" s="62"/>
+      <c r="F24" s="60"/>
+      <c r="G24" s="62"/>
+      <c r="H24" s="65"/>
+      <c r="I24" s="66"/>
       <c r="J24" s="44" t="e">
         <f t="shared" ref="J24" si="25">F24/$B$50</f>
         <v>#DIV/0!</v>
@@ -1981,9 +1978,9 @@
         <f t="shared" ref="L24" si="27">G24/$B$50</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M24" s="69"/>
-      <c r="N24" s="61"/>
-      <c r="O24" s="61"/>
+      <c r="M24" s="68"/>
+      <c r="N24" s="60"/>
+      <c r="O24" s="60"/>
       <c r="P24" s="30" t="e">
         <f t="shared" ref="P24" si="28">I24/(J24*$B$51)</f>
         <v>#DIV/0!</v>
@@ -1997,16 +1994,16 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="25" spans="1:18" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:18" ht="12.45" customHeight="1">
       <c r="A25" s="40"/>
       <c r="B25" s="41"/>
       <c r="C25" s="42"/>
-      <c r="D25" s="61"/>
-      <c r="E25" s="63"/>
-      <c r="F25" s="61"/>
-      <c r="G25" s="63"/>
-      <c r="H25" s="66"/>
-      <c r="I25" s="67"/>
+      <c r="D25" s="60"/>
+      <c r="E25" s="62"/>
+      <c r="F25" s="60"/>
+      <c r="G25" s="62"/>
+      <c r="H25" s="65"/>
+      <c r="I25" s="66"/>
       <c r="J25" s="44" t="e">
         <f t="shared" ref="J25:J32" si="31">F25/$B$50</f>
         <v>#DIV/0!</v>
@@ -2019,32 +2016,32 @@
         <f t="shared" ref="L25:L32" si="32">G25/$B$50</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M25" s="69"/>
-      <c r="N25" s="61"/>
-      <c r="O25" s="61"/>
+      <c r="M25" s="68"/>
+      <c r="N25" s="60"/>
+      <c r="O25" s="60"/>
       <c r="P25" s="30" t="e">
-        <f>I25/(J25*$B$51)</f>
+        <f t="shared" ref="P25:P32" si="33">I25/(J25*$B$51)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q25" s="45" t="e">
-        <f>I25/((F25/$B$50*$B$51)*R25)</f>
+        <f t="shared" ref="Q25:Q32" si="34">I25/((F25/$B$50*$B$51)*R25)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R25" s="45" t="e">
-        <f>H25/(L25*$B$51)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="26" spans="1:18" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
+        <f t="shared" ref="R25:R32" si="35">H25/(L25*$B$51)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" ht="12.45" customHeight="1">
       <c r="A26" s="40"/>
       <c r="B26" s="41"/>
       <c r="C26" s="42"/>
-      <c r="D26" s="61"/>
-      <c r="E26" s="63"/>
-      <c r="F26" s="61"/>
-      <c r="G26" s="63"/>
-      <c r="H26" s="66"/>
-      <c r="I26" s="67"/>
+      <c r="D26" s="60"/>
+      <c r="E26" s="62"/>
+      <c r="F26" s="60"/>
+      <c r="G26" s="62"/>
+      <c r="H26" s="65"/>
+      <c r="I26" s="66"/>
       <c r="J26" s="44" t="e">
         <f t="shared" si="31"/>
         <v>#DIV/0!</v>
@@ -2057,782 +2054,819 @@
         <f t="shared" si="32"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="M26" s="69"/>
-      <c r="N26" s="61"/>
-      <c r="O26" s="61"/>
+      <c r="M26" s="68"/>
+      <c r="N26" s="60"/>
+      <c r="O26" s="60"/>
       <c r="P26" s="30" t="e">
-        <f>I26/(J26*$B$51)</f>
+        <f t="shared" si="33"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Q26" s="45" t="e">
-        <f>I26/((F26/$B$50*$B$51)*R26)</f>
+        <f t="shared" si="34"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R26" s="45" t="e">
-        <f>H26/(L26*$B$51)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="27" spans="1:18" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="35"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" ht="12.45" customHeight="1">
       <c r="A27" s="40"/>
       <c r="B27" s="41"/>
       <c r="C27" s="42"/>
-      <c r="D27" s="61"/>
-      <c r="E27" s="63"/>
-      <c r="F27" s="61"/>
-      <c r="G27" s="63"/>
-      <c r="H27" s="66"/>
-      <c r="I27" s="67"/>
+      <c r="D27" s="60"/>
+      <c r="E27" s="62"/>
+      <c r="F27" s="60"/>
+      <c r="G27" s="62"/>
+      <c r="H27" s="65"/>
+      <c r="I27" s="66"/>
       <c r="J27" s="44" t="e">
         <f t="shared" si="31"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K27" s="43" t="e">
-        <f t="shared" ref="K27:K29" si="33">J27*(M27/L27)</f>
+        <f t="shared" ref="K27:K29" si="36">J27*(M27/L27)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="L27" s="44" t="e">
         <f t="shared" si="32"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="M27" s="69"/>
-      <c r="N27" s="61"/>
-      <c r="O27" s="61"/>
+      <c r="M27" s="68"/>
+      <c r="N27" s="60"/>
+      <c r="O27" s="60"/>
       <c r="P27" s="30" t="e">
-        <f>I27/(J27*$B$51)</f>
+        <f t="shared" si="33"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Q27" s="45" t="e">
-        <f>I27/((F27/$B$50*$B$51)*R27)</f>
+        <f t="shared" si="34"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R27" s="45" t="e">
-        <f>H27/(L27*$B$51)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="28" spans="1:18" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="35"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" ht="12.45" customHeight="1">
       <c r="A28" s="40"/>
       <c r="B28" s="41"/>
       <c r="C28" s="42"/>
-      <c r="D28" s="61"/>
-      <c r="E28" s="63"/>
-      <c r="F28" s="61"/>
-      <c r="G28" s="63"/>
-      <c r="H28" s="66"/>
-      <c r="I28" s="67"/>
+      <c r="D28" s="60"/>
+      <c r="E28" s="62"/>
+      <c r="F28" s="60"/>
+      <c r="G28" s="62"/>
+      <c r="H28" s="65"/>
+      <c r="I28" s="66"/>
       <c r="J28" s="44" t="e">
         <f t="shared" si="31"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K28" s="43" t="e">
-        <f t="shared" si="33"/>
+        <f t="shared" si="36"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L28" s="44" t="e">
         <f t="shared" si="32"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="M28" s="69"/>
-      <c r="N28" s="61"/>
-      <c r="O28" s="61"/>
+      <c r="M28" s="68"/>
+      <c r="N28" s="60"/>
+      <c r="O28" s="60"/>
       <c r="P28" s="30" t="e">
-        <f>I28/(J28*$B$51)</f>
+        <f t="shared" si="33"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Q28" s="45" t="e">
-        <f>I28/((F28/$B$50*$B$51)*R28)</f>
+        <f t="shared" si="34"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R28" s="45" t="e">
-        <f>H28/(L28*$B$51)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="29" spans="1:18" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="35"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" ht="12.45" customHeight="1">
       <c r="A29" s="40"/>
       <c r="B29" s="41"/>
       <c r="C29" s="42"/>
-      <c r="D29" s="61"/>
-      <c r="E29" s="63"/>
-      <c r="F29" s="61"/>
-      <c r="G29" s="63"/>
-      <c r="H29" s="66"/>
-      <c r="I29" s="67"/>
+      <c r="D29" s="60"/>
+      <c r="E29" s="62"/>
+      <c r="F29" s="60"/>
+      <c r="G29" s="62"/>
+      <c r="H29" s="65"/>
+      <c r="I29" s="66"/>
       <c r="J29" s="44" t="e">
         <f t="shared" si="31"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K29" s="43" t="e">
-        <f t="shared" si="33"/>
+        <f t="shared" si="36"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L29" s="44" t="e">
         <f t="shared" si="32"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="M29" s="69"/>
-      <c r="N29" s="61"/>
-      <c r="O29" s="61"/>
+      <c r="M29" s="68"/>
+      <c r="N29" s="60"/>
+      <c r="O29" s="60"/>
       <c r="P29" s="30" t="e">
-        <f>I29/(J29*$B$51)</f>
+        <f t="shared" si="33"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Q29" s="45" t="e">
-        <f>I29/((F29/$B$50*$B$51)*R29)</f>
+        <f t="shared" si="34"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R29" s="45" t="e">
-        <f>H29/(L29*$B$51)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="30" spans="1:18" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="35"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" ht="12.45" customHeight="1">
       <c r="A30" s="40"/>
       <c r="B30" s="41"/>
       <c r="C30" s="42"/>
-      <c r="D30" s="61"/>
-      <c r="E30" s="63"/>
-      <c r="F30" s="61"/>
-      <c r="G30" s="63"/>
-      <c r="H30" s="66"/>
-      <c r="I30" s="67"/>
+      <c r="D30" s="60"/>
+      <c r="E30" s="62"/>
+      <c r="F30" s="60"/>
+      <c r="G30" s="62"/>
+      <c r="H30" s="65"/>
+      <c r="I30" s="66"/>
       <c r="J30" s="44" t="e">
         <f t="shared" si="31"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K30" s="43" t="e">
-        <f t="shared" ref="K30:K32" si="34">J30*(M30/L30)</f>
+        <f t="shared" ref="K30:K32" si="37">J30*(M30/L30)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="L30" s="44" t="e">
         <f t="shared" si="32"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="M30" s="69"/>
-      <c r="N30" s="61"/>
-      <c r="O30" s="61"/>
+      <c r="M30" s="68"/>
+      <c r="N30" s="60"/>
+      <c r="O30" s="60"/>
       <c r="P30" s="30" t="e">
-        <f>I30/(J30*$B$51)</f>
+        <f t="shared" si="33"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Q30" s="45" t="e">
-        <f>I30/((F30/$B$50*$B$51)*R30)</f>
+        <f t="shared" si="34"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R30" s="45" t="e">
-        <f>H30/(L30*$B$51)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="31" spans="1:18" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="35"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" ht="12.45" customHeight="1">
       <c r="A31" s="40"/>
       <c r="B31" s="41"/>
       <c r="C31" s="42"/>
-      <c r="D31" s="61"/>
-      <c r="E31" s="63"/>
-      <c r="F31" s="61"/>
-      <c r="G31" s="63"/>
-      <c r="H31" s="66"/>
-      <c r="I31" s="67"/>
+      <c r="D31" s="60"/>
+      <c r="E31" s="62"/>
+      <c r="F31" s="60"/>
+      <c r="G31" s="62"/>
+      <c r="H31" s="65"/>
+      <c r="I31" s="66"/>
       <c r="J31" s="44" t="e">
         <f t="shared" si="31"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K31" s="43" t="e">
-        <f t="shared" si="34"/>
+        <f t="shared" si="37"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L31" s="44" t="e">
         <f t="shared" si="32"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="M31" s="69"/>
-      <c r="N31" s="61"/>
-      <c r="O31" s="61"/>
+      <c r="M31" s="68"/>
+      <c r="N31" s="60"/>
+      <c r="O31" s="60"/>
       <c r="P31" s="30" t="e">
-        <f>I31/(J31*$B$51)</f>
+        <f t="shared" si="33"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Q31" s="45" t="e">
-        <f>I31/((F31/$B$50*$B$51)*R31)</f>
+        <f t="shared" si="34"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R31" s="45" t="e">
-        <f>H31/(L31*$B$51)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="32" spans="1:18" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="35"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" ht="12.45" customHeight="1">
       <c r="A32" s="40"/>
       <c r="B32" s="41"/>
       <c r="C32" s="42"/>
-      <c r="D32" s="61"/>
-      <c r="E32" s="63"/>
-      <c r="F32" s="61"/>
-      <c r="G32" s="63"/>
-      <c r="H32" s="66"/>
-      <c r="I32" s="67"/>
+      <c r="D32" s="60"/>
+      <c r="E32" s="62"/>
+      <c r="F32" s="60"/>
+      <c r="G32" s="62"/>
+      <c r="H32" s="65"/>
+      <c r="I32" s="66"/>
       <c r="J32" s="44" t="e">
         <f t="shared" si="31"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K32" s="43" t="e">
-        <f t="shared" si="34"/>
+        <f t="shared" si="37"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L32" s="44" t="e">
         <f t="shared" si="32"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="M32" s="69"/>
-      <c r="N32" s="61"/>
-      <c r="O32" s="61"/>
+      <c r="M32" s="68"/>
+      <c r="N32" s="60"/>
+      <c r="O32" s="60"/>
       <c r="P32" s="30" t="e">
-        <f>I32/(J32*$B$51)</f>
+        <f t="shared" si="33"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Q32" s="45" t="e">
-        <f>I32/((F32/$B$50*$B$51)*R32)</f>
+        <f t="shared" si="34"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R32" s="45" t="e">
-        <f>H32/(L32*$B$51)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="33" spans="1:19" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="35"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" ht="12.45" customHeight="1">
       <c r="A33" s="40"/>
       <c r="B33" s="41"/>
       <c r="C33" s="42"/>
-      <c r="D33" s="61"/>
-      <c r="E33" s="63"/>
-      <c r="F33" s="61"/>
-      <c r="G33" s="63"/>
-      <c r="H33" s="66"/>
-      <c r="I33" s="67"/>
+      <c r="D33" s="60"/>
+      <c r="E33" s="62"/>
+      <c r="F33" s="60"/>
+      <c r="G33" s="62"/>
+      <c r="H33" s="65"/>
+      <c r="I33" s="66"/>
       <c r="J33" s="44" t="e">
-        <f t="shared" ref="J33" si="35">F33/$B$50</f>
+        <f t="shared" ref="J33" si="38">F33/$B$50</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K33" s="43" t="e">
-        <f t="shared" ref="K33" si="36">J33*(M33/L33)</f>
+        <f t="shared" ref="K33" si="39">J33*(M33/L33)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="L33" s="44" t="e">
-        <f t="shared" ref="L33" si="37">G33/$B$50</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M33" s="69"/>
-      <c r="N33" s="61"/>
-      <c r="O33" s="61"/>
+        <f t="shared" ref="L33" si="40">G33/$B$50</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M33" s="68"/>
+      <c r="N33" s="60"/>
+      <c r="O33" s="60"/>
       <c r="P33" s="30" t="e">
-        <f t="shared" ref="P33" si="38">I33/(J33*$B$51)</f>
+        <f t="shared" ref="P33" si="41">I33/(J33*$B$51)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q33" s="45" t="e">
-        <f t="shared" ref="Q33" si="39">I33/((F33/$B$50*$B$51)*R33)</f>
+        <f t="shared" ref="Q33" si="42">I33/((F33/$B$50*$B$51)*R33)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R33" s="45" t="e">
-        <f t="shared" ref="R33" si="40">H33/(L33*$B$51)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="34" spans="1:19" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
+        <f t="shared" ref="R33" si="43">H33/(L33*$B$51)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" ht="12.45" customHeight="1">
       <c r="A34" s="40"/>
       <c r="B34" s="41"/>
       <c r="C34" s="42"/>
-      <c r="D34" s="61"/>
-      <c r="E34" s="63"/>
-      <c r="F34" s="61"/>
-      <c r="G34" s="63"/>
-      <c r="H34" s="66"/>
-      <c r="I34" s="67"/>
+      <c r="D34" s="60"/>
+      <c r="E34" s="62"/>
+      <c r="F34" s="60"/>
+      <c r="G34" s="62"/>
+      <c r="H34" s="65"/>
+      <c r="I34" s="66"/>
       <c r="J34" s="44" t="e">
-        <f t="shared" ref="J34" si="41">F34/$B$50</f>
+        <f t="shared" ref="J34" si="44">F34/$B$50</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K34" s="43" t="e">
-        <f t="shared" ref="K34" si="42">J34*(M34/L34)</f>
+        <f t="shared" ref="K34" si="45">J34*(M34/L34)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="L34" s="44" t="e">
-        <f t="shared" ref="L34" si="43">G34/$B$50</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M34" s="69"/>
-      <c r="N34" s="61"/>
-      <c r="O34" s="61"/>
+        <f t="shared" ref="L34" si="46">G34/$B$50</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M34" s="68"/>
+      <c r="N34" s="60"/>
+      <c r="O34" s="60"/>
       <c r="P34" s="30" t="e">
-        <f t="shared" ref="P34" si="44">I34/(J34*$B$51)</f>
+        <f t="shared" ref="P34" si="47">I34/(J34*$B$51)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q34" s="45" t="e">
-        <f t="shared" ref="Q34" si="45">I34/((F34/$B$50*$B$51)*R34)</f>
+        <f t="shared" ref="Q34" si="48">I34/((F34/$B$50*$B$51)*R34)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R34" s="45" t="e">
-        <f t="shared" ref="R34" si="46">H34/(L34*$B$51)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="35" spans="1:19" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
+        <f t="shared" ref="R34" si="49">H34/(L34*$B$51)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" ht="12.45" customHeight="1">
       <c r="A35" s="40"/>
       <c r="B35" s="41"/>
       <c r="C35" s="42"/>
-      <c r="D35" s="61"/>
-      <c r="E35" s="63"/>
-      <c r="F35" s="61"/>
-      <c r="G35" s="63"/>
-      <c r="H35" s="66"/>
-      <c r="I35" s="67"/>
+      <c r="D35" s="60"/>
+      <c r="E35" s="62"/>
+      <c r="F35" s="60"/>
+      <c r="G35" s="62"/>
+      <c r="H35" s="65"/>
+      <c r="I35" s="66"/>
       <c r="J35" s="44" t="e">
-        <f t="shared" ref="J35" si="47">F35/$B$50</f>
+        <f t="shared" ref="J35" si="50">F35/$B$50</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K35" s="43" t="e">
-        <f t="shared" ref="K35:K39" si="48">J35*(M35/L35)</f>
+        <f t="shared" ref="K35:K39" si="51">J35*(M35/L35)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="L35" s="44" t="e">
-        <f t="shared" ref="L35" si="49">G35/$B$50</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M35" s="69"/>
-      <c r="N35" s="61"/>
-      <c r="O35" s="61"/>
+        <f t="shared" ref="L35" si="52">G35/$B$50</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M35" s="68"/>
+      <c r="N35" s="60"/>
+      <c r="O35" s="60"/>
       <c r="P35" s="30" t="e">
-        <f t="shared" ref="P35" si="50">I35/(J35*$B$51)</f>
+        <f t="shared" ref="P35" si="53">I35/(J35*$B$51)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q35" s="45" t="e">
-        <f t="shared" ref="Q35" si="51">I35/((F35/$B$50*$B$51)*R35)</f>
+        <f t="shared" ref="Q35" si="54">I35/((F35/$B$50*$B$51)*R35)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R35" s="45" t="e">
-        <f t="shared" ref="R35" si="52">H35/(L35*$B$51)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="36" spans="1:19" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
+        <f t="shared" ref="R35" si="55">H35/(L35*$B$51)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" ht="12.45" customHeight="1">
       <c r="A36" s="40"/>
       <c r="B36" s="41"/>
       <c r="C36" s="42"/>
-      <c r="D36" s="61"/>
-      <c r="E36" s="63"/>
-      <c r="F36" s="61"/>
-      <c r="G36" s="63"/>
-      <c r="H36" s="66"/>
-      <c r="I36" s="67"/>
+      <c r="D36" s="60"/>
+      <c r="E36" s="62"/>
+      <c r="F36" s="60"/>
+      <c r="G36" s="62"/>
+      <c r="H36" s="65"/>
+      <c r="I36" s="66"/>
       <c r="J36" s="44" t="e">
-        <f>F36/$B$50</f>
+        <f t="shared" ref="J36:J42" si="56">F36/$B$50</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K36" s="43" t="e">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L36" s="44" t="e">
-        <f>G36/$B$50</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M36" s="69"/>
-      <c r="N36" s="61"/>
-      <c r="O36" s="61"/>
+        <f t="shared" ref="L36:L42" si="57">G36/$B$50</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M36" s="68"/>
+      <c r="N36" s="60"/>
+      <c r="O36" s="60"/>
       <c r="P36" s="30" t="e">
-        <f>I36/(J36*$B$51)</f>
+        <f t="shared" ref="P36:P42" si="58">I36/(J36*$B$51)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q36" s="45" t="e">
-        <f>I36/((F36/$B$50*$B$51)*R36)</f>
+        <f t="shared" ref="Q36:Q42" si="59">I36/((F36/$B$50*$B$51)*R36)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R36" s="45" t="e">
-        <f>H36/(L36*$B$51)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="37" spans="1:19" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
+        <f t="shared" ref="R36:R42" si="60">H36/(L36*$B$51)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" ht="12.45" customHeight="1">
       <c r="A37" s="40"/>
       <c r="B37" s="41"/>
       <c r="C37" s="42"/>
-      <c r="D37" s="61"/>
-      <c r="E37" s="63"/>
-      <c r="F37" s="61"/>
-      <c r="G37" s="63"/>
-      <c r="H37" s="66"/>
-      <c r="I37" s="67"/>
+      <c r="D37" s="60"/>
+      <c r="E37" s="62"/>
+      <c r="F37" s="60"/>
+      <c r="G37" s="62"/>
+      <c r="H37" s="65"/>
+      <c r="I37" s="66"/>
       <c r="J37" s="44" t="e">
-        <f>F37/$B$50</f>
+        <f t="shared" si="56"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K37" s="43" t="e">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L37" s="44" t="e">
-        <f>G37/$B$50</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M37" s="69"/>
-      <c r="N37" s="61"/>
-      <c r="O37" s="61"/>
+        <f t="shared" si="57"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M37" s="68"/>
+      <c r="N37" s="60"/>
+      <c r="O37" s="60"/>
       <c r="P37" s="30" t="e">
-        <f>I37/(J37*$B$51)</f>
+        <f t="shared" si="58"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Q37" s="45" t="e">
-        <f>I37/((F37/$B$50*$B$51)*R37)</f>
+        <f t="shared" si="59"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R37" s="45" t="e">
-        <f>H37/(L37*$B$51)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="38" spans="1:19" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="60"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" ht="12.45" customHeight="1">
       <c r="A38" s="40"/>
       <c r="B38" s="41"/>
       <c r="C38" s="42"/>
-      <c r="D38" s="61"/>
-      <c r="E38" s="63"/>
-      <c r="F38" s="61"/>
-      <c r="G38" s="63"/>
-      <c r="H38" s="66"/>
-      <c r="I38" s="67"/>
+      <c r="D38" s="60"/>
+      <c r="E38" s="62"/>
+      <c r="F38" s="60"/>
+      <c r="G38" s="62"/>
+      <c r="H38" s="65"/>
+      <c r="I38" s="66"/>
       <c r="J38" s="44" t="e">
-        <f>F38/$B$50</f>
+        <f t="shared" si="56"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K38" s="43" t="e">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L38" s="44" t="e">
-        <f>G38/$B$50</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M38" s="69"/>
-      <c r="N38" s="61"/>
-      <c r="O38" s="61"/>
+        <f t="shared" si="57"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M38" s="68"/>
+      <c r="N38" s="60"/>
+      <c r="O38" s="60"/>
       <c r="P38" s="30" t="e">
-        <f>I38/(J38*$B$51)</f>
+        <f t="shared" si="58"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Q38" s="45" t="e">
-        <f>I38/((F38/$B$50*$B$51)*R38)</f>
+        <f t="shared" si="59"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R38" s="45" t="e">
-        <f>H38/(L38*$B$51)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="39" spans="1:19" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="60"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" ht="12.45" customHeight="1">
       <c r="A39" s="40"/>
       <c r="B39" s="41"/>
       <c r="C39" s="42"/>
-      <c r="D39" s="61"/>
-      <c r="E39" s="63"/>
-      <c r="F39" s="61"/>
-      <c r="G39" s="63"/>
-      <c r="H39" s="66"/>
-      <c r="I39" s="67"/>
+      <c r="D39" s="60"/>
+      <c r="E39" s="62"/>
+      <c r="F39" s="60"/>
+      <c r="G39" s="62"/>
+      <c r="H39" s="65"/>
+      <c r="I39" s="66"/>
       <c r="J39" s="44" t="e">
-        <f>F39/$B$50</f>
+        <f t="shared" si="56"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K39" s="43" t="e">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L39" s="44" t="e">
-        <f>G39/$B$50</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M39" s="69"/>
-      <c r="N39" s="61"/>
-      <c r="O39" s="61"/>
+        <f t="shared" si="57"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M39" s="68"/>
+      <c r="N39" s="60"/>
+      <c r="O39" s="60"/>
       <c r="P39" s="30" t="e">
-        <f>I39/(J39*$B$51)</f>
+        <f t="shared" si="58"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Q39" s="45" t="e">
-        <f>I39/((F39/$B$50*$B$51)*R39)</f>
+        <f t="shared" si="59"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R39" s="45" t="e">
-        <f>H39/(L39*$B$51)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="40" spans="1:19" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="60"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" ht="12.45" customHeight="1">
       <c r="A40" s="40"/>
       <c r="B40" s="41"/>
       <c r="C40" s="42"/>
-      <c r="D40" s="61"/>
-      <c r="E40" s="63"/>
-      <c r="F40" s="61"/>
-      <c r="G40" s="63"/>
-      <c r="H40" s="66"/>
-      <c r="I40" s="67"/>
+      <c r="D40" s="60"/>
+      <c r="E40" s="62"/>
+      <c r="F40" s="60"/>
+      <c r="G40" s="62"/>
+      <c r="H40" s="65"/>
+      <c r="I40" s="66"/>
       <c r="J40" s="44" t="e">
-        <f>F40/$B$50</f>
+        <f t="shared" si="56"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K40" s="43" t="e">
-        <f t="shared" ref="K40:K41" si="53">J40*(M40/L40)</f>
+        <f t="shared" ref="K40:K41" si="61">J40*(M40/L40)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="L40" s="44" t="e">
-        <f>G40/$B$50</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M40" s="69"/>
-      <c r="N40" s="61"/>
-      <c r="O40" s="61"/>
+        <f t="shared" si="57"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M40" s="68"/>
+      <c r="N40" s="60"/>
+      <c r="O40" s="60"/>
       <c r="P40" s="30" t="e">
-        <f>I40/(J40*$B$51)</f>
+        <f t="shared" si="58"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Q40" s="45" t="e">
-        <f>I40/((F40/$B$50*$B$51)*R40)</f>
+        <f t="shared" si="59"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R40" s="45" t="e">
-        <f>H40/(L40*$B$51)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="41" spans="1:19" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="60"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" ht="12.45" customHeight="1">
       <c r="A41" s="40"/>
       <c r="B41" s="41"/>
       <c r="C41" s="42"/>
-      <c r="D41" s="61"/>
-      <c r="E41" s="63"/>
-      <c r="F41" s="61"/>
-      <c r="G41" s="63"/>
-      <c r="H41" s="66"/>
-      <c r="I41" s="67"/>
+      <c r="D41" s="60"/>
+      <c r="E41" s="62"/>
+      <c r="F41" s="60"/>
+      <c r="G41" s="62"/>
+      <c r="H41" s="65"/>
+      <c r="I41" s="66"/>
       <c r="J41" s="44" t="e">
-        <f>F41/$B$50</f>
+        <f t="shared" si="56"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K41" s="43" t="e">
-        <f t="shared" si="53"/>
+        <f t="shared" si="61"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L41" s="44" t="e">
-        <f>G41/$B$50</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M41" s="69"/>
-      <c r="N41" s="61"/>
-      <c r="O41" s="61"/>
+        <f t="shared" si="57"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M41" s="68"/>
+      <c r="N41" s="60"/>
+      <c r="O41" s="60"/>
       <c r="P41" s="30" t="e">
-        <f>I41/(J41*$B$51)</f>
+        <f t="shared" si="58"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Q41" s="45" t="e">
-        <f>I41/((F41/$B$50*$B$51)*R41)</f>
+        <f t="shared" si="59"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R41" s="45" t="e">
-        <f>H41/(L41*$B$51)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="42" spans="1:19" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="60"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" ht="12.45" customHeight="1">
       <c r="A42" s="40"/>
       <c r="B42" s="41"/>
       <c r="C42" s="42"/>
-      <c r="D42" s="61"/>
-      <c r="E42" s="63"/>
-      <c r="F42" s="61"/>
-      <c r="G42" s="63"/>
-      <c r="H42" s="66"/>
-      <c r="I42" s="67"/>
+      <c r="D42" s="60"/>
+      <c r="E42" s="62"/>
+      <c r="F42" s="60"/>
+      <c r="G42" s="62"/>
+      <c r="H42" s="65"/>
+      <c r="I42" s="66"/>
       <c r="J42" s="44" t="e">
-        <f>F42/$B$50</f>
+        <f t="shared" si="56"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K42" s="43" t="e">
-        <f t="shared" ref="K42" si="54">J42*(M42/L42)</f>
+        <f t="shared" ref="K42" si="62">J42*(M42/L42)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="L42" s="44" t="e">
-        <f>G42/$B$50</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M42" s="69"/>
-      <c r="N42" s="61"/>
-      <c r="O42" s="61"/>
+        <f t="shared" si="57"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M42" s="68"/>
+      <c r="N42" s="60"/>
+      <c r="O42" s="60"/>
       <c r="P42" s="30" t="e">
-        <f>I42/(J42*$B$51)</f>
+        <f t="shared" si="58"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Q42" s="45" t="e">
-        <f>I42/((F42/$B$50*$B$51)*R42)</f>
+        <f t="shared" si="59"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R42" s="45" t="e">
-        <f>H42/(L42*$B$51)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="43" spans="1:19" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="60"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19" ht="12.45" customHeight="1">
       <c r="A43" s="40"/>
       <c r="B43" s="41"/>
       <c r="C43" s="42"/>
-      <c r="D43" s="61"/>
-      <c r="E43" s="63"/>
-      <c r="F43" s="61"/>
-      <c r="G43" s="63"/>
-      <c r="H43" s="66"/>
-      <c r="I43" s="67"/>
-      <c r="J43" s="44" t="e">
-        <f t="shared" ref="J43" si="55">F43/$B$50</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K43" s="43" t="e">
-        <f t="shared" ref="K43" si="56">J43*(M43/L43)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L43" s="44" t="e">
-        <f t="shared" ref="L43" si="57">G43/$B$50</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M43" s="69"/>
-      <c r="N43" s="61"/>
-      <c r="O43" s="61"/>
-      <c r="P43" s="30" t="e">
-        <f t="shared" ref="P43" si="58">I43/(J43*$B$51)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q43" s="45" t="e">
-        <f t="shared" ref="Q43" si="59">I43/((F43/$B$50*$B$51)*R43)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R43" s="45" t="e">
-        <f t="shared" ref="R43" si="60">H43/(L43*$B$51)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="44" spans="1:19" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D43" s="60"/>
+      <c r="E43" s="62"/>
+      <c r="F43" s="60"/>
+      <c r="G43" s="62"/>
+      <c r="H43" s="65"/>
+      <c r="I43" s="66"/>
+      <c r="J43" s="44"/>
+      <c r="K43" s="43"/>
+      <c r="L43" s="44"/>
+      <c r="M43" s="68"/>
+      <c r="N43" s="60"/>
+      <c r="O43" s="60"/>
+      <c r="P43" s="30"/>
+      <c r="Q43" s="45"/>
+      <c r="R43" s="45"/>
+    </row>
+    <row r="44" spans="1:19" ht="12.45" customHeight="1">
       <c r="A44" s="40"/>
       <c r="B44" s="41"/>
       <c r="C44" s="42"/>
-      <c r="D44" s="61"/>
-      <c r="E44" s="63"/>
-      <c r="F44" s="61"/>
-      <c r="G44" s="63"/>
-      <c r="H44" s="66"/>
-      <c r="I44" s="67"/>
+      <c r="D44" s="60"/>
+      <c r="E44" s="62"/>
+      <c r="F44" s="60"/>
+      <c r="G44" s="62"/>
+      <c r="H44" s="65"/>
+      <c r="I44" s="66"/>
       <c r="J44" s="44" t="e">
-        <f>F44/$B$50</f>
+        <f t="shared" ref="J44" si="63">F44/$B$50</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K44" s="43" t="e">
+        <f t="shared" ref="K44" si="64">J44*(M44/L44)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L44" s="44" t="e">
+        <f t="shared" ref="L44" si="65">G44/$B$50</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M44" s="68"/>
+      <c r="N44" s="60"/>
+      <c r="O44" s="60"/>
+      <c r="P44" s="30" t="e">
+        <f t="shared" ref="P44" si="66">I44/(J44*$B$51)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q44" s="45" t="e">
+        <f t="shared" ref="Q44" si="67">I44/((F44/$B$50*$B$51)*R44)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R44" s="45" t="e">
+        <f t="shared" ref="R44" si="68">H44/(L44*$B$51)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19" ht="12.45" customHeight="1">
+      <c r="A45" s="40"/>
+      <c r="B45" s="41"/>
+      <c r="C45" s="42"/>
+      <c r="D45" s="60"/>
+      <c r="E45" s="62"/>
+      <c r="F45" s="60"/>
+      <c r="G45" s="62"/>
+      <c r="H45" s="65"/>
+      <c r="I45" s="66"/>
+      <c r="J45" s="44"/>
+      <c r="K45" s="43"/>
+      <c r="L45" s="44"/>
+      <c r="M45" s="68"/>
+      <c r="N45" s="60"/>
+      <c r="O45" s="60"/>
+      <c r="P45" s="30"/>
+      <c r="Q45" s="45"/>
+      <c r="R45" s="45"/>
+    </row>
+    <row r="46" spans="1:19" ht="12.45" customHeight="1" thickBot="1">
+      <c r="A46" s="40"/>
+      <c r="B46" s="41"/>
+      <c r="C46" s="42"/>
+      <c r="D46" s="60"/>
+      <c r="E46" s="62"/>
+      <c r="F46" s="60"/>
+      <c r="G46" s="62"/>
+      <c r="H46" s="65"/>
+      <c r="I46" s="66"/>
+      <c r="J46" s="44" t="e">
+        <f>F46/$B$50</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K46" s="43" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="L44" s="44" t="e">
-        <f>G44/$B$50</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M44" s="69"/>
-      <c r="N44" s="61"/>
-      <c r="O44" s="61"/>
-      <c r="P44" s="30" t="e">
-        <f>I44/(J44*$B$51)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q44" s="45" t="e">
-        <f>I44/((F44/$B$50*$B$51)*R44)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R44" s="45" t="e">
-        <f>H44/(L44*$B$51)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="45" spans="1:19" ht="13.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="46"/>
-      <c r="B45" s="47" t="s">
+      <c r="L46" s="44" t="e">
+        <f>G46/$B$50</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M46" s="68"/>
+      <c r="N46" s="60"/>
+      <c r="O46" s="60"/>
+      <c r="P46" s="30" t="e">
+        <f>I46/(J46*$B$51)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q46" s="45" t="e">
+        <f>I46/((F46/$B$50*$B$51)*R46)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R46" s="45" t="e">
+        <f>H46/(L46*$B$51)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19" ht="13.2" customHeight="1" thickBot="1">
+      <c r="A47" s="46"/>
+      <c r="B47" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="C45" s="48"/>
-      <c r="D45" s="49">
-        <f t="shared" ref="D45:N45" si="61">SUM(D10:D44)</f>
+      <c r="C47" s="48"/>
+      <c r="D47" s="49">
+        <f t="shared" ref="D47:N47" si="69">SUM(D10:D46)</f>
         <v>0</v>
       </c>
-      <c r="E45" s="49">
-        <f t="shared" si="61"/>
+      <c r="E47" s="49">
+        <f t="shared" si="69"/>
         <v>0</v>
       </c>
-      <c r="F45" s="49">
-        <f t="shared" si="61"/>
+      <c r="F47" s="49">
+        <f t="shared" si="69"/>
         <v>0</v>
       </c>
-      <c r="G45" s="49">
-        <f t="shared" si="61"/>
+      <c r="G47" s="49">
+        <f t="shared" si="69"/>
         <v>0</v>
       </c>
-      <c r="H45" s="49">
-        <f t="shared" si="61"/>
+      <c r="H47" s="49">
+        <f t="shared" si="69"/>
         <v>0</v>
       </c>
-      <c r="I45" s="50">
-        <f t="shared" si="61"/>
+      <c r="I47" s="50">
+        <f t="shared" si="69"/>
         <v>0</v>
       </c>
-      <c r="J45" s="51" t="e">
-        <f t="shared" si="61"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K45" s="52" t="e">
-        <f t="shared" si="61"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L45" s="52" t="e">
-        <f t="shared" si="61"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M45" s="53">
-        <f t="shared" si="61"/>
+      <c r="J47" s="51" t="e">
+        <f t="shared" si="69"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K47" s="52" t="e">
+        <f t="shared" si="69"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L47" s="52" t="e">
+        <f t="shared" si="69"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M47" s="53">
+        <f t="shared" si="69"/>
         <v>0</v>
       </c>
-      <c r="N45" s="54">
-        <f t="shared" si="61"/>
+      <c r="N47" s="54">
+        <f t="shared" si="69"/>
         <v>0</v>
       </c>
-      <c r="O45" s="54"/>
-      <c r="P45" s="57" t="e">
-        <f>I45/(J45*$B$51)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q45" s="57" t="e">
-        <f>I45/((F45/$B$50*$B$51)*R45)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R45" s="57" t="e">
-        <f>H45/(L45*$B$51)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S45" s="58"/>
-    </row>
-    <row r="47" spans="1:19" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q47" s="59"/>
-    </row>
-    <row r="50" spans="1:3" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O47" s="54"/>
+      <c r="P47" s="57" t="e">
+        <f>I47/(J47*$B$51)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q47" s="57" t="e">
+        <f>I47/((F47/$B$50*$B$51)*R47)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R47" s="57" t="e">
+        <f>H47/(L47*$B$51)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S47" s="58"/>
+    </row>
+    <row r="50" spans="1:3" ht="12.45" customHeight="1">
       <c r="A50" s="56" t="s">
         <v>25</v>
       </c>
       <c r="B50" s="56"/>
       <c r="C50" s="55"/>
     </row>
-    <row r="51" spans="1:3" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3" ht="12.45" customHeight="1">
       <c r="A51" s="56" t="s">
         <v>26</v>
       </c>
@@ -2858,8 +2892,8 @@
 &amp;I© 2017 SunEdison&amp;I &amp;C&amp;R&amp;"Arial"&amp;8 Page 1 of 2 </oddFooter>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="D45:H45 J10:L13 P10:R13 P45:R45 J45:N45" unlockedFormula="1"/>
-    <ignoredError sqref="I45" formula="1" unlockedFormula="1"/>
+    <ignoredError sqref="D47:H47 J10:L13 P10:R13 P47:R47 J47:N47" unlockedFormula="1"/>
+    <ignoredError sqref="I47" formula="1" unlockedFormula="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
excel template change, add more rows
</commit_message>
<xml_diff>
--- a/job/templates/DailyReport-v3.xlsx
+++ b/job/templates/DailyReport-v3.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6948"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6945"/>
   </bookViews>
   <sheets>
     <sheet name="DailyProductionReport" sheetId="1" r:id="rId1"/>
@@ -12,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">DailyProductionReport!$1:$1</definedName>
   </definedNames>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -124,14 +129,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="[$-10409]#,##0;\(#,##0\)"/>
     <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
     <numFmt numFmtId="166" formatCode="0.0%"/>
     <numFmt numFmtId="167" formatCode="[$-10409]#,##0.0;\(#,##0.0\)"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -981,7 +986,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1013,9 +1018,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1047,6 +1053,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1222,28 +1229,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S51"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S61"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.45" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="12.4" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="25.33203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="21.33203125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="17.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="21.28515625" style="2" customWidth="1"/>
     <col min="4" max="9" width="13" style="2" customWidth="1"/>
-    <col min="10" max="12" width="12.88671875" style="2" customWidth="1"/>
-    <col min="13" max="13" width="19.33203125" style="2" customWidth="1"/>
-    <col min="14" max="14" width="21.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21.6640625" style="2" customWidth="1"/>
-    <col min="16" max="18" width="19.33203125" style="2" customWidth="1"/>
+    <col min="10" max="12" width="12.85546875" style="2" customWidth="1"/>
+    <col min="13" max="13" width="19.28515625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="21.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.7109375" style="2" customWidth="1"/>
+    <col min="16" max="18" width="19.28515625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="28.5" customHeight="1">
+    <row r="1" spans="1:18" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="71" t="s">
         <v>0</v>
       </c>
@@ -1265,8 +1272,8 @@
       <c r="Q1" s="71"/>
       <c r="R1" s="71"/>
     </row>
-    <row r="2" spans="1:18" ht="1.2" customHeight="1"/>
-    <row r="3" spans="1:18" ht="15.75" customHeight="1">
+    <row r="2" spans="1:18" ht="1.1499999999999999" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -1274,10 +1281,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="15.75" customHeight="1">
+    <row r="4" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="4"/>
     </row>
-    <row r="5" spans="1:18" ht="18" customHeight="1">
+    <row r="5" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="71" t="s">
         <v>3</v>
       </c>
@@ -1291,8 +1298,8 @@
       <c r="I5" s="1"/>
       <c r="J5" s="28"/>
     </row>
-    <row r="6" spans="1:18" ht="2.7" customHeight="1" thickBot="1"/>
-    <row r="7" spans="1:18" s="9" customFormat="1" ht="22.5" customHeight="1" thickBot="1">
+    <row r="6" spans="1:18" ht="2.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:18" s="9" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10"/>
       <c r="B7" s="13"/>
       <c r="C7" s="18"/>
@@ -1322,7 +1329,7 @@
       <c r="Q7" s="76"/>
       <c r="R7" s="76"/>
     </row>
-    <row r="8" spans="1:18" s="3" customFormat="1" ht="12.45" customHeight="1">
+    <row r="8" spans="1:18" s="3" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
         <v>5</v>
       </c>
@@ -1376,7 +1383,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:18" s="17" customFormat="1" ht="12.45" customHeight="1">
+    <row r="9" spans="1:18" s="17" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="16"/>
       <c r="B9" s="5"/>
       <c r="C9" s="8"/>
@@ -1424,7 +1431,7 @@
       </c>
       <c r="R9" s="32"/>
     </row>
-    <row r="10" spans="1:18" ht="12.45" customHeight="1">
+    <row r="10" spans="1:18" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="12"/>
       <c r="B10" s="6"/>
       <c r="C10" s="20"/>
@@ -1435,34 +1442,34 @@
       <c r="H10" s="63"/>
       <c r="I10" s="64"/>
       <c r="J10" s="39" t="e">
-        <f t="shared" ref="J10:J15" si="0">F10/$B$50</f>
+        <f>F10/$B$60</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K10" s="38" t="e">
-        <f t="shared" ref="K10:K46" si="1">J10*(M10/L10)</f>
+        <f t="shared" ref="K10:K53" si="0">J10*(M10/L10)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="L10" s="39" t="e">
-        <f t="shared" ref="L10:L15" si="2">G10/$B$50</f>
+        <f>G10/$B$60</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M10" s="67"/>
       <c r="N10" s="59"/>
       <c r="O10" s="59"/>
       <c r="P10" s="30" t="e">
-        <f>I10/(J10*$B$51)</f>
+        <f>I10/(J10*$B$61)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q10" s="33" t="e">
-        <f>I10/((J10*$B$51)*R10)</f>
+        <f>I10/((J10*$B$61)*R10)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R10" s="33" t="e">
-        <f>H10/(L10*$B$51)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" ht="12.45" customHeight="1">
+        <f>H10/(L10*$B$61)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12"/>
       <c r="B11" s="6"/>
       <c r="C11" s="20"/>
@@ -1473,34 +1480,34 @@
       <c r="H11" s="63"/>
       <c r="I11" s="64"/>
       <c r="J11" s="39" t="e">
+        <f>F11/$B$60</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K11" s="38" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K11" s="38" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
       <c r="L11" s="39" t="e">
-        <f t="shared" si="2"/>
+        <f>G11/$B$60</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M11" s="67"/>
       <c r="N11" s="59"/>
       <c r="O11" s="59"/>
       <c r="P11" s="30" t="e">
-        <f>I11/(J11*$B$51)</f>
+        <f>I11/(J11*$B$61)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q11" s="33" t="e">
-        <f>I11/((F11/$B$50*$B$51)*R11)</f>
+        <f>I11/((F11/$B$60*$B$61)*R11)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R11" s="33" t="e">
-        <f>H11/(L11*$B$51)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" ht="12.45" customHeight="1">
+        <f>H11/(L11*$B$61)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="12"/>
       <c r="B12" s="6"/>
       <c r="C12" s="20"/>
@@ -1511,34 +1518,34 @@
       <c r="H12" s="63"/>
       <c r="I12" s="64"/>
       <c r="J12" s="39" t="e">
+        <f>F12/$B$60</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K12" s="38" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K12" s="38" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
       <c r="L12" s="39" t="e">
-        <f t="shared" si="2"/>
+        <f>G12/$B$60</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M12" s="67"/>
       <c r="N12" s="59"/>
       <c r="O12" s="59"/>
       <c r="P12" s="30" t="e">
-        <f>I12/(J12*$B$51)</f>
+        <f>I12/(J12*$B$61)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q12" s="33" t="e">
-        <f>I12/((F12/$B$50*$B$51)*R12)</f>
+        <f>I12/((F12/$B$60*$B$61)*R12)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R12" s="33" t="e">
-        <f>H12/(L12*$B$51)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" ht="12.45" customHeight="1">
+        <f>H12/(L12*$B$61)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="6"/>
       <c r="C13" s="20"/>
@@ -1549,34 +1556,34 @@
       <c r="H13" s="63"/>
       <c r="I13" s="64"/>
       <c r="J13" s="39" t="e">
+        <f>F13/$B$60</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K13" s="38" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K13" s="38" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
       <c r="L13" s="39" t="e">
-        <f t="shared" si="2"/>
+        <f>G13/$B$60</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M13" s="67"/>
       <c r="N13" s="59"/>
       <c r="O13" s="59"/>
       <c r="P13" s="30" t="e">
-        <f>I13/(J13*$B$51)</f>
+        <f>I13/(J13*$B$61)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q13" s="33" t="e">
-        <f>I13/((F13/$B$50*$B$51)*R13)</f>
+        <f>I13/((F13/$B$60*$B$61)*R13)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R13" s="33" t="e">
-        <f>H13/(L13*$B$51)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" ht="12.45" customHeight="1">
+        <f>H13/(L13*$B$61)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="40"/>
       <c r="B14" s="41"/>
       <c r="C14" s="42"/>
@@ -1587,34 +1594,34 @@
       <c r="H14" s="65"/>
       <c r="I14" s="66"/>
       <c r="J14" s="44" t="e">
+        <f>F14/$B$60</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K14" s="43" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K14" s="43" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
       <c r="L14" s="44" t="e">
-        <f t="shared" si="2"/>
+        <f>G14/$B$60</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M14" s="68"/>
       <c r="N14" s="60"/>
       <c r="O14" s="60"/>
       <c r="P14" s="30" t="e">
-        <f t="shared" ref="P14" si="3">I14/(J14*$B$51)</f>
+        <f>I14/(J14*$B$61)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q14" s="45" t="e">
-        <f>I14/((F14/$B$50*$B$51)*R14)</f>
+        <f>I14/((F14/$B$60*$B$61)*R14)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R14" s="45" t="e">
-        <f t="shared" ref="R14" si="4">H14/(L14*$B$51)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" ht="12.45" customHeight="1">
+        <f>H14/(L14*$B$61)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="40"/>
       <c r="B15" s="41"/>
       <c r="C15" s="42"/>
@@ -1625,34 +1632,34 @@
       <c r="H15" s="65"/>
       <c r="I15" s="66"/>
       <c r="J15" s="44" t="e">
-        <f t="shared" si="0"/>
+        <f>F15/$B$60</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K15" s="43" t="e">
-        <f t="shared" ref="K15:K16" si="5">J15*(M15/L15)</f>
+        <f t="shared" ref="K15:K16" si="1">J15*(M15/L15)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="L15" s="44" t="e">
-        <f t="shared" si="2"/>
+        <f>G15/$B$60</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M15" s="68"/>
       <c r="N15" s="60"/>
       <c r="O15" s="60"/>
       <c r="P15" s="30" t="e">
-        <f>I15/(J15*$B$51)</f>
+        <f>I15/(J15*$B$61)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q15" s="45" t="e">
-        <f>I15/((F15/$B$50*$B$51)*R15)</f>
+        <f>I15/((F15/$B$60*$B$61)*R15)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R15" s="45" t="e">
-        <f>H15/(L15*$B$51)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" ht="12.45" customHeight="1">
+        <f>H15/(L15*$B$61)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="40"/>
       <c r="B16" s="41"/>
       <c r="C16" s="42"/>
@@ -1663,34 +1670,34 @@
       <c r="H16" s="65"/>
       <c r="I16" s="66"/>
       <c r="J16" s="44" t="e">
-        <f t="shared" ref="J16" si="6">F16/$B$50</f>
+        <f>F16/$B$60</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K16" s="43" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L16" s="44" t="e">
-        <f t="shared" ref="L16" si="7">G16/$B$50</f>
+        <f>G16/$B$60</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M16" s="68"/>
       <c r="N16" s="60"/>
       <c r="O16" s="60"/>
       <c r="P16" s="30" t="e">
-        <f>I16/(J16*$B$51)</f>
+        <f>I16/(J16*$B$61)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q16" s="45" t="e">
-        <f t="shared" ref="Q16" si="8">I16/((F16/$B$50*$B$51)*R16)</f>
+        <f>I16/((F16/$B$60*$B$61)*R16)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R16" s="45" t="e">
-        <f>H16/(L16*$B$51)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" ht="12.45" customHeight="1">
+        <f>H16/(L16*$B$61)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="40"/>
       <c r="B17" s="41"/>
       <c r="C17" s="42"/>
@@ -1701,34 +1708,34 @@
       <c r="H17" s="65"/>
       <c r="I17" s="66"/>
       <c r="J17" s="44" t="e">
-        <f t="shared" ref="J17" si="9">F17/$B$50</f>
+        <f>F17/$B$60</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K17" s="43" t="e">
-        <f t="shared" ref="K17" si="10">J17*(M17/L17)</f>
+        <f t="shared" ref="K17" si="2">J17*(M17/L17)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="L17" s="44" t="e">
-        <f t="shared" ref="L17" si="11">G17/$B$50</f>
+        <f>G17/$B$60</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M17" s="68"/>
       <c r="N17" s="60"/>
       <c r="O17" s="60"/>
       <c r="P17" s="30" t="e">
-        <f>I17/(J17*$B$51)</f>
+        <f>I17/(J17*$B$61)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q17" s="45" t="e">
-        <f t="shared" ref="Q17" si="12">I17/((F17/$B$50*$B$51)*R17)</f>
+        <f>I17/((F17/$B$60*$B$61)*R17)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R17" s="45" t="e">
-        <f>H17/(L17*$B$51)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" ht="12.45" customHeight="1">
+        <f>H17/(L17*$B$61)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="40"/>
       <c r="B18" s="41"/>
       <c r="C18" s="42"/>
@@ -1739,34 +1746,34 @@
       <c r="H18" s="65"/>
       <c r="I18" s="66"/>
       <c r="J18" s="44" t="e">
-        <f t="shared" ref="J18" si="13">F18/$B$50</f>
+        <f>F18/$B$60</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K18" s="43" t="e">
-        <f t="shared" ref="K18" si="14">J18*(M18/L18)</f>
+        <f t="shared" ref="K18" si="3">J18*(M18/L18)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="L18" s="44" t="e">
-        <f t="shared" ref="L18" si="15">G18/$B$50</f>
+        <f>G18/$B$60</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M18" s="68"/>
       <c r="N18" s="60"/>
       <c r="O18" s="60"/>
       <c r="P18" s="30" t="e">
-        <f>I18/(J18*$B$51)</f>
+        <f>I18/(J18*$B$61)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q18" s="45" t="e">
-        <f t="shared" ref="Q18" si="16">I18/((F18/$B$50*$B$51)*R18)</f>
+        <f>I18/((F18/$B$60*$B$61)*R18)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R18" s="45" t="e">
-        <f>H18/(L18*$B$51)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18" ht="12.45" customHeight="1">
+        <f>H18/(L18*$B$61)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="40"/>
       <c r="B19" s="41"/>
       <c r="C19" s="42"/>
@@ -1777,34 +1784,34 @@
       <c r="H19" s="65"/>
       <c r="I19" s="66"/>
       <c r="J19" s="44" t="e">
-        <f>F19/$B$50</f>
+        <f>F19/$B$60</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K19" s="43" t="e">
-        <f t="shared" ref="K19:K26" si="17">J19*(M19/L19)</f>
+        <f t="shared" ref="K19:K26" si="4">J19*(M19/L19)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="L19" s="44" t="e">
-        <f>G19/$B$50</f>
+        <f>G19/$B$60</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M19" s="68"/>
       <c r="N19" s="60"/>
       <c r="O19" s="60"/>
       <c r="P19" s="30" t="e">
-        <f>I19/(J19*$B$51)</f>
+        <f>I19/(J19*$B$61)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q19" s="45" t="e">
-        <f>I19/((F19/$B$50*$B$51)*R19)</f>
+        <f>I19/((F19/$B$60*$B$61)*R19)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R19" s="45" t="e">
-        <f>H19/(L19*$B$51)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" ht="12.45" customHeight="1">
+        <f>H19/(L19*$B$61)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="40"/>
       <c r="B20" s="41"/>
       <c r="C20" s="42"/>
@@ -1815,34 +1822,34 @@
       <c r="H20" s="65"/>
       <c r="I20" s="66"/>
       <c r="J20" s="44" t="e">
-        <f t="shared" ref="J20" si="18">F20/$B$50</f>
+        <f>F20/$B$60</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K20" s="43" t="e">
-        <f t="shared" ref="K20" si="19">J20*(M20/L20)</f>
+        <f t="shared" ref="K20" si="5">J20*(M20/L20)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="L20" s="44" t="e">
-        <f t="shared" ref="L20" si="20">G20/$B$50</f>
+        <f>G20/$B$60</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M20" s="68"/>
       <c r="N20" s="60"/>
       <c r="O20" s="60"/>
       <c r="P20" s="30" t="e">
-        <f t="shared" ref="P20" si="21">I20/(J20*$B$51)</f>
+        <f>I20/(J20*$B$61)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q20" s="45" t="e">
-        <f t="shared" ref="Q20" si="22">I20/((F20/$B$50*$B$51)*R20)</f>
+        <f>I20/((F20/$B$60*$B$61)*R20)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R20" s="45" t="e">
-        <f t="shared" ref="R20" si="23">H20/(L20*$B$51)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="21" spans="1:18" ht="12.45" customHeight="1">
+        <f>H20/(L20*$B$61)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="40"/>
       <c r="B21" s="41"/>
       <c r="C21" s="42"/>
@@ -1853,34 +1860,34 @@
       <c r="H21" s="65"/>
       <c r="I21" s="66"/>
       <c r="J21" s="44" t="e">
-        <f>F21/$B$50</f>
+        <f>F21/$B$60</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K21" s="43" t="e">
-        <f t="shared" si="17"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L21" s="44" t="e">
-        <f>G21/$B$50</f>
+        <f>G21/$B$60</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M21" s="68"/>
       <c r="N21" s="60"/>
       <c r="O21" s="60"/>
       <c r="P21" s="30" t="e">
-        <f>I21/(J21*$B$51)</f>
+        <f>I21/(J21*$B$61)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q21" s="45" t="e">
-        <f>I21/((F21/$B$50*$B$51)*R21)</f>
+        <f>I21/((F21/$B$60*$B$61)*R21)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R21" s="45" t="e">
-        <f>H21/(L21*$B$51)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="22" spans="1:18" ht="12.45" customHeight="1">
+        <f>H21/(L21*$B$61)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="40"/>
       <c r="B22" s="41"/>
       <c r="C22" s="42"/>
@@ -1891,34 +1898,34 @@
       <c r="H22" s="65"/>
       <c r="I22" s="66"/>
       <c r="J22" s="44" t="e">
-        <f>F22/$B$50</f>
+        <f>F22/$B$60</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K22" s="43" t="e">
-        <f t="shared" ref="K22:K23" si="24">J22*(M22/L22)</f>
+        <f t="shared" ref="K22:K23" si="6">J22*(M22/L22)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="L22" s="44" t="e">
-        <f>G22/$B$50</f>
+        <f>G22/$B$60</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M22" s="68"/>
       <c r="N22" s="60"/>
       <c r="O22" s="60"/>
       <c r="P22" s="30" t="e">
-        <f>I22/(J22*$B$51)</f>
+        <f>I22/(J22*$B$61)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q22" s="45" t="e">
-        <f>I22/((F22/$B$50*$B$51)*R22)</f>
+        <f>I22/((F22/$B$60*$B$61)*R22)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R22" s="45" t="e">
-        <f>H22/(L22*$B$51)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="23" spans="1:18" ht="12.45" customHeight="1">
+        <f>H22/(L22*$B$61)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="40"/>
       <c r="B23" s="41"/>
       <c r="C23" s="42"/>
@@ -1929,34 +1936,34 @@
       <c r="H23" s="65"/>
       <c r="I23" s="66"/>
       <c r="J23" s="44" t="e">
-        <f>F23/$B$50</f>
+        <f>F23/$B$60</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K23" s="43" t="e">
-        <f t="shared" si="24"/>
+        <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L23" s="44" t="e">
-        <f>G23/$B$50</f>
+        <f>G23/$B$60</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M23" s="68"/>
       <c r="N23" s="60"/>
       <c r="O23" s="60"/>
       <c r="P23" s="30" t="e">
-        <f>I23/(J23*$B$51)</f>
+        <f>I23/(J23*$B$61)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q23" s="45" t="e">
-        <f>I23/((F23/$B$50*$B$51)*R23)</f>
+        <f>I23/((F23/$B$60*$B$61)*R23)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R23" s="45" t="e">
-        <f>H23/(L23*$B$51)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="24" spans="1:18" ht="12.45" customHeight="1">
+        <f>H23/(L23*$B$61)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="40"/>
       <c r="B24" s="41"/>
       <c r="C24" s="42"/>
@@ -1967,34 +1974,34 @@
       <c r="H24" s="65"/>
       <c r="I24" s="66"/>
       <c r="J24" s="44" t="e">
-        <f t="shared" ref="J24" si="25">F24/$B$50</f>
+        <f>F24/$B$60</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K24" s="43" t="e">
-        <f t="shared" ref="K24" si="26">J24*(M24/L24)</f>
+        <f t="shared" ref="K24" si="7">J24*(M24/L24)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="L24" s="44" t="e">
-        <f t="shared" ref="L24" si="27">G24/$B$50</f>
+        <f>G24/$B$60</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M24" s="68"/>
       <c r="N24" s="60"/>
       <c r="O24" s="60"/>
       <c r="P24" s="30" t="e">
-        <f t="shared" ref="P24" si="28">I24/(J24*$B$51)</f>
+        <f>I24/(J24*$B$61)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q24" s="45" t="e">
-        <f t="shared" ref="Q24" si="29">I24/((F24/$B$50*$B$51)*R24)</f>
+        <f>I24/((F24/$B$60*$B$61)*R24)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R24" s="45" t="e">
-        <f t="shared" ref="R24" si="30">H24/(L24*$B$51)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="25" spans="1:18" ht="12.45" customHeight="1">
+        <f>H24/(L24*$B$61)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="40"/>
       <c r="B25" s="41"/>
       <c r="C25" s="42"/>
@@ -2005,34 +2012,34 @@
       <c r="H25" s="65"/>
       <c r="I25" s="66"/>
       <c r="J25" s="44" t="e">
-        <f t="shared" ref="J25:J32" si="31">F25/$B$50</f>
+        <f>F25/$B$60</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K25" s="43" t="e">
-        <f t="shared" si="17"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L25" s="44" t="e">
-        <f t="shared" ref="L25:L32" si="32">G25/$B$50</f>
+        <f>G25/$B$60</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M25" s="68"/>
       <c r="N25" s="60"/>
       <c r="O25" s="60"/>
       <c r="P25" s="30" t="e">
-        <f t="shared" ref="P25:P32" si="33">I25/(J25*$B$51)</f>
+        <f>I25/(J25*$B$61)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q25" s="45" t="e">
-        <f t="shared" ref="Q25:Q32" si="34">I25/((F25/$B$50*$B$51)*R25)</f>
+        <f>I25/((F25/$B$60*$B$61)*R25)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R25" s="45" t="e">
-        <f t="shared" ref="R25:R32" si="35">H25/(L25*$B$51)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="26" spans="1:18" ht="12.45" customHeight="1">
+        <f>H25/(L25*$B$61)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="40"/>
       <c r="B26" s="41"/>
       <c r="C26" s="42"/>
@@ -2043,34 +2050,34 @@
       <c r="H26" s="65"/>
       <c r="I26" s="66"/>
       <c r="J26" s="44" t="e">
-        <f t="shared" si="31"/>
+        <f>F26/$B$60</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K26" s="43" t="e">
-        <f t="shared" si="17"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L26" s="44" t="e">
-        <f t="shared" si="32"/>
+        <f>G26/$B$60</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M26" s="68"/>
       <c r="N26" s="60"/>
       <c r="O26" s="60"/>
       <c r="P26" s="30" t="e">
-        <f t="shared" si="33"/>
+        <f>I26/(J26*$B$61)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q26" s="45" t="e">
-        <f t="shared" si="34"/>
+        <f>I26/((F26/$B$60*$B$61)*R26)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R26" s="45" t="e">
-        <f t="shared" si="35"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="27" spans="1:18" ht="12.45" customHeight="1">
+        <f>H26/(L26*$B$61)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="40"/>
       <c r="B27" s="41"/>
       <c r="C27" s="42"/>
@@ -2081,34 +2088,34 @@
       <c r="H27" s="65"/>
       <c r="I27" s="66"/>
       <c r="J27" s="44" t="e">
-        <f t="shared" si="31"/>
+        <f>F27/$B$60</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K27" s="43" t="e">
-        <f t="shared" ref="K27:K29" si="36">J27*(M27/L27)</f>
+        <f t="shared" ref="K27:K29" si="8">J27*(M27/L27)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="L27" s="44" t="e">
-        <f t="shared" si="32"/>
+        <f>G27/$B$60</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M27" s="68"/>
       <c r="N27" s="60"/>
       <c r="O27" s="60"/>
       <c r="P27" s="30" t="e">
-        <f t="shared" si="33"/>
+        <f>I27/(J27*$B$61)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q27" s="45" t="e">
-        <f t="shared" si="34"/>
+        <f>I27/((F27/$B$60*$B$61)*R27)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R27" s="45" t="e">
-        <f t="shared" si="35"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="28" spans="1:18" ht="12.45" customHeight="1">
+        <f>H27/(L27*$B$61)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="40"/>
       <c r="B28" s="41"/>
       <c r="C28" s="42"/>
@@ -2119,34 +2126,34 @@
       <c r="H28" s="65"/>
       <c r="I28" s="66"/>
       <c r="J28" s="44" t="e">
-        <f t="shared" si="31"/>
+        <f>F28/$B$60</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K28" s="43" t="e">
-        <f t="shared" si="36"/>
+        <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L28" s="44" t="e">
-        <f t="shared" si="32"/>
+        <f>G28/$B$60</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M28" s="68"/>
       <c r="N28" s="60"/>
       <c r="O28" s="60"/>
       <c r="P28" s="30" t="e">
-        <f t="shared" si="33"/>
+        <f>I28/(J28*$B$61)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q28" s="45" t="e">
-        <f t="shared" si="34"/>
+        <f>I28/((F28/$B$60*$B$61)*R28)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R28" s="45" t="e">
-        <f t="shared" si="35"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="29" spans="1:18" ht="12.45" customHeight="1">
+        <f>H28/(L28*$B$61)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="40"/>
       <c r="B29" s="41"/>
       <c r="C29" s="42"/>
@@ -2157,34 +2164,34 @@
       <c r="H29" s="65"/>
       <c r="I29" s="66"/>
       <c r="J29" s="44" t="e">
-        <f t="shared" si="31"/>
+        <f>F29/$B$60</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K29" s="43" t="e">
-        <f t="shared" si="36"/>
+        <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L29" s="44" t="e">
-        <f t="shared" si="32"/>
+        <f>G29/$B$60</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M29" s="68"/>
       <c r="N29" s="60"/>
       <c r="O29" s="60"/>
       <c r="P29" s="30" t="e">
-        <f t="shared" si="33"/>
+        <f>I29/(J29*$B$61)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q29" s="45" t="e">
-        <f t="shared" si="34"/>
+        <f>I29/((F29/$B$60*$B$61)*R29)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R29" s="45" t="e">
-        <f t="shared" si="35"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="30" spans="1:18" ht="12.45" customHeight="1">
+        <f>H29/(L29*$B$61)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="40"/>
       <c r="B30" s="41"/>
       <c r="C30" s="42"/>
@@ -2195,34 +2202,34 @@
       <c r="H30" s="65"/>
       <c r="I30" s="66"/>
       <c r="J30" s="44" t="e">
-        <f t="shared" si="31"/>
+        <f>F30/$B$60</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K30" s="43" t="e">
-        <f t="shared" ref="K30:K32" si="37">J30*(M30/L30)</f>
+        <f t="shared" ref="K30:K32" si="9">J30*(M30/L30)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="L30" s="44" t="e">
-        <f t="shared" si="32"/>
+        <f>G30/$B$60</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M30" s="68"/>
       <c r="N30" s="60"/>
       <c r="O30" s="60"/>
       <c r="P30" s="30" t="e">
-        <f t="shared" si="33"/>
+        <f>I30/(J30*$B$61)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q30" s="45" t="e">
-        <f t="shared" si="34"/>
+        <f>I30/((F30/$B$60*$B$61)*R30)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R30" s="45" t="e">
-        <f t="shared" si="35"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="31" spans="1:18" ht="12.45" customHeight="1">
+        <f>H30/(L30*$B$61)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="40"/>
       <c r="B31" s="41"/>
       <c r="C31" s="42"/>
@@ -2233,34 +2240,34 @@
       <c r="H31" s="65"/>
       <c r="I31" s="66"/>
       <c r="J31" s="44" t="e">
-        <f t="shared" si="31"/>
+        <f>F31/$B$60</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K31" s="43" t="e">
-        <f t="shared" si="37"/>
+        <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L31" s="44" t="e">
-        <f t="shared" si="32"/>
+        <f>G31/$B$60</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M31" s="68"/>
       <c r="N31" s="60"/>
       <c r="O31" s="60"/>
       <c r="P31" s="30" t="e">
-        <f t="shared" si="33"/>
+        <f>I31/(J31*$B$61)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q31" s="45" t="e">
-        <f t="shared" si="34"/>
+        <f>I31/((F31/$B$60*$B$61)*R31)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R31" s="45" t="e">
-        <f t="shared" si="35"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="32" spans="1:18" ht="12.45" customHeight="1">
+        <f>H31/(L31*$B$61)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="40"/>
       <c r="B32" s="41"/>
       <c r="C32" s="42"/>
@@ -2271,34 +2278,34 @@
       <c r="H32" s="65"/>
       <c r="I32" s="66"/>
       <c r="J32" s="44" t="e">
-        <f t="shared" si="31"/>
+        <f>F32/$B$60</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K32" s="43" t="e">
-        <f t="shared" si="37"/>
+        <f t="shared" si="9"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L32" s="44" t="e">
-        <f t="shared" si="32"/>
+        <f>G32/$B$60</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M32" s="68"/>
       <c r="N32" s="60"/>
       <c r="O32" s="60"/>
       <c r="P32" s="30" t="e">
-        <f t="shared" si="33"/>
+        <f>I32/(J32*$B$61)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q32" s="45" t="e">
-        <f t="shared" si="34"/>
+        <f>I32/((F32/$B$60*$B$61)*R32)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R32" s="45" t="e">
-        <f t="shared" si="35"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="33" spans="1:19" ht="12.45" customHeight="1">
+        <f>H32/(L32*$B$61)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="40"/>
       <c r="B33" s="41"/>
       <c r="C33" s="42"/>
@@ -2309,34 +2316,34 @@
       <c r="H33" s="65"/>
       <c r="I33" s="66"/>
       <c r="J33" s="44" t="e">
-        <f t="shared" ref="J33" si="38">F33/$B$50</f>
+        <f>F33/$B$60</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K33" s="43" t="e">
-        <f t="shared" ref="K33" si="39">J33*(M33/L33)</f>
+        <f t="shared" ref="K33" si="10">J33*(M33/L33)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="L33" s="44" t="e">
-        <f t="shared" ref="L33" si="40">G33/$B$50</f>
+        <f>G33/$B$60</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M33" s="68"/>
       <c r="N33" s="60"/>
       <c r="O33" s="60"/>
       <c r="P33" s="30" t="e">
-        <f t="shared" ref="P33" si="41">I33/(J33*$B$51)</f>
+        <f>I33/(J33*$B$61)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q33" s="45" t="e">
-        <f t="shared" ref="Q33" si="42">I33/((F33/$B$50*$B$51)*R33)</f>
+        <f>I33/((F33/$B$60*$B$61)*R33)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R33" s="45" t="e">
-        <f t="shared" ref="R33" si="43">H33/(L33*$B$51)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="34" spans="1:19" ht="12.45" customHeight="1">
+        <f>H33/(L33*$B$61)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="40"/>
       <c r="B34" s="41"/>
       <c r="C34" s="42"/>
@@ -2347,34 +2354,34 @@
       <c r="H34" s="65"/>
       <c r="I34" s="66"/>
       <c r="J34" s="44" t="e">
-        <f t="shared" ref="J34" si="44">F34/$B$50</f>
+        <f>F34/$B$60</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K34" s="43" t="e">
-        <f t="shared" ref="K34" si="45">J34*(M34/L34)</f>
+        <f t="shared" ref="K34" si="11">J34*(M34/L34)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="L34" s="44" t="e">
-        <f t="shared" ref="L34" si="46">G34/$B$50</f>
+        <f>G34/$B$60</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M34" s="68"/>
       <c r="N34" s="60"/>
       <c r="O34" s="60"/>
       <c r="P34" s="30" t="e">
-        <f t="shared" ref="P34" si="47">I34/(J34*$B$51)</f>
+        <f>I34/(J34*$B$61)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q34" s="45" t="e">
-        <f t="shared" ref="Q34" si="48">I34/((F34/$B$50*$B$51)*R34)</f>
+        <f>I34/((F34/$B$60*$B$61)*R34)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R34" s="45" t="e">
-        <f t="shared" ref="R34" si="49">H34/(L34*$B$51)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="35" spans="1:19" ht="12.45" customHeight="1">
+        <f>H34/(L34*$B$61)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="40"/>
       <c r="B35" s="41"/>
       <c r="C35" s="42"/>
@@ -2385,34 +2392,34 @@
       <c r="H35" s="65"/>
       <c r="I35" s="66"/>
       <c r="J35" s="44" t="e">
-        <f t="shared" ref="J35" si="50">F35/$B$50</f>
+        <f>F35/$B$60</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K35" s="43" t="e">
-        <f t="shared" ref="K35:K39" si="51">J35*(M35/L35)</f>
+        <f t="shared" ref="K35:K39" si="12">J35*(M35/L35)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="L35" s="44" t="e">
-        <f t="shared" ref="L35" si="52">G35/$B$50</f>
+        <f>G35/$B$60</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M35" s="68"/>
       <c r="N35" s="60"/>
       <c r="O35" s="60"/>
       <c r="P35" s="30" t="e">
-        <f t="shared" ref="P35" si="53">I35/(J35*$B$51)</f>
+        <f>I35/(J35*$B$61)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q35" s="45" t="e">
-        <f t="shared" ref="Q35" si="54">I35/((F35/$B$50*$B$51)*R35)</f>
+        <f>I35/((F35/$B$60*$B$61)*R35)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R35" s="45" t="e">
-        <f t="shared" ref="R35" si="55">H35/(L35*$B$51)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="36" spans="1:19" ht="12.45" customHeight="1">
+        <f>H35/(L35*$B$61)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="40"/>
       <c r="B36" s="41"/>
       <c r="C36" s="42"/>
@@ -2423,34 +2430,34 @@
       <c r="H36" s="65"/>
       <c r="I36" s="66"/>
       <c r="J36" s="44" t="e">
-        <f t="shared" ref="J36:J42" si="56">F36/$B$50</f>
+        <f>F36/$B$60</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K36" s="43" t="e">
-        <f t="shared" si="51"/>
+        <f t="shared" si="12"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L36" s="44" t="e">
-        <f t="shared" ref="L36:L42" si="57">G36/$B$50</f>
+        <f>G36/$B$60</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M36" s="68"/>
       <c r="N36" s="60"/>
       <c r="O36" s="60"/>
       <c r="P36" s="30" t="e">
-        <f t="shared" ref="P36:P42" si="58">I36/(J36*$B$51)</f>
+        <f>I36/(J36*$B$61)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q36" s="45" t="e">
-        <f t="shared" ref="Q36:Q42" si="59">I36/((F36/$B$50*$B$51)*R36)</f>
+        <f>I36/((F36/$B$60*$B$61)*R36)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R36" s="45" t="e">
-        <f t="shared" ref="R36:R42" si="60">H36/(L36*$B$51)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="37" spans="1:19" ht="12.45" customHeight="1">
+        <f>H36/(L36*$B$61)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="40"/>
       <c r="B37" s="41"/>
       <c r="C37" s="42"/>
@@ -2461,34 +2468,34 @@
       <c r="H37" s="65"/>
       <c r="I37" s="66"/>
       <c r="J37" s="44" t="e">
-        <f t="shared" si="56"/>
+        <f>F37/$B$60</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K37" s="43" t="e">
-        <f t="shared" si="51"/>
+        <f t="shared" si="12"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L37" s="44" t="e">
-        <f t="shared" si="57"/>
+        <f>G37/$B$60</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M37" s="68"/>
       <c r="N37" s="60"/>
       <c r="O37" s="60"/>
       <c r="P37" s="30" t="e">
-        <f t="shared" si="58"/>
+        <f>I37/(J37*$B$61)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q37" s="45" t="e">
-        <f t="shared" si="59"/>
+        <f>I37/((F37/$B$60*$B$61)*R37)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R37" s="45" t="e">
-        <f t="shared" si="60"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="38" spans="1:19" ht="12.45" customHeight="1">
+        <f>H37/(L37*$B$61)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="40"/>
       <c r="B38" s="41"/>
       <c r="C38" s="42"/>
@@ -2499,34 +2506,34 @@
       <c r="H38" s="65"/>
       <c r="I38" s="66"/>
       <c r="J38" s="44" t="e">
-        <f t="shared" si="56"/>
+        <f>F38/$B$60</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K38" s="43" t="e">
-        <f t="shared" si="51"/>
+        <f t="shared" si="12"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L38" s="44" t="e">
-        <f t="shared" si="57"/>
+        <f>G38/$B$60</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M38" s="68"/>
       <c r="N38" s="60"/>
       <c r="O38" s="60"/>
       <c r="P38" s="30" t="e">
-        <f t="shared" si="58"/>
+        <f>I38/(J38*$B$61)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q38" s="45" t="e">
-        <f t="shared" si="59"/>
+        <f>I38/((F38/$B$60*$B$61)*R38)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R38" s="45" t="e">
-        <f t="shared" si="60"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="39" spans="1:19" ht="12.45" customHeight="1">
+        <f>H38/(L38*$B$61)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="40"/>
       <c r="B39" s="41"/>
       <c r="C39" s="42"/>
@@ -2537,34 +2544,34 @@
       <c r="H39" s="65"/>
       <c r="I39" s="66"/>
       <c r="J39" s="44" t="e">
-        <f t="shared" si="56"/>
+        <f>F39/$B$60</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K39" s="43" t="e">
-        <f t="shared" si="51"/>
+        <f t="shared" si="12"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L39" s="44" t="e">
-        <f t="shared" si="57"/>
+        <f>G39/$B$60</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M39" s="68"/>
       <c r="N39" s="60"/>
       <c r="O39" s="60"/>
       <c r="P39" s="30" t="e">
-        <f t="shared" si="58"/>
+        <f>I39/(J39*$B$61)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q39" s="45" t="e">
-        <f t="shared" si="59"/>
+        <f>I39/((F39/$B$60*$B$61)*R39)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R39" s="45" t="e">
-        <f t="shared" si="60"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="40" spans="1:19" ht="12.45" customHeight="1">
+        <f>H39/(L39*$B$61)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="40"/>
       <c r="B40" s="41"/>
       <c r="C40" s="42"/>
@@ -2575,34 +2582,34 @@
       <c r="H40" s="65"/>
       <c r="I40" s="66"/>
       <c r="J40" s="44" t="e">
-        <f t="shared" si="56"/>
+        <f>F40/$B$60</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K40" s="43" t="e">
-        <f t="shared" ref="K40:K41" si="61">J40*(M40/L40)</f>
+        <f t="shared" ref="K40:K46" si="13">J40*(M40/L40)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="L40" s="44" t="e">
-        <f t="shared" si="57"/>
+        <f>G40/$B$60</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M40" s="68"/>
       <c r="N40" s="60"/>
       <c r="O40" s="60"/>
       <c r="P40" s="30" t="e">
-        <f t="shared" si="58"/>
+        <f>I40/(J40*$B$61)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q40" s="45" t="e">
-        <f t="shared" si="59"/>
+        <f>I40/((F40/$B$60*$B$61)*R40)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R40" s="45" t="e">
-        <f t="shared" si="60"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="41" spans="1:19" ht="12.45" customHeight="1">
+        <f>H40/(L40*$B$61)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="40"/>
       <c r="B41" s="41"/>
       <c r="C41" s="42"/>
@@ -2613,34 +2620,19 @@
       <c r="H41" s="65"/>
       <c r="I41" s="66"/>
       <c r="J41" s="44" t="e">
-        <f t="shared" si="56"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K41" s="43" t="e">
-        <f t="shared" si="61"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L41" s="44" t="e">
-        <f t="shared" si="57"/>
-        <v>#DIV/0!</v>
-      </c>
+        <f>F41/$B$60</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K41" s="43"/>
+      <c r="L41" s="44"/>
       <c r="M41" s="68"/>
       <c r="N41" s="60"/>
       <c r="O41" s="60"/>
-      <c r="P41" s="30" t="e">
-        <f t="shared" si="58"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q41" s="45" t="e">
-        <f t="shared" si="59"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R41" s="45" t="e">
-        <f t="shared" si="60"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="42" spans="1:19" ht="12.45" customHeight="1">
+      <c r="P41" s="30"/>
+      <c r="Q41" s="45"/>
+      <c r="R41" s="45"/>
+    </row>
+    <row r="42" spans="1:18" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="40"/>
       <c r="B42" s="41"/>
       <c r="C42" s="42"/>
@@ -2651,34 +2643,19 @@
       <c r="H42" s="65"/>
       <c r="I42" s="66"/>
       <c r="J42" s="44" t="e">
-        <f t="shared" si="56"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K42" s="43" t="e">
-        <f t="shared" ref="K42" si="62">J42*(M42/L42)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L42" s="44" t="e">
-        <f t="shared" si="57"/>
-        <v>#DIV/0!</v>
-      </c>
+        <f>F42/$B$60</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K42" s="43"/>
+      <c r="L42" s="44"/>
       <c r="M42" s="68"/>
       <c r="N42" s="60"/>
       <c r="O42" s="60"/>
-      <c r="P42" s="30" t="e">
-        <f t="shared" si="58"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q42" s="45" t="e">
-        <f t="shared" si="59"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R42" s="45" t="e">
-        <f t="shared" si="60"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="43" spans="1:19" ht="12.45" customHeight="1">
+      <c r="P42" s="30"/>
+      <c r="Q42" s="45"/>
+      <c r="R42" s="45"/>
+    </row>
+    <row r="43" spans="1:18" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="40"/>
       <c r="B43" s="41"/>
       <c r="C43" s="42"/>
@@ -2688,7 +2665,10 @@
       <c r="G43" s="62"/>
       <c r="H43" s="65"/>
       <c r="I43" s="66"/>
-      <c r="J43" s="44"/>
+      <c r="J43" s="44" t="e">
+        <f>F43/$B$60</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="K43" s="43"/>
       <c r="L43" s="44"/>
       <c r="M43" s="68"/>
@@ -2698,7 +2678,7 @@
       <c r="Q43" s="45"/>
       <c r="R43" s="45"/>
     </row>
-    <row r="44" spans="1:19" ht="12.45" customHeight="1">
+    <row r="44" spans="1:18" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="40"/>
       <c r="B44" s="41"/>
       <c r="C44" s="42"/>
@@ -2709,34 +2689,19 @@
       <c r="H44" s="65"/>
       <c r="I44" s="66"/>
       <c r="J44" s="44" t="e">
-        <f t="shared" ref="J44" si="63">F44/$B$50</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K44" s="43" t="e">
-        <f t="shared" ref="K44" si="64">J44*(M44/L44)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L44" s="44" t="e">
-        <f t="shared" ref="L44" si="65">G44/$B$50</f>
-        <v>#DIV/0!</v>
-      </c>
+        <f>F44/$B$60</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K44" s="43"/>
+      <c r="L44" s="44"/>
       <c r="M44" s="68"/>
       <c r="N44" s="60"/>
       <c r="O44" s="60"/>
-      <c r="P44" s="30" t="e">
-        <f t="shared" ref="P44" si="66">I44/(J44*$B$51)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q44" s="45" t="e">
-        <f t="shared" ref="Q44" si="67">I44/((F44/$B$50*$B$51)*R44)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R44" s="45" t="e">
-        <f t="shared" ref="R44" si="68">H44/(L44*$B$51)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="45" spans="1:19" ht="12.45" customHeight="1">
+      <c r="P44" s="30"/>
+      <c r="Q44" s="45"/>
+      <c r="R44" s="45"/>
+    </row>
+    <row r="45" spans="1:18" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="40"/>
       <c r="B45" s="41"/>
       <c r="C45" s="42"/>
@@ -2746,7 +2711,10 @@
       <c r="G45" s="62"/>
       <c r="H45" s="65"/>
       <c r="I45" s="66"/>
-      <c r="J45" s="44"/>
+      <c r="J45" s="44" t="e">
+        <f>F45/$B$60</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="K45" s="43"/>
       <c r="L45" s="44"/>
       <c r="M45" s="68"/>
@@ -2756,7 +2724,7 @@
       <c r="Q45" s="45"/>
       <c r="R45" s="45"/>
     </row>
-    <row r="46" spans="1:19" ht="12.45" customHeight="1" thickBot="1">
+    <row r="46" spans="1:18" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="40"/>
       <c r="B46" s="41"/>
       <c r="C46" s="42"/>
@@ -2767,111 +2735,321 @@
       <c r="H46" s="65"/>
       <c r="I46" s="66"/>
       <c r="J46" s="44" t="e">
-        <f>F46/$B$50</f>
+        <f>F46/$B$60</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K46" s="43" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="13"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L46" s="44" t="e">
-        <f>G46/$B$50</f>
+        <f>G46/$B$60</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M46" s="68"/>
       <c r="N46" s="60"/>
       <c r="O46" s="60"/>
       <c r="P46" s="30" t="e">
-        <f>I46/(J46*$B$51)</f>
+        <f>I46/(J46*$B$61)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q46" s="45" t="e">
-        <f>I46/((F46/$B$50*$B$51)*R46)</f>
+        <f>I46/((F46/$B$60*$B$61)*R46)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R46" s="45" t="e">
-        <f>H46/(L46*$B$51)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="47" spans="1:19" ht="13.2" customHeight="1" thickBot="1">
-      <c r="A47" s="46"/>
-      <c r="B47" s="47" t="s">
+        <f>H46/(L46*$B$61)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="40"/>
+      <c r="B47" s="41"/>
+      <c r="C47" s="42"/>
+      <c r="D47" s="60"/>
+      <c r="E47" s="62"/>
+      <c r="F47" s="60"/>
+      <c r="G47" s="62"/>
+      <c r="H47" s="65"/>
+      <c r="I47" s="66"/>
+      <c r="J47" s="44" t="e">
+        <f>F47/$B$60</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K47" s="43" t="e">
+        <f t="shared" ref="K47" si="14">J47*(M47/L47)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L47" s="44" t="e">
+        <f>G47/$B$60</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M47" s="68"/>
+      <c r="N47" s="60"/>
+      <c r="O47" s="60"/>
+      <c r="P47" s="30" t="e">
+        <f>I47/(J47*$B$61)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q47" s="45" t="e">
+        <f>I47/((F47/$B$60*$B$61)*R47)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R47" s="45" t="e">
+        <f>H47/(L47*$B$61)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="40"/>
+      <c r="B48" s="41"/>
+      <c r="C48" s="42"/>
+      <c r="D48" s="60"/>
+      <c r="E48" s="62"/>
+      <c r="F48" s="60"/>
+      <c r="G48" s="62"/>
+      <c r="H48" s="65"/>
+      <c r="I48" s="66"/>
+      <c r="J48" s="44" t="e">
+        <f>F48/$B$60</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K48" s="43"/>
+      <c r="L48" s="44"/>
+      <c r="M48" s="68"/>
+      <c r="N48" s="60"/>
+      <c r="O48" s="60"/>
+      <c r="P48" s="30"/>
+      <c r="Q48" s="45"/>
+      <c r="R48" s="45"/>
+    </row>
+    <row r="49" spans="1:19" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="40"/>
+      <c r="B49" s="41"/>
+      <c r="C49" s="42"/>
+      <c r="D49" s="60"/>
+      <c r="E49" s="62"/>
+      <c r="F49" s="60"/>
+      <c r="G49" s="62"/>
+      <c r="H49" s="65"/>
+      <c r="I49" s="66"/>
+      <c r="J49" s="44" t="e">
+        <f>F49/$B$60</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K49" s="43"/>
+      <c r="L49" s="44"/>
+      <c r="M49" s="68"/>
+      <c r="N49" s="60"/>
+      <c r="O49" s="60"/>
+      <c r="P49" s="30"/>
+      <c r="Q49" s="45"/>
+      <c r="R49" s="45"/>
+    </row>
+    <row r="50" spans="1:19" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="40"/>
+      <c r="B50" s="41"/>
+      <c r="C50" s="42"/>
+      <c r="D50" s="60"/>
+      <c r="E50" s="62"/>
+      <c r="F50" s="60"/>
+      <c r="G50" s="62"/>
+      <c r="H50" s="65"/>
+      <c r="I50" s="66"/>
+      <c r="J50" s="44" t="e">
+        <f>F50/$B$60</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K50" s="43"/>
+      <c r="L50" s="44"/>
+      <c r="M50" s="68"/>
+      <c r="N50" s="60"/>
+      <c r="O50" s="60"/>
+      <c r="P50" s="30"/>
+      <c r="Q50" s="45"/>
+      <c r="R50" s="45"/>
+    </row>
+    <row r="51" spans="1:19" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="40"/>
+      <c r="B51" s="41"/>
+      <c r="C51" s="42"/>
+      <c r="D51" s="60"/>
+      <c r="E51" s="62"/>
+      <c r="F51" s="60"/>
+      <c r="G51" s="62"/>
+      <c r="H51" s="65"/>
+      <c r="I51" s="66"/>
+      <c r="J51" s="44" t="e">
+        <f>F51/$B$60</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K51" s="43" t="e">
+        <f t="shared" ref="K51:K54" si="15">J51*(M51/L51)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L51" s="44" t="e">
+        <f>G51/$B$60</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M51" s="68"/>
+      <c r="N51" s="60"/>
+      <c r="O51" s="60"/>
+      <c r="P51" s="30" t="e">
+        <f>I51/(J51*$B$61)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q51" s="45" t="e">
+        <f>I51/((F51/$B$60*$B$61)*R51)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R51" s="45" t="e">
+        <f>H51/(L51*$B$61)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="52" spans="1:19" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="40"/>
+      <c r="B52" s="41"/>
+      <c r="C52" s="42"/>
+      <c r="D52" s="60"/>
+      <c r="E52" s="62"/>
+      <c r="F52" s="60"/>
+      <c r="G52" s="62"/>
+      <c r="H52" s="65"/>
+      <c r="I52" s="66"/>
+      <c r="J52" s="44" t="e">
+        <f>F52/$B$60</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K52" s="43"/>
+      <c r="L52" s="44"/>
+      <c r="M52" s="68"/>
+      <c r="N52" s="60"/>
+      <c r="O52" s="60"/>
+      <c r="P52" s="30"/>
+      <c r="Q52" s="45"/>
+      <c r="R52" s="45"/>
+    </row>
+    <row r="53" spans="1:19" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="40"/>
+      <c r="B53" s="41"/>
+      <c r="C53" s="42"/>
+      <c r="D53" s="60"/>
+      <c r="E53" s="62"/>
+      <c r="F53" s="60"/>
+      <c r="G53" s="62"/>
+      <c r="H53" s="65"/>
+      <c r="I53" s="66"/>
+      <c r="J53" s="44" t="e">
+        <f>F53/$B$60</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K53" s="43" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L53" s="44" t="e">
+        <f>G53/$B$60</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M53" s="68"/>
+      <c r="N53" s="60"/>
+      <c r="O53" s="60"/>
+      <c r="P53" s="30" t="e">
+        <f>I53/(J53*$B$61)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q53" s="45" t="e">
+        <f>I53/((F53/$B$60*$B$61)*R53)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R53" s="45" t="e">
+        <f>H53/(L53*$B$61)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="54" spans="1:19" ht="13.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="46"/>
+      <c r="B54" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="C47" s="48"/>
-      <c r="D47" s="49">
-        <f t="shared" ref="D47:N47" si="69">SUM(D10:D46)</f>
+      <c r="C54" s="48"/>
+      <c r="D54" s="49">
+        <f t="shared" ref="D54:N54" si="16">SUM(D10:D53)</f>
         <v>0</v>
       </c>
-      <c r="E47" s="49">
-        <f t="shared" si="69"/>
+      <c r="E54" s="49">
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="F47" s="49">
-        <f t="shared" si="69"/>
+      <c r="F54" s="49">
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="G47" s="49">
-        <f t="shared" si="69"/>
+      <c r="G54" s="49">
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="H47" s="49">
-        <f t="shared" si="69"/>
+      <c r="H54" s="49">
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="I47" s="50">
-        <f t="shared" si="69"/>
+      <c r="I54" s="50">
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="J47" s="51" t="e">
-        <f t="shared" si="69"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K47" s="52" t="e">
-        <f t="shared" si="69"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L47" s="52" t="e">
-        <f t="shared" si="69"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M47" s="53">
-        <f t="shared" si="69"/>
+      <c r="J54" s="51" t="e">
+        <f t="shared" si="16"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K54" s="52" t="e">
+        <f t="shared" si="16"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L54" s="52" t="e">
+        <f t="shared" si="16"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M54" s="53">
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="N47" s="54">
-        <f t="shared" si="69"/>
+      <c r="N54" s="54">
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="O47" s="54"/>
-      <c r="P47" s="57" t="e">
-        <f>I47/(J47*$B$51)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q47" s="57" t="e">
-        <f>I47/((F47/$B$50*$B$51)*R47)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R47" s="57" t="e">
-        <f>H47/(L47*$B$51)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S47" s="58"/>
-    </row>
-    <row r="50" spans="1:3" ht="12.45" customHeight="1">
-      <c r="A50" s="56" t="s">
+      <c r="O54" s="54"/>
+      <c r="P54" s="57" t="e">
+        <f>I54/(J54*$B$61)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q54" s="57" t="e">
+        <f>I54/((F54/$B$60*$B$61)*R54)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R54" s="57" t="e">
+        <f>H54/(L54*$B$61)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S54" s="58"/>
+    </row>
+    <row r="57" spans="1:19" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C57" s="55"/>
+    </row>
+    <row r="58" spans="1:19" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C58" s="55"/>
+    </row>
+    <row r="60" spans="1:19" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="56" t="s">
         <v>25</v>
       </c>
-      <c r="B50" s="56"/>
-      <c r="C50" s="55"/>
-    </row>
-    <row r="51" spans="1:3" ht="12.45" customHeight="1">
-      <c r="A51" s="56" t="s">
+      <c r="B60" s="56"/>
+    </row>
+    <row r="61" spans="1:19" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="56" t="s">
         <v>26</v>
       </c>
-      <c r="B51" s="56"/>
-      <c r="C51" s="55"/>
+      <c r="B61" s="56"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
@@ -2892,8 +3070,8 @@
 &amp;I© 2017 SunEdison&amp;I &amp;C&amp;R&amp;"Arial"&amp;8 Page 1 of 2 </oddFooter>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="D47:H47 J10:L13 P10:R13 P47:R47 J47:N47" unlockedFormula="1"/>
-    <ignoredError sqref="I47" formula="1" unlockedFormula="1"/>
+    <ignoredError sqref="D54:H54 J10:L13 P10:R13 P54:R54 J54:N54" unlockedFormula="1"/>
+    <ignoredError sqref="I54" formula="1" unlockedFormula="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
change excel templates of daily/monthly report
</commit_message>
<xml_diff>
--- a/job/templates/DailyReport-v3.xlsx
+++ b/job/templates/DailyReport-v3.xlsx
@@ -1230,11 +1230,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S61"/>
+  <dimension ref="A1:S67"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.4" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1442,30 +1442,30 @@
       <c r="H10" s="63"/>
       <c r="I10" s="64"/>
       <c r="J10" s="39" t="e">
-        <f>F10/$B$60</f>
+        <f t="shared" ref="J10:J59" si="0">F10/$B$66</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K10" s="38" t="e">
-        <f t="shared" ref="K10:K53" si="0">J10*(M10/L10)</f>
+        <f t="shared" ref="K10:K59" si="1">J10*(M10/L10)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="L10" s="39" t="e">
-        <f>G10/$B$60</f>
+        <f t="shared" ref="L10:L52" si="2">G10/$B$66</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M10" s="67"/>
       <c r="N10" s="59"/>
       <c r="O10" s="59"/>
       <c r="P10" s="30" t="e">
-        <f>I10/(J10*$B$61)</f>
+        <f>I10/(J10*$B$67)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q10" s="33" t="e">
-        <f>I10/((J10*$B$61)*R10)</f>
+        <f>I10/((J10*$B$67)*R10)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R10" s="33" t="e">
-        <f>H10/(L10*$B$61)</f>
+        <f>H10/(L10*$B$67)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1480,30 +1480,30 @@
       <c r="H11" s="63"/>
       <c r="I11" s="64"/>
       <c r="J11" s="39" t="e">
-        <f>F11/$B$60</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K11" s="38" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L11" s="39" t="e">
-        <f>G11/$B$60</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M11" s="67"/>
       <c r="N11" s="59"/>
       <c r="O11" s="59"/>
       <c r="P11" s="30" t="e">
-        <f>I11/(J11*$B$61)</f>
+        <f>I11/(J11*$B$67)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q11" s="33" t="e">
-        <f>I11/((F11/$B$60*$B$61)*R11)</f>
+        <f>I11/((F11/$B$66*$B$67)*R11)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R11" s="33" t="e">
-        <f>H11/(L11*$B$61)</f>
+        <f>H11/(L11*$B$67)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1518,30 +1518,30 @@
       <c r="H12" s="63"/>
       <c r="I12" s="64"/>
       <c r="J12" s="39" t="e">
-        <f>F12/$B$60</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K12" s="38" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L12" s="39" t="e">
-        <f>G12/$B$60</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M12" s="67"/>
       <c r="N12" s="59"/>
       <c r="O12" s="59"/>
       <c r="P12" s="30" t="e">
-        <f>I12/(J12*$B$61)</f>
+        <f>I12/(J12*$B$67)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q12" s="33" t="e">
-        <f>I12/((F12/$B$60*$B$61)*R12)</f>
+        <f>I12/((F12/$B$66*$B$67)*R12)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R12" s="33" t="e">
-        <f>H12/(L12*$B$61)</f>
+        <f>H12/(L12*$B$67)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1556,30 +1556,30 @@
       <c r="H13" s="63"/>
       <c r="I13" s="64"/>
       <c r="J13" s="39" t="e">
-        <f>F13/$B$60</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K13" s="38" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L13" s="39" t="e">
-        <f>G13/$B$60</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M13" s="67"/>
       <c r="N13" s="59"/>
       <c r="O13" s="59"/>
       <c r="P13" s="30" t="e">
-        <f>I13/(J13*$B$61)</f>
+        <f>I13/(J13*$B$67)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q13" s="33" t="e">
-        <f>I13/((F13/$B$60*$B$61)*R13)</f>
+        <f>I13/((F13/$B$66*$B$67)*R13)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R13" s="33" t="e">
-        <f>H13/(L13*$B$61)</f>
+        <f>H13/(L13*$B$67)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1594,30 +1594,30 @@
       <c r="H14" s="65"/>
       <c r="I14" s="66"/>
       <c r="J14" s="44" t="e">
-        <f>F14/$B$60</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K14" s="43" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L14" s="44" t="e">
-        <f>G14/$B$60</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M14" s="68"/>
       <c r="N14" s="60"/>
       <c r="O14" s="60"/>
       <c r="P14" s="30" t="e">
-        <f>I14/(J14*$B$61)</f>
+        <f>I14/(J14*$B$67)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q14" s="45" t="e">
-        <f>I14/((F14/$B$60*$B$61)*R14)</f>
+        <f>I14/((F14/$B$66*$B$67)*R14)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R14" s="45" t="e">
-        <f>H14/(L14*$B$61)</f>
+        <f>H14/(L14*$B$67)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1632,30 +1632,30 @@
       <c r="H15" s="65"/>
       <c r="I15" s="66"/>
       <c r="J15" s="44" t="e">
-        <f>F15/$B$60</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K15" s="43" t="e">
-        <f t="shared" ref="K15:K16" si="1">J15*(M15/L15)</f>
+        <f t="shared" ref="K15:K16" si="3">J15*(M15/L15)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="L15" s="44" t="e">
-        <f>G15/$B$60</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M15" s="68"/>
       <c r="N15" s="60"/>
       <c r="O15" s="60"/>
       <c r="P15" s="30" t="e">
-        <f>I15/(J15*$B$61)</f>
+        <f>I15/(J15*$B$67)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q15" s="45" t="e">
-        <f>I15/((F15/$B$60*$B$61)*R15)</f>
+        <f>I15/((F15/$B$66*$B$67)*R15)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R15" s="45" t="e">
-        <f>H15/(L15*$B$61)</f>
+        <f>H15/(L15*$B$67)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1670,30 +1670,30 @@
       <c r="H16" s="65"/>
       <c r="I16" s="66"/>
       <c r="J16" s="44" t="e">
-        <f>F16/$B$60</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K16" s="43" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L16" s="44" t="e">
-        <f>G16/$B$60</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M16" s="68"/>
       <c r="N16" s="60"/>
       <c r="O16" s="60"/>
       <c r="P16" s="30" t="e">
-        <f>I16/(J16*$B$61)</f>
+        <f>I16/(J16*$B$67)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q16" s="45" t="e">
-        <f>I16/((F16/$B$60*$B$61)*R16)</f>
+        <f>I16/((F16/$B$66*$B$67)*R16)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R16" s="45" t="e">
-        <f>H16/(L16*$B$61)</f>
+        <f>H16/(L16*$B$67)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1708,30 +1708,30 @@
       <c r="H17" s="65"/>
       <c r="I17" s="66"/>
       <c r="J17" s="44" t="e">
-        <f>F17/$B$60</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K17" s="43" t="e">
-        <f t="shared" ref="K17" si="2">J17*(M17/L17)</f>
+        <f t="shared" ref="K17" si="4">J17*(M17/L17)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="L17" s="44" t="e">
-        <f>G17/$B$60</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M17" s="68"/>
       <c r="N17" s="60"/>
       <c r="O17" s="60"/>
       <c r="P17" s="30" t="e">
-        <f>I17/(J17*$B$61)</f>
+        <f>I17/(J17*$B$67)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q17" s="45" t="e">
-        <f>I17/((F17/$B$60*$B$61)*R17)</f>
+        <f>I17/((F17/$B$66*$B$67)*R17)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R17" s="45" t="e">
-        <f>H17/(L17*$B$61)</f>
+        <f>H17/(L17*$B$67)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1746,30 +1746,30 @@
       <c r="H18" s="65"/>
       <c r="I18" s="66"/>
       <c r="J18" s="44" t="e">
-        <f>F18/$B$60</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K18" s="43" t="e">
-        <f t="shared" ref="K18" si="3">J18*(M18/L18)</f>
+        <f t="shared" ref="K18" si="5">J18*(M18/L18)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="L18" s="44" t="e">
-        <f>G18/$B$60</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M18" s="68"/>
       <c r="N18" s="60"/>
       <c r="O18" s="60"/>
       <c r="P18" s="30" t="e">
-        <f>I18/(J18*$B$61)</f>
+        <f>I18/(J18*$B$67)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q18" s="45" t="e">
-        <f>I18/((F18/$B$60*$B$61)*R18)</f>
+        <f>I18/((F18/$B$66*$B$67)*R18)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R18" s="45" t="e">
-        <f>H18/(L18*$B$61)</f>
+        <f>H18/(L18*$B$67)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1784,30 +1784,30 @@
       <c r="H19" s="65"/>
       <c r="I19" s="66"/>
       <c r="J19" s="44" t="e">
-        <f>F19/$B$60</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K19" s="43" t="e">
-        <f t="shared" ref="K19:K26" si="4">J19*(M19/L19)</f>
+        <f t="shared" ref="K19:K26" si="6">J19*(M19/L19)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="L19" s="44" t="e">
-        <f>G19/$B$60</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M19" s="68"/>
       <c r="N19" s="60"/>
       <c r="O19" s="60"/>
       <c r="P19" s="30" t="e">
-        <f>I19/(J19*$B$61)</f>
+        <f>I19/(J19*$B$67)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q19" s="45" t="e">
-        <f>I19/((F19/$B$60*$B$61)*R19)</f>
+        <f>I19/((F19/$B$66*$B$67)*R19)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R19" s="45" t="e">
-        <f>H19/(L19*$B$61)</f>
+        <f>H19/(L19*$B$67)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1822,30 +1822,30 @@
       <c r="H20" s="65"/>
       <c r="I20" s="66"/>
       <c r="J20" s="44" t="e">
-        <f>F20/$B$60</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K20" s="43" t="e">
-        <f t="shared" ref="K20" si="5">J20*(M20/L20)</f>
+        <f t="shared" ref="K20" si="7">J20*(M20/L20)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="L20" s="44" t="e">
-        <f>G20/$B$60</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M20" s="68"/>
       <c r="N20" s="60"/>
       <c r="O20" s="60"/>
       <c r="P20" s="30" t="e">
-        <f>I20/(J20*$B$61)</f>
+        <f>I20/(J20*$B$67)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q20" s="45" t="e">
-        <f>I20/((F20/$B$60*$B$61)*R20)</f>
+        <f>I20/((F20/$B$66*$B$67)*R20)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R20" s="45" t="e">
-        <f>H20/(L20*$B$61)</f>
+        <f>H20/(L20*$B$67)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1860,30 +1860,30 @@
       <c r="H21" s="65"/>
       <c r="I21" s="66"/>
       <c r="J21" s="44" t="e">
-        <f>F21/$B$60</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K21" s="43" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L21" s="44" t="e">
-        <f>G21/$B$60</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M21" s="68"/>
       <c r="N21" s="60"/>
       <c r="O21" s="60"/>
       <c r="P21" s="30" t="e">
-        <f>I21/(J21*$B$61)</f>
+        <f>I21/(J21*$B$67)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q21" s="45" t="e">
-        <f>I21/((F21/$B$60*$B$61)*R21)</f>
+        <f>I21/((F21/$B$66*$B$67)*R21)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R21" s="45" t="e">
-        <f>H21/(L21*$B$61)</f>
+        <f>H21/(L21*$B$67)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1898,30 +1898,30 @@
       <c r="H22" s="65"/>
       <c r="I22" s="66"/>
       <c r="J22" s="44" t="e">
-        <f>F22/$B$60</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K22" s="43" t="e">
-        <f t="shared" ref="K22:K23" si="6">J22*(M22/L22)</f>
+        <f t="shared" ref="K22:K23" si="8">J22*(M22/L22)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="L22" s="44" t="e">
-        <f>G22/$B$60</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M22" s="68"/>
       <c r="N22" s="60"/>
       <c r="O22" s="60"/>
       <c r="P22" s="30" t="e">
-        <f>I22/(J22*$B$61)</f>
+        <f>I22/(J22*$B$67)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q22" s="45" t="e">
-        <f>I22/((F22/$B$60*$B$61)*R22)</f>
+        <f>I22/((F22/$B$66*$B$67)*R22)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R22" s="45" t="e">
-        <f>H22/(L22*$B$61)</f>
+        <f>H22/(L22*$B$67)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1936,30 +1936,30 @@
       <c r="H23" s="65"/>
       <c r="I23" s="66"/>
       <c r="J23" s="44" t="e">
-        <f>F23/$B$60</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K23" s="43" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L23" s="44" t="e">
-        <f>G23/$B$60</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M23" s="68"/>
       <c r="N23" s="60"/>
       <c r="O23" s="60"/>
       <c r="P23" s="30" t="e">
-        <f>I23/(J23*$B$61)</f>
+        <f>I23/(J23*$B$67)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q23" s="45" t="e">
-        <f>I23/((F23/$B$60*$B$61)*R23)</f>
+        <f>I23/((F23/$B$66*$B$67)*R23)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R23" s="45" t="e">
-        <f>H23/(L23*$B$61)</f>
+        <f>H23/(L23*$B$67)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1974,30 +1974,30 @@
       <c r="H24" s="65"/>
       <c r="I24" s="66"/>
       <c r="J24" s="44" t="e">
-        <f>F24/$B$60</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K24" s="43" t="e">
-        <f t="shared" ref="K24" si="7">J24*(M24/L24)</f>
+        <f t="shared" ref="K24" si="9">J24*(M24/L24)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="L24" s="44" t="e">
-        <f>G24/$B$60</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M24" s="68"/>
       <c r="N24" s="60"/>
       <c r="O24" s="60"/>
       <c r="P24" s="30" t="e">
-        <f>I24/(J24*$B$61)</f>
+        <f>I24/(J24*$B$67)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q24" s="45" t="e">
-        <f>I24/((F24/$B$60*$B$61)*R24)</f>
+        <f>I24/((F24/$B$66*$B$67)*R24)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R24" s="45" t="e">
-        <f>H24/(L24*$B$61)</f>
+        <f>H24/(L24*$B$67)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2012,30 +2012,30 @@
       <c r="H25" s="65"/>
       <c r="I25" s="66"/>
       <c r="J25" s="44" t="e">
-        <f>F25/$B$60</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K25" s="43" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L25" s="44" t="e">
-        <f>G25/$B$60</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M25" s="68"/>
       <c r="N25" s="60"/>
       <c r="O25" s="60"/>
       <c r="P25" s="30" t="e">
-        <f>I25/(J25*$B$61)</f>
+        <f>I25/(J25*$B$67)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q25" s="45" t="e">
-        <f>I25/((F25/$B$60*$B$61)*R25)</f>
+        <f>I25/((F25/$B$66*$B$67)*R25)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R25" s="45" t="e">
-        <f>H25/(L25*$B$61)</f>
+        <f>H25/(L25*$B$67)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2050,30 +2050,30 @@
       <c r="H26" s="65"/>
       <c r="I26" s="66"/>
       <c r="J26" s="44" t="e">
-        <f>F26/$B$60</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K26" s="43" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L26" s="44" t="e">
-        <f>G26/$B$60</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M26" s="68"/>
       <c r="N26" s="60"/>
       <c r="O26" s="60"/>
       <c r="P26" s="30" t="e">
-        <f>I26/(J26*$B$61)</f>
+        <f>I26/(J26*$B$67)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q26" s="45" t="e">
-        <f>I26/((F26/$B$60*$B$61)*R26)</f>
+        <f>I26/((F26/$B$66*$B$67)*R26)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R26" s="45" t="e">
-        <f>H26/(L26*$B$61)</f>
+        <f>H26/(L26*$B$67)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2088,30 +2088,30 @@
       <c r="H27" s="65"/>
       <c r="I27" s="66"/>
       <c r="J27" s="44" t="e">
-        <f>F27/$B$60</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K27" s="43" t="e">
-        <f t="shared" ref="K27:K29" si="8">J27*(M27/L27)</f>
+        <f t="shared" ref="K27:K29" si="10">J27*(M27/L27)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="L27" s="44" t="e">
-        <f>G27/$B$60</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M27" s="68"/>
       <c r="N27" s="60"/>
       <c r="O27" s="60"/>
       <c r="P27" s="30" t="e">
-        <f>I27/(J27*$B$61)</f>
+        <f>I27/(J27*$B$67)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q27" s="45" t="e">
-        <f>I27/((F27/$B$60*$B$61)*R27)</f>
+        <f>I27/((F27/$B$66*$B$67)*R27)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R27" s="45" t="e">
-        <f>H27/(L27*$B$61)</f>
+        <f>H27/(L27*$B$67)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2126,30 +2126,30 @@
       <c r="H28" s="65"/>
       <c r="I28" s="66"/>
       <c r="J28" s="44" t="e">
-        <f>F28/$B$60</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K28" s="43" t="e">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L28" s="44" t="e">
-        <f>G28/$B$60</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M28" s="68"/>
       <c r="N28" s="60"/>
       <c r="O28" s="60"/>
       <c r="P28" s="30" t="e">
-        <f>I28/(J28*$B$61)</f>
+        <f>I28/(J28*$B$67)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q28" s="45" t="e">
-        <f>I28/((F28/$B$60*$B$61)*R28)</f>
+        <f>I28/((F28/$B$66*$B$67)*R28)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R28" s="45" t="e">
-        <f>H28/(L28*$B$61)</f>
+        <f>H28/(L28*$B$67)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2164,30 +2164,30 @@
       <c r="H29" s="65"/>
       <c r="I29" s="66"/>
       <c r="J29" s="44" t="e">
-        <f>F29/$B$60</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K29" s="43" t="e">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L29" s="44" t="e">
-        <f>G29/$B$60</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M29" s="68"/>
       <c r="N29" s="60"/>
       <c r="O29" s="60"/>
       <c r="P29" s="30" t="e">
-        <f>I29/(J29*$B$61)</f>
+        <f>I29/(J29*$B$67)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q29" s="45" t="e">
-        <f>I29/((F29/$B$60*$B$61)*R29)</f>
+        <f>I29/((F29/$B$66*$B$67)*R29)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R29" s="45" t="e">
-        <f>H29/(L29*$B$61)</f>
+        <f>H29/(L29*$B$67)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2202,30 +2202,30 @@
       <c r="H30" s="65"/>
       <c r="I30" s="66"/>
       <c r="J30" s="44" t="e">
-        <f>F30/$B$60</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K30" s="43" t="e">
-        <f t="shared" ref="K30:K32" si="9">J30*(M30/L30)</f>
+        <f t="shared" ref="K30:K32" si="11">J30*(M30/L30)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="L30" s="44" t="e">
-        <f>G30/$B$60</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M30" s="68"/>
       <c r="N30" s="60"/>
       <c r="O30" s="60"/>
       <c r="P30" s="30" t="e">
-        <f>I30/(J30*$B$61)</f>
+        <f>I30/(J30*$B$67)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q30" s="45" t="e">
-        <f>I30/((F30/$B$60*$B$61)*R30)</f>
+        <f>I30/((F30/$B$66*$B$67)*R30)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R30" s="45" t="e">
-        <f>H30/(L30*$B$61)</f>
+        <f>H30/(L30*$B$67)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2240,30 +2240,30 @@
       <c r="H31" s="65"/>
       <c r="I31" s="66"/>
       <c r="J31" s="44" t="e">
-        <f>F31/$B$60</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K31" s="43" t="e">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L31" s="44" t="e">
-        <f>G31/$B$60</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M31" s="68"/>
       <c r="N31" s="60"/>
       <c r="O31" s="60"/>
       <c r="P31" s="30" t="e">
-        <f>I31/(J31*$B$61)</f>
+        <f>I31/(J31*$B$67)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q31" s="45" t="e">
-        <f>I31/((F31/$B$60*$B$61)*R31)</f>
+        <f>I31/((F31/$B$66*$B$67)*R31)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R31" s="45" t="e">
-        <f>H31/(L31*$B$61)</f>
+        <f>H31/(L31*$B$67)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2278,30 +2278,30 @@
       <c r="H32" s="65"/>
       <c r="I32" s="66"/>
       <c r="J32" s="44" t="e">
-        <f>F32/$B$60</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K32" s="43" t="e">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L32" s="44" t="e">
-        <f>G32/$B$60</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M32" s="68"/>
       <c r="N32" s="60"/>
       <c r="O32" s="60"/>
       <c r="P32" s="30" t="e">
-        <f>I32/(J32*$B$61)</f>
+        <f>I32/(J32*$B$67)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q32" s="45" t="e">
-        <f>I32/((F32/$B$60*$B$61)*R32)</f>
+        <f>I32/((F32/$B$66*$B$67)*R32)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R32" s="45" t="e">
-        <f>H32/(L32*$B$61)</f>
+        <f>H32/(L32*$B$67)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2316,30 +2316,30 @@
       <c r="H33" s="65"/>
       <c r="I33" s="66"/>
       <c r="J33" s="44" t="e">
-        <f>F33/$B$60</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K33" s="43" t="e">
-        <f t="shared" ref="K33" si="10">J33*(M33/L33)</f>
+        <f t="shared" ref="K33" si="12">J33*(M33/L33)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="L33" s="44" t="e">
-        <f>G33/$B$60</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M33" s="68"/>
       <c r="N33" s="60"/>
       <c r="O33" s="60"/>
       <c r="P33" s="30" t="e">
-        <f>I33/(J33*$B$61)</f>
+        <f>I33/(J33*$B$67)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q33" s="45" t="e">
-        <f>I33/((F33/$B$60*$B$61)*R33)</f>
+        <f>I33/((F33/$B$66*$B$67)*R33)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R33" s="45" t="e">
-        <f>H33/(L33*$B$61)</f>
+        <f>H33/(L33*$B$67)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2354,30 +2354,30 @@
       <c r="H34" s="65"/>
       <c r="I34" s="66"/>
       <c r="J34" s="44" t="e">
-        <f>F34/$B$60</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K34" s="43" t="e">
-        <f t="shared" ref="K34" si="11">J34*(M34/L34)</f>
+        <f t="shared" ref="K34" si="13">J34*(M34/L34)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="L34" s="44" t="e">
-        <f>G34/$B$60</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M34" s="68"/>
       <c r="N34" s="60"/>
       <c r="O34" s="60"/>
       <c r="P34" s="30" t="e">
-        <f>I34/(J34*$B$61)</f>
+        <f>I34/(J34*$B$67)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q34" s="45" t="e">
-        <f>I34/((F34/$B$60*$B$61)*R34)</f>
+        <f>I34/((F34/$B$66*$B$67)*R34)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R34" s="45" t="e">
-        <f>H34/(L34*$B$61)</f>
+        <f>H34/(L34*$B$67)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2392,30 +2392,30 @@
       <c r="H35" s="65"/>
       <c r="I35" s="66"/>
       <c r="J35" s="44" t="e">
-        <f>F35/$B$60</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K35" s="43" t="e">
-        <f t="shared" ref="K35:K39" si="12">J35*(M35/L35)</f>
+        <f t="shared" ref="K35:K39" si="14">J35*(M35/L35)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="L35" s="44" t="e">
-        <f>G35/$B$60</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M35" s="68"/>
       <c r="N35" s="60"/>
       <c r="O35" s="60"/>
       <c r="P35" s="30" t="e">
-        <f>I35/(J35*$B$61)</f>
+        <f>I35/(J35*$B$67)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q35" s="45" t="e">
-        <f>I35/((F35/$B$60*$B$61)*R35)</f>
+        <f>I35/((F35/$B$66*$B$67)*R35)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R35" s="45" t="e">
-        <f>H35/(L35*$B$61)</f>
+        <f>H35/(L35*$B$67)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2430,30 +2430,30 @@
       <c r="H36" s="65"/>
       <c r="I36" s="66"/>
       <c r="J36" s="44" t="e">
-        <f>F36/$B$60</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K36" s="43" t="e">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L36" s="44" t="e">
-        <f>G36/$B$60</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M36" s="68"/>
       <c r="N36" s="60"/>
       <c r="O36" s="60"/>
       <c r="P36" s="30" t="e">
-        <f>I36/(J36*$B$61)</f>
+        <f>I36/(J36*$B$67)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q36" s="45" t="e">
-        <f>I36/((F36/$B$60*$B$61)*R36)</f>
+        <f>I36/((F36/$B$66*$B$67)*R36)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R36" s="45" t="e">
-        <f>H36/(L36*$B$61)</f>
+        <f>H36/(L36*$B$67)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2468,30 +2468,30 @@
       <c r="H37" s="65"/>
       <c r="I37" s="66"/>
       <c r="J37" s="44" t="e">
-        <f>F37/$B$60</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K37" s="43" t="e">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L37" s="44" t="e">
-        <f>G37/$B$60</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M37" s="68"/>
       <c r="N37" s="60"/>
       <c r="O37" s="60"/>
       <c r="P37" s="30" t="e">
-        <f>I37/(J37*$B$61)</f>
+        <f>I37/(J37*$B$67)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q37" s="45" t="e">
-        <f>I37/((F37/$B$60*$B$61)*R37)</f>
+        <f>I37/((F37/$B$66*$B$67)*R37)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R37" s="45" t="e">
-        <f>H37/(L37*$B$61)</f>
+        <f>H37/(L37*$B$67)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2506,30 +2506,30 @@
       <c r="H38" s="65"/>
       <c r="I38" s="66"/>
       <c r="J38" s="44" t="e">
-        <f>F38/$B$60</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K38" s="43" t="e">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L38" s="44" t="e">
-        <f>G38/$B$60</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M38" s="68"/>
       <c r="N38" s="60"/>
       <c r="O38" s="60"/>
       <c r="P38" s="30" t="e">
-        <f>I38/(J38*$B$61)</f>
+        <f>I38/(J38*$B$67)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q38" s="45" t="e">
-        <f>I38/((F38/$B$60*$B$61)*R38)</f>
+        <f>I38/((F38/$B$66*$B$67)*R38)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R38" s="45" t="e">
-        <f>H38/(L38*$B$61)</f>
+        <f>H38/(L38*$B$67)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2544,30 +2544,30 @@
       <c r="H39" s="65"/>
       <c r="I39" s="66"/>
       <c r="J39" s="44" t="e">
-        <f>F39/$B$60</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K39" s="43" t="e">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L39" s="44" t="e">
-        <f>G39/$B$60</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M39" s="68"/>
       <c r="N39" s="60"/>
       <c r="O39" s="60"/>
       <c r="P39" s="30" t="e">
-        <f>I39/(J39*$B$61)</f>
+        <f>I39/(J39*$B$67)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q39" s="45" t="e">
-        <f>I39/((F39/$B$60*$B$61)*R39)</f>
+        <f>I39/((F39/$B$66*$B$67)*R39)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R39" s="45" t="e">
-        <f>H39/(L39*$B$61)</f>
+        <f>H39/(L39*$B$67)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2582,30 +2582,30 @@
       <c r="H40" s="65"/>
       <c r="I40" s="66"/>
       <c r="J40" s="44" t="e">
-        <f>F40/$B$60</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K40" s="43" t="e">
-        <f t="shared" ref="K40:K46" si="13">J40*(M40/L40)</f>
+        <f t="shared" ref="K40:K52" si="15">J40*(M40/L40)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="L40" s="44" t="e">
-        <f>G40/$B$60</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M40" s="68"/>
       <c r="N40" s="60"/>
       <c r="O40" s="60"/>
       <c r="P40" s="30" t="e">
-        <f>I40/(J40*$B$61)</f>
+        <f>I40/(J40*$B$67)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q40" s="45" t="e">
-        <f>I40/((F40/$B$60*$B$61)*R40)</f>
+        <f>I40/((F40/$B$66*$B$67)*R40)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R40" s="45" t="e">
-        <f>H40/(L40*$B$61)</f>
+        <f>H40/(L40*$B$67)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2620,17 +2620,32 @@
       <c r="H41" s="65"/>
       <c r="I41" s="66"/>
       <c r="J41" s="44" t="e">
-        <f>F41/$B$60</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K41" s="43"/>
-      <c r="L41" s="44"/>
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K41" s="43" t="e">
+        <f t="shared" si="15"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L41" s="44" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
       <c r="M41" s="68"/>
       <c r="N41" s="60"/>
       <c r="O41" s="60"/>
-      <c r="P41" s="30"/>
-      <c r="Q41" s="45"/>
-      <c r="R41" s="45"/>
+      <c r="P41" s="30" t="e">
+        <f>I41/(J41*$B$67)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q41" s="45" t="e">
+        <f>I41/((F41/$B$66*$B$67)*R41)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R41" s="45" t="e">
+        <f>H41/(L41*$B$67)</f>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="42" spans="1:18" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="40"/>
@@ -2643,17 +2658,32 @@
       <c r="H42" s="65"/>
       <c r="I42" s="66"/>
       <c r="J42" s="44" t="e">
-        <f>F42/$B$60</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K42" s="43"/>
-      <c r="L42" s="44"/>
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K42" s="43" t="e">
+        <f t="shared" si="15"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L42" s="44" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
       <c r="M42" s="68"/>
       <c r="N42" s="60"/>
       <c r="O42" s="60"/>
-      <c r="P42" s="30"/>
-      <c r="Q42" s="45"/>
-      <c r="R42" s="45"/>
+      <c r="P42" s="30" t="e">
+        <f>I42/(J42*$B$67)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q42" s="45" t="e">
+        <f>I42/((F42/$B$66*$B$67)*R42)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R42" s="45" t="e">
+        <f>H42/(L42*$B$67)</f>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="43" spans="1:18" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="40"/>
@@ -2666,17 +2696,32 @@
       <c r="H43" s="65"/>
       <c r="I43" s="66"/>
       <c r="J43" s="44" t="e">
-        <f>F43/$B$60</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K43" s="43"/>
-      <c r="L43" s="44"/>
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K43" s="43" t="e">
+        <f t="shared" si="15"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L43" s="44" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
       <c r="M43" s="68"/>
       <c r="N43" s="60"/>
       <c r="O43" s="60"/>
-      <c r="P43" s="30"/>
-      <c r="Q43" s="45"/>
-      <c r="R43" s="45"/>
+      <c r="P43" s="30" t="e">
+        <f>I43/(J43*$B$67)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q43" s="45" t="e">
+        <f>I43/((F43/$B$66*$B$67)*R43)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R43" s="45" t="e">
+        <f>H43/(L43*$B$67)</f>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="44" spans="1:18" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="40"/>
@@ -2689,17 +2734,32 @@
       <c r="H44" s="65"/>
       <c r="I44" s="66"/>
       <c r="J44" s="44" t="e">
-        <f>F44/$B$60</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K44" s="43"/>
-      <c r="L44" s="44"/>
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K44" s="43" t="e">
+        <f t="shared" si="15"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L44" s="44" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
       <c r="M44" s="68"/>
       <c r="N44" s="60"/>
       <c r="O44" s="60"/>
-      <c r="P44" s="30"/>
-      <c r="Q44" s="45"/>
-      <c r="R44" s="45"/>
+      <c r="P44" s="30" t="e">
+        <f>I44/(J44*$B$67)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q44" s="45" t="e">
+        <f>I44/((F44/$B$66*$B$67)*R44)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R44" s="45" t="e">
+        <f>H44/(L44*$B$67)</f>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="45" spans="1:18" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="40"/>
@@ -2712,17 +2772,32 @@
       <c r="H45" s="65"/>
       <c r="I45" s="66"/>
       <c r="J45" s="44" t="e">
-        <f>F45/$B$60</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K45" s="43"/>
-      <c r="L45" s="44"/>
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K45" s="43" t="e">
+        <f t="shared" si="15"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L45" s="44" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
       <c r="M45" s="68"/>
       <c r="N45" s="60"/>
       <c r="O45" s="60"/>
-      <c r="P45" s="30"/>
-      <c r="Q45" s="45"/>
-      <c r="R45" s="45"/>
+      <c r="P45" s="30" t="e">
+        <f>I45/(J45*$B$67)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q45" s="45" t="e">
+        <f>I45/((F45/$B$66*$B$67)*R45)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R45" s="45" t="e">
+        <f>H45/(L45*$B$67)</f>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="46" spans="1:18" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="40"/>
@@ -2735,30 +2810,30 @@
       <c r="H46" s="65"/>
       <c r="I46" s="66"/>
       <c r="J46" s="44" t="e">
-        <f>F46/$B$60</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K46" s="43" t="e">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L46" s="44" t="e">
-        <f>G46/$B$60</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M46" s="68"/>
       <c r="N46" s="60"/>
       <c r="O46" s="60"/>
       <c r="P46" s="30" t="e">
-        <f>I46/(J46*$B$61)</f>
+        <f>I46/(J46*$B$67)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q46" s="45" t="e">
-        <f>I46/((F46/$B$60*$B$61)*R46)</f>
+        <f>I46/((F46/$B$66*$B$67)*R46)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R46" s="45" t="e">
-        <f>H46/(L46*$B$61)</f>
+        <f>H46/(L46*$B$67)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2773,30 +2848,30 @@
       <c r="H47" s="65"/>
       <c r="I47" s="66"/>
       <c r="J47" s="44" t="e">
-        <f>F47/$B$60</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K47" s="43" t="e">
-        <f t="shared" ref="K47" si="14">J47*(M47/L47)</f>
+        <f t="shared" si="15"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L47" s="44" t="e">
-        <f>G47/$B$60</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M47" s="68"/>
       <c r="N47" s="60"/>
       <c r="O47" s="60"/>
       <c r="P47" s="30" t="e">
-        <f>I47/(J47*$B$61)</f>
+        <f>I47/(J47*$B$67)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q47" s="45" t="e">
-        <f>I47/((F47/$B$60*$B$61)*R47)</f>
+        <f>I47/((F47/$B$66*$B$67)*R47)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R47" s="45" t="e">
-        <f>H47/(L47*$B$61)</f>
+        <f>H47/(L47*$B$67)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2811,17 +2886,32 @@
       <c r="H48" s="65"/>
       <c r="I48" s="66"/>
       <c r="J48" s="44" t="e">
-        <f>F48/$B$60</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K48" s="43"/>
-      <c r="L48" s="44"/>
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K48" s="43" t="e">
+        <f t="shared" si="15"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L48" s="44" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
       <c r="M48" s="68"/>
       <c r="N48" s="60"/>
       <c r="O48" s="60"/>
-      <c r="P48" s="30"/>
-      <c r="Q48" s="45"/>
-      <c r="R48" s="45"/>
+      <c r="P48" s="30" t="e">
+        <f>I48/(J48*$B$67)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q48" s="45" t="e">
+        <f>I48/((F48/$B$66*$B$67)*R48)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R48" s="45" t="e">
+        <f>H48/(L48*$B$67)</f>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="49" spans="1:19" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="40"/>
@@ -2834,17 +2924,32 @@
       <c r="H49" s="65"/>
       <c r="I49" s="66"/>
       <c r="J49" s="44" t="e">
-        <f>F49/$B$60</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K49" s="43"/>
-      <c r="L49" s="44"/>
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K49" s="43" t="e">
+        <f t="shared" si="15"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L49" s="44" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
       <c r="M49" s="68"/>
       <c r="N49" s="60"/>
       <c r="O49" s="60"/>
-      <c r="P49" s="30"/>
-      <c r="Q49" s="45"/>
-      <c r="R49" s="45"/>
+      <c r="P49" s="30" t="e">
+        <f>I49/(J49*$B$67)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q49" s="45" t="e">
+        <f>I49/((F49/$B$66*$B$67)*R49)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R49" s="45" t="e">
+        <f>H49/(L49*$B$67)</f>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="50" spans="1:19" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="40"/>
@@ -2857,17 +2962,32 @@
       <c r="H50" s="65"/>
       <c r="I50" s="66"/>
       <c r="J50" s="44" t="e">
-        <f>F50/$B$60</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K50" s="43"/>
-      <c r="L50" s="44"/>
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K50" s="43" t="e">
+        <f t="shared" si="15"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L50" s="44" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
       <c r="M50" s="68"/>
       <c r="N50" s="60"/>
       <c r="O50" s="60"/>
-      <c r="P50" s="30"/>
-      <c r="Q50" s="45"/>
-      <c r="R50" s="45"/>
+      <c r="P50" s="30" t="e">
+        <f>I50/(J50*$B$67)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q50" s="45" t="e">
+        <f>I50/((F50/$B$66*$B$67)*R50)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R50" s="45" t="e">
+        <f>H50/(L50*$B$67)</f>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="51" spans="1:19" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="40"/>
@@ -2880,30 +3000,30 @@
       <c r="H51" s="65"/>
       <c r="I51" s="66"/>
       <c r="J51" s="44" t="e">
-        <f>F51/$B$60</f>
+        <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K51" s="43" t="e">
-        <f t="shared" ref="K51:K54" si="15">J51*(M51/L51)</f>
+        <f t="shared" si="15"/>
         <v>#DIV/0!</v>
       </c>
       <c r="L51" s="44" t="e">
-        <f>G51/$B$60</f>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="M51" s="68"/>
       <c r="N51" s="60"/>
       <c r="O51" s="60"/>
       <c r="P51" s="30" t="e">
-        <f>I51/(J51*$B$61)</f>
+        <f>I51/(J51*$B$67)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q51" s="45" t="e">
-        <f>I51/((F51/$B$60*$B$61)*R51)</f>
+        <f>I51/((F51/$B$66*$B$67)*R51)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R51" s="45" t="e">
-        <f>H51/(L51*$B$61)</f>
+        <f>H51/(L51*$B$67)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2918,19 +3038,34 @@
       <c r="H52" s="65"/>
       <c r="I52" s="66"/>
       <c r="J52" s="44" t="e">
-        <f>F52/$B$60</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K52" s="43"/>
-      <c r="L52" s="44"/>
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K52" s="43" t="e">
+        <f t="shared" si="15"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L52" s="44" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
       <c r="M52" s="68"/>
       <c r="N52" s="60"/>
       <c r="O52" s="60"/>
-      <c r="P52" s="30"/>
-      <c r="Q52" s="45"/>
-      <c r="R52" s="45"/>
-    </row>
-    <row r="53" spans="1:19" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="P52" s="30" t="e">
+        <f>I52/(J52*$B$67)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q52" s="45" t="e">
+        <f>I52/((F52/$B$66*$B$67)*R52)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R52" s="45" t="e">
+        <f>H52/(L52*$B$67)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="53" spans="1:19" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="40"/>
       <c r="B53" s="41"/>
       <c r="C53" s="42"/>
@@ -2941,115 +3076,343 @@
       <c r="H53" s="65"/>
       <c r="I53" s="66"/>
       <c r="J53" s="44" t="e">
-        <f>F53/$B$60</f>
+        <f t="shared" ref="J53:J58" si="16">F53/$B$66</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K53" s="43" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="K53:K58" si="17">J53*(M53/L53)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="L53" s="44" t="e">
-        <f>G53/$B$60</f>
+        <f t="shared" ref="L53:L58" si="18">G53/$B$66</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M53" s="68"/>
       <c r="N53" s="60"/>
       <c r="O53" s="60"/>
       <c r="P53" s="30" t="e">
-        <f>I53/(J53*$B$61)</f>
+        <f>I53/(J53*$B$67)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="Q53" s="45" t="e">
-        <f>I53/((F53/$B$60*$B$61)*R53)</f>
+        <f>I53/((F53/$B$66*$B$67)*R53)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R53" s="45" t="e">
-        <f>H53/(L53*$B$61)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="54" spans="1:19" ht="13.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="46"/>
-      <c r="B54" s="47" t="s">
+        <f>H53/(L53*$B$67)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="54" spans="1:19" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="40"/>
+      <c r="B54" s="41"/>
+      <c r="C54" s="42"/>
+      <c r="D54" s="60"/>
+      <c r="E54" s="62"/>
+      <c r="F54" s="60"/>
+      <c r="G54" s="62"/>
+      <c r="H54" s="65"/>
+      <c r="I54" s="66"/>
+      <c r="J54" s="44" t="e">
+        <f t="shared" si="16"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K54" s="43" t="e">
+        <f t="shared" si="17"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L54" s="44" t="e">
+        <f t="shared" si="18"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M54" s="68"/>
+      <c r="N54" s="60"/>
+      <c r="O54" s="60"/>
+      <c r="P54" s="30" t="e">
+        <f>I54/(J54*$B$67)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q54" s="45" t="e">
+        <f>I54/((F54/$B$66*$B$67)*R54)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R54" s="45" t="e">
+        <f>H54/(L54*$B$67)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="55" spans="1:19" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="40"/>
+      <c r="B55" s="41"/>
+      <c r="C55" s="42"/>
+      <c r="D55" s="60"/>
+      <c r="E55" s="62"/>
+      <c r="F55" s="60"/>
+      <c r="G55" s="62"/>
+      <c r="H55" s="65"/>
+      <c r="I55" s="66"/>
+      <c r="J55" s="44" t="e">
+        <f t="shared" si="16"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K55" s="43" t="e">
+        <f t="shared" si="17"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L55" s="44" t="e">
+        <f t="shared" si="18"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M55" s="68"/>
+      <c r="N55" s="60"/>
+      <c r="O55" s="60"/>
+      <c r="P55" s="30" t="e">
+        <f>I55/(J55*$B$67)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q55" s="45" t="e">
+        <f>I55/((F55/$B$66*$B$67)*R55)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R55" s="45" t="e">
+        <f>H55/(L55*$B$67)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="56" spans="1:19" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="40"/>
+      <c r="B56" s="41"/>
+      <c r="C56" s="42"/>
+      <c r="D56" s="60"/>
+      <c r="E56" s="62"/>
+      <c r="F56" s="60"/>
+      <c r="G56" s="62"/>
+      <c r="H56" s="65"/>
+      <c r="I56" s="66"/>
+      <c r="J56" s="44" t="e">
+        <f t="shared" si="16"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K56" s="43" t="e">
+        <f t="shared" si="17"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L56" s="44" t="e">
+        <f t="shared" si="18"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M56" s="68"/>
+      <c r="N56" s="60"/>
+      <c r="O56" s="60"/>
+      <c r="P56" s="30" t="e">
+        <f>I56/(J56*$B$67)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q56" s="45" t="e">
+        <f>I56/((F56/$B$66*$B$67)*R56)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R56" s="45" t="e">
+        <f>H56/(L56*$B$67)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="57" spans="1:19" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="40"/>
+      <c r="B57" s="41"/>
+      <c r="C57" s="42"/>
+      <c r="D57" s="60"/>
+      <c r="E57" s="62"/>
+      <c r="F57" s="60"/>
+      <c r="G57" s="62"/>
+      <c r="H57" s="65"/>
+      <c r="I57" s="66"/>
+      <c r="J57" s="44" t="e">
+        <f t="shared" si="16"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K57" s="43" t="e">
+        <f t="shared" si="17"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L57" s="44" t="e">
+        <f t="shared" si="18"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M57" s="68"/>
+      <c r="N57" s="60"/>
+      <c r="O57" s="60"/>
+      <c r="P57" s="30" t="e">
+        <f>I57/(J57*$B$67)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q57" s="45" t="e">
+        <f>I57/((F57/$B$66*$B$67)*R57)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R57" s="45" t="e">
+        <f>H57/(L57*$B$67)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="58" spans="1:19" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="40"/>
+      <c r="B58" s="41"/>
+      <c r="C58" s="42"/>
+      <c r="D58" s="60"/>
+      <c r="E58" s="62"/>
+      <c r="F58" s="60"/>
+      <c r="G58" s="62"/>
+      <c r="H58" s="65"/>
+      <c r="I58" s="66"/>
+      <c r="J58" s="44" t="e">
+        <f t="shared" si="16"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K58" s="43" t="e">
+        <f t="shared" si="17"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L58" s="44" t="e">
+        <f t="shared" si="18"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M58" s="68"/>
+      <c r="N58" s="60"/>
+      <c r="O58" s="60"/>
+      <c r="P58" s="30" t="e">
+        <f>I58/(J58*$B$67)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q58" s="45" t="e">
+        <f>I58/((F58/$B$66*$B$67)*R58)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R58" s="45" t="e">
+        <f>H58/(L58*$B$67)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="59" spans="1:19" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="40"/>
+      <c r="B59" s="41"/>
+      <c r="C59" s="42"/>
+      <c r="D59" s="60"/>
+      <c r="E59" s="62"/>
+      <c r="F59" s="60"/>
+      <c r="G59" s="62"/>
+      <c r="H59" s="65"/>
+      <c r="I59" s="66"/>
+      <c r="J59" s="44" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K59" s="43" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L59" s="44" t="e">
+        <f>G59/$B$66</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M59" s="68"/>
+      <c r="N59" s="60"/>
+      <c r="O59" s="60"/>
+      <c r="P59" s="30" t="e">
+        <f>I59/(J59*$B$67)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q59" s="45" t="e">
+        <f>I59/((F59/$B$66*$B$67)*R59)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R59" s="45" t="e">
+        <f>H59/(L59*$B$67)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="60" spans="1:19" ht="13.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="46"/>
+      <c r="B60" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="C54" s="48"/>
-      <c r="D54" s="49">
-        <f t="shared" ref="D54:N54" si="16">SUM(D10:D53)</f>
+      <c r="C60" s="48"/>
+      <c r="D60" s="49">
+        <f t="shared" ref="D60:N60" si="19">SUM(D10:D59)</f>
         <v>0</v>
       </c>
-      <c r="E54" s="49">
-        <f t="shared" si="16"/>
+      <c r="E60" s="49">
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="F54" s="49">
-        <f t="shared" si="16"/>
+      <c r="F60" s="49">
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="G54" s="49">
-        <f t="shared" si="16"/>
+      <c r="G60" s="49">
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="H54" s="49">
-        <f t="shared" si="16"/>
+      <c r="H60" s="49">
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="I54" s="50">
-        <f t="shared" si="16"/>
+      <c r="I60" s="50">
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="J54" s="51" t="e">
-        <f t="shared" si="16"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K54" s="52" t="e">
-        <f t="shared" si="16"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L54" s="52" t="e">
-        <f t="shared" si="16"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M54" s="53">
-        <f t="shared" si="16"/>
+      <c r="J60" s="51" t="e">
+        <f t="shared" si="19"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K60" s="52" t="e">
+        <f t="shared" si="19"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L60" s="52" t="e">
+        <f t="shared" si="19"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M60" s="53">
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="N54" s="54">
-        <f t="shared" si="16"/>
+      <c r="N60" s="54">
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="O54" s="54"/>
-      <c r="P54" s="57" t="e">
-        <f>I54/(J54*$B$61)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q54" s="57" t="e">
-        <f>I54/((F54/$B$60*$B$61)*R54)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R54" s="57" t="e">
-        <f>H54/(L54*$B$61)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S54" s="58"/>
-    </row>
-    <row r="57" spans="1:19" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C57" s="55"/>
-    </row>
-    <row r="58" spans="1:19" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C58" s="55"/>
-    </row>
-    <row r="60" spans="1:19" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="56" t="s">
+      <c r="O60" s="54"/>
+      <c r="P60" s="57" t="e">
+        <f>I60/(J60*$B$67)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q60" s="57" t="e">
+        <f>I60/((F60/$B$66*$B$67)*R60)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R60" s="57" t="e">
+        <f>H60/(L60*$B$67)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S60" s="58"/>
+    </row>
+    <row r="63" spans="1:19" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C63" s="55"/>
+    </row>
+    <row r="64" spans="1:19" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C64" s="55"/>
+    </row>
+    <row r="66" spans="1:2" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="56" t="s">
         <v>25</v>
       </c>
-      <c r="B60" s="56"/>
-    </row>
-    <row r="61" spans="1:19" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="56" t="s">
+      <c r="B66" s="56"/>
+    </row>
+    <row r="67" spans="1:2" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="56" t="s">
         <v>26</v>
       </c>
-      <c r="B61" s="56"/>
+      <c r="B67" s="56"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
@@ -3070,8 +3433,8 @@
 &amp;I© 2017 SunEdison&amp;I &amp;C&amp;R&amp;"Arial"&amp;8 Page 1 of 2 </oddFooter>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="D54:H54 J10:L13 P10:R13 P54:R54 J54:N54" unlockedFormula="1"/>
-    <ignoredError sqref="I54" formula="1" unlockedFormula="1"/>
+    <ignoredError sqref="D60:H60 J10:L13 P10:R13 P60:R60 J60:N60" unlockedFormula="1"/>
+    <ignoredError sqref="I60" formula="1" unlockedFormula="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>